<commit_message>
Update EE_Project_Dashboard.xlsx with latest data
https://claude.ai/code/session_015Yj1rKpkcryqiDrxyhDemu
</commit_message>
<xml_diff>
--- a/EE_Project_Dashboard.xlsx
+++ b/EE_Project_Dashboard.xlsx
@@ -96,7 +96,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="11">
     <border/>
     <border>
       <left/>
@@ -132,11 +132,67 @@
         <color rgb="FFB0B0B0"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF0078D4"/>
+      </left>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF0078D4"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF0078D4"/>
+      </right>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF0078D4"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF0078D4"/>
+      </right>
+      <bottom style="medium">
+        <color rgb="FF005A9E"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF0078D4"/>
+      </top>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF0078D4"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF0078D4"/>
+      </top>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF0078D4"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF005A9E"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF0078D4"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF0078D4"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF005A9E"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -212,6 +268,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -708,8 +767,8 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
       <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -772,6 +831,12 @@
           <t>RASI</t>
         </is>
       </c>
+      <c r="E1" s="27" t="n"/>
+      <c r="F1" s="27" t="n"/>
+      <c r="G1" s="27" t="n"/>
+      <c r="H1" s="27" t="n"/>
+      <c r="I1" s="27" t="n"/>
+      <c r="J1" s="28" t="n"/>
       <c r="K1" s="19" t="inlineStr">
         <is>
           <t>T1/2025</t>
@@ -894,9 +959,9 @@
       </c>
     </row>
     <row r="2" ht="30" customHeight="1" s="18">
-      <c r="A2" s="24" t="n"/>
-      <c r="B2" s="24" t="n"/>
-      <c r="C2" s="24" t="n"/>
+      <c r="A2" s="29" t="n"/>
+      <c r="B2" s="29" t="n"/>
+      <c r="C2" s="29" t="n"/>
       <c r="D2" s="25" t="inlineStr">
         <is>
           <t>Đinh Hoàng Phú</t>
@@ -932,30 +997,30 @@
           <t>Tôn Thất Phúc Khánh</t>
         </is>
       </c>
-      <c r="K2" s="24" t="n"/>
-      <c r="L2" s="24" t="n"/>
-      <c r="M2" s="24" t="n"/>
-      <c r="N2" s="24" t="n"/>
-      <c r="O2" s="24" t="n"/>
-      <c r="P2" s="24" t="n"/>
-      <c r="Q2" s="24" t="n"/>
-      <c r="R2" s="24" t="n"/>
-      <c r="S2" s="24" t="n"/>
-      <c r="T2" s="24" t="n"/>
-      <c r="U2" s="24" t="n"/>
-      <c r="V2" s="24" t="n"/>
-      <c r="W2" s="24" t="n"/>
-      <c r="X2" s="24" t="n"/>
-      <c r="Y2" s="24" t="n"/>
-      <c r="Z2" s="24" t="n"/>
-      <c r="AA2" s="24" t="n"/>
-      <c r="AB2" s="24" t="n"/>
-      <c r="AC2" s="24" t="n"/>
-      <c r="AD2" s="24" t="n"/>
-      <c r="AE2" s="24" t="n"/>
-      <c r="AF2" s="24" t="n"/>
-      <c r="AG2" s="24" t="n"/>
-      <c r="AH2" s="24" t="n"/>
+      <c r="K2" s="29" t="n"/>
+      <c r="L2" s="29" t="n"/>
+      <c r="M2" s="29" t="n"/>
+      <c r="N2" s="29" t="n"/>
+      <c r="O2" s="29" t="n"/>
+      <c r="P2" s="29" t="n"/>
+      <c r="Q2" s="29" t="n"/>
+      <c r="R2" s="29" t="n"/>
+      <c r="S2" s="29" t="n"/>
+      <c r="T2" s="29" t="n"/>
+      <c r="U2" s="29" t="n"/>
+      <c r="V2" s="29" t="n"/>
+      <c r="W2" s="29" t="n"/>
+      <c r="X2" s="29" t="n"/>
+      <c r="Y2" s="29" t="n"/>
+      <c r="Z2" s="29" t="n"/>
+      <c r="AA2" s="29" t="n"/>
+      <c r="AB2" s="29" t="n"/>
+      <c r="AC2" s="29" t="n"/>
+      <c r="AD2" s="29" t="n"/>
+      <c r="AE2" s="29" t="n"/>
+      <c r="AF2" s="29" t="n"/>
+      <c r="AG2" s="29" t="n"/>
+      <c r="AH2" s="29" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="20" t="n">
@@ -963,7 +1028,7 @@
       </c>
       <c r="B3" s="20" t="inlineStr">
         <is>
-          <t>MOT200</t>
+          <t>MOT0200</t>
         </is>
       </c>
       <c r="C3" s="21" t="inlineStr">
@@ -1033,7 +1098,7 @@
       </c>
       <c r="B4" s="20" t="inlineStr">
         <is>
-          <t>MOT300</t>
+          <t>MOT0300</t>
         </is>
       </c>
       <c r="C4" s="21" t="inlineStr">
@@ -2894,12 +2959,12 @@
     <mergeCell ref="Y1:Y2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="D1:J1"/>
+    <mergeCell ref="AC1:AC2"/>
     <mergeCell ref="L1:L2"/>
-    <mergeCell ref="AC1:AC2"/>
     <mergeCell ref="AG1:AG2"/>
     <mergeCell ref="N1:N2"/>
+    <mergeCell ref="AE1:AE2"/>
     <mergeCell ref="T1:T2"/>
-    <mergeCell ref="AE1:AE2"/>
     <mergeCell ref="AF1:AF2"/>
     <mergeCell ref="X1:X2"/>
     <mergeCell ref="Z1:Z2"/>
@@ -3124,7 +3189,7 @@
       </c>
       <c r="B3" s="20" t="inlineStr">
         <is>
-          <t>MOT200</t>
+          <t>MOT0200</t>
         </is>
       </c>
       <c r="C3" s="21">
@@ -3181,7 +3246,7 @@
       </c>
       <c r="B4" s="20" t="inlineStr">
         <is>
-          <t>MOT200</t>
+          <t>MOT0200</t>
         </is>
       </c>
       <c r="C4" s="21">
@@ -3238,7 +3303,7 @@
       </c>
       <c r="B5" s="20" t="inlineStr">
         <is>
-          <t>MOT200</t>
+          <t>MOT0200</t>
         </is>
       </c>
       <c r="C5" s="21">
@@ -3466,7 +3531,7 @@
       </c>
       <c r="B9" s="20" t="inlineStr">
         <is>
-          <t>MOT200</t>
+          <t>MOT0200</t>
         </is>
       </c>
       <c r="C9" s="21">
@@ -3523,7 +3588,7 @@
       </c>
       <c r="B10" s="20" t="inlineStr">
         <is>
-          <t>MOT200</t>
+          <t>MOT0200</t>
         </is>
       </c>
       <c r="C10" s="21">
@@ -3580,7 +3645,7 @@
       </c>
       <c r="B11" s="20" t="inlineStr">
         <is>
-          <t>MOT200</t>
+          <t>MOT0200</t>
         </is>
       </c>
       <c r="C11" s="21">
@@ -3637,7 +3702,7 @@
       </c>
       <c r="B12" s="20" t="inlineStr">
         <is>
-          <t>MOT200</t>
+          <t>MOT0200</t>
         </is>
       </c>
       <c r="C12" s="21">
@@ -3694,7 +3759,7 @@
       </c>
       <c r="B13" s="20" t="inlineStr">
         <is>
-          <t>MOT200</t>
+          <t>MOT0200</t>
         </is>
       </c>
       <c r="C13" s="21">
@@ -3751,7 +3816,7 @@
       </c>
       <c r="B14" s="20" t="inlineStr">
         <is>
-          <t>MOT200</t>
+          <t>MOT0200</t>
         </is>
       </c>
       <c r="C14" s="21">
@@ -3808,7 +3873,7 @@
       </c>
       <c r="B15" s="20" t="inlineStr">
         <is>
-          <t>MOT200</t>
+          <t>MOT0200</t>
         </is>
       </c>
       <c r="C15" s="21">
@@ -3865,7 +3930,7 @@
       </c>
       <c r="B16" s="20" t="inlineStr">
         <is>
-          <t>MOT200</t>
+          <t>MOT0200</t>
         </is>
       </c>
       <c r="C16" s="21">
@@ -3922,7 +3987,7 @@
       </c>
       <c r="B17" s="20" t="inlineStr">
         <is>
-          <t>MOT200</t>
+          <t>MOT0200</t>
         </is>
       </c>
       <c r="C17" s="21">
@@ -3979,7 +4044,7 @@
       </c>
       <c r="B18" s="20" t="inlineStr">
         <is>
-          <t>MOT200</t>
+          <t>MOT0200</t>
         </is>
       </c>
       <c r="C18" s="21">
@@ -4036,7 +4101,7 @@
       </c>
       <c r="B19" s="20" t="inlineStr">
         <is>
-          <t>MOT200</t>
+          <t>MOT0200</t>
         </is>
       </c>
       <c r="C19" s="21">
@@ -4093,7 +4158,7 @@
       </c>
       <c r="B20" s="20" t="inlineStr">
         <is>
-          <t>MOT200</t>
+          <t>MOT0200</t>
         </is>
       </c>
       <c r="C20" s="21">

</xml_diff>

<commit_message>
Fix Board/Module: dependent dropdown, remove Tổng hợp
- Board/Module dropdown now depends on Project ID using INDIRECT:
  - MOT0200: shows PDU, LLB, Hub Ethernet, Hot Swap, Wire Harness
  - Other projects: dropdown is empty (no board selection possible)
- Named ranges created for each project ID pointing to board lists
- Removed "Tổng hợp" from dropdown and cleared from existing data
- Helper board list stored on Roadmap sheet (column AK)
- Error message shown when trying to set Board for non-MOT0200 project

https://claude.ai/code/session_015Yj1rKpkcryqiDrxyhDemu
</commit_message>
<xml_diff>
--- a/EE_Project_Dashboard.xlsx
+++ b/EE_Project_Dashboard.xlsx
@@ -10,6 +10,13 @@
     <sheet name="Tasks" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="MOT0200">'Roadmap'!$AK$2:$AK$6</definedName>
+    <definedName name="MOT0300">'Roadmap'!$AL$2</definedName>
+    <definedName name="HSCR01">'Roadmap'!$AL$2</definedName>
+    <definedName name="HBR00">'Roadmap'!$AL$2</definedName>
+    <definedName name="EMBPC00">'Roadmap'!$AL$2</definedName>
+    <definedName name="HCR00">'Roadmap'!$AL$2</definedName>
+    <definedName name="BATERY00">'Roadmap'!$AL$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Tasks'!$A$1:$M$58</definedName>
   </definedNames>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -22,7 +29,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
@@ -54,6 +61,17 @@
       <b val="1"/>
       <color rgb="FFFFFFFF"/>
       <sz val="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <i val="1"/>
+      <color rgb="FF999999"/>
+      <sz val="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FF999999"/>
+      <sz val="9"/>
     </font>
   </fonts>
   <fills count="5">
@@ -229,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -273,6 +291,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -820,7 +840,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH52"/>
+  <dimension ref="A1:AL52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
@@ -836,6 +856,8 @@
     <col width="50" customWidth="1" min="3" max="3"/>
     <col width="6.81640625" customWidth="1" min="4" max="10"/>
     <col width="10" customWidth="1" min="11" max="34"/>
+    <col width="14" customWidth="1" min="37" max="37"/>
+    <col width="3" customWidth="1" min="38" max="38"/>
   </cols>
   <sheetData>
     <row r="1" ht="16" customHeight="1">
@@ -983,6 +1005,11 @@
       <c r="AH1" s="10" t="inlineStr">
         <is>
           <t>T12/2026</t>
+        </is>
+      </c>
+      <c r="AK1" s="19" t="inlineStr">
+        <is>
+          <t>Board List</t>
         </is>
       </c>
     </row>
@@ -1049,6 +1076,16 @@
       <c r="AF2" s="11" t="n"/>
       <c r="AG2" s="11" t="n"/>
       <c r="AH2" s="11" t="n"/>
+      <c r="AK2" s="20" t="inlineStr">
+        <is>
+          <t>PDU</t>
+        </is>
+      </c>
+      <c r="AL2" s="20" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="45.5" customHeight="1">
       <c r="A3" s="5" t="n">
@@ -1123,6 +1160,11 @@
       <c r="AF3" s="5" t="n"/>
       <c r="AG3" s="5" t="n"/>
       <c r="AH3" s="5" t="n"/>
+      <c r="AK3" s="20" t="inlineStr">
+        <is>
+          <t>LLB</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="45.5" customHeight="1">
       <c r="A4" s="5" t="n">
@@ -1177,6 +1219,11 @@
       <c r="AF4" s="5" t="n"/>
       <c r="AG4" s="5" t="n"/>
       <c r="AH4" s="5" t="n"/>
+      <c r="AK4" s="20" t="inlineStr">
+        <is>
+          <t>Hub Ethernet</t>
+        </is>
+      </c>
     </row>
     <row r="5" ht="45.5" customHeight="1">
       <c r="A5" s="5" t="n">
@@ -1235,6 +1282,11 @@
       <c r="AF5" s="5" t="n"/>
       <c r="AG5" s="5" t="n"/>
       <c r="AH5" s="5" t="n"/>
+      <c r="AK5" s="20" t="inlineStr">
+        <is>
+          <t>Hot Swap</t>
+        </is>
+      </c>
     </row>
     <row r="6" ht="45.5" customHeight="1">
       <c r="A6" s="5" t="n">
@@ -1285,6 +1337,11 @@
       <c r="AF6" s="5" t="n"/>
       <c r="AG6" s="5" t="n"/>
       <c r="AH6" s="5" t="n"/>
+      <c r="AK6" s="20" t="inlineStr">
+        <is>
+          <t>Wire Harness</t>
+        </is>
+      </c>
     </row>
     <row r="7" ht="45.5" customHeight="1">
       <c r="A7" s="5" t="n">
@@ -4647,11 +4704,7 @@
         <f>IF(B26="","",VLOOKUP(B26,Roadmap!$B$3:$C$100,2,FALSE()))</f>
         <v/>
       </c>
-      <c r="D26" s="14" t="inlineStr">
-        <is>
-          <t>Tổng hợp</t>
-        </is>
-      </c>
+      <c r="D26" s="14" t="n"/>
       <c r="E26" s="15" t="inlineStr">
         <is>
           <t>Lắp ráp và test Robot</t>
@@ -4957,11 +5010,7 @@
         <f>IF(B31="","",VLOOKUP(B31,Roadmap!$B$3:$C$100,2,FALSE()))</f>
         <v/>
       </c>
-      <c r="D31" s="14" t="inlineStr">
-        <is>
-          <t>Tổng hợp</t>
-        </is>
-      </c>
+      <c r="D31" s="14" t="n"/>
       <c r="E31" s="15" t="inlineStr">
         <is>
           <t>Lựa chọn linh kiện nút nhấn cho Robot Vin Motion 2</t>
@@ -5019,11 +5068,7 @@
         <f>IF(B32="","",VLOOKUP(B32,Roadmap!$B$3:$C$100,2,FALSE()))</f>
         <v/>
       </c>
-      <c r="D32" s="14" t="inlineStr">
-        <is>
-          <t>Tổng hợp</t>
-        </is>
-      </c>
+      <c r="D32" s="14" t="n"/>
       <c r="E32" s="15" t="inlineStr">
         <is>
           <t>Benchmarking hệ thống điện tử, máy tính, camera các robot trên thế giới (Engine AI, Unitree, Ubitech,…)</t>
@@ -5081,11 +5126,7 @@
         <f>IF(B33="","",VLOOKUP(B33,Roadmap!$B$3:$C$100,2,FALSE()))</f>
         <v/>
       </c>
-      <c r="D33" s="14" t="inlineStr">
-        <is>
-          <t>Tổng hợp</t>
-        </is>
-      </c>
+      <c r="D33" s="14" t="n"/>
       <c r="E33" s="15" t="inlineStr">
         <is>
           <t>Test Anten đặt trên đầu xem có ổn không</t>
@@ -5143,11 +5184,7 @@
         <f>IF(B34="","",VLOOKUP(B34,Roadmap!$B$3:$C$100,2,FALSE()))</f>
         <v/>
       </c>
-      <c r="D34" s="14" t="inlineStr">
-        <is>
-          <t>Tổng hợp</t>
-        </is>
-      </c>
+      <c r="D34" s="14" t="n"/>
       <c r="E34" s="15" t="inlineStr">
         <is>
           <t>Test loa</t>
@@ -5263,11 +5300,7 @@
         <f>IF(B36="","",VLOOKUP(B36,Roadmap!$B$3:$C$100,2,FALSE()))</f>
         <v/>
       </c>
-      <c r="D36" s="14" t="inlineStr">
-        <is>
-          <t>Tổng hợp</t>
-        </is>
-      </c>
+      <c r="D36" s="14" t="n"/>
       <c r="E36" s="15" t="inlineStr">
         <is>
           <t>Test dây cho Robot</t>
@@ -5325,11 +5358,7 @@
         <f>IF(B37="","",VLOOKUP(B37,Roadmap!$B$3:$C$100,2,FALSE()))</f>
         <v/>
       </c>
-      <c r="D37" s="14" t="inlineStr">
-        <is>
-          <t>Tổng hợp</t>
-        </is>
-      </c>
+      <c r="D37" s="14" t="n"/>
       <c r="E37" s="15" t="inlineStr">
         <is>
           <t>Làm việc nhà máy Vfe</t>
@@ -5387,11 +5416,7 @@
         <f>IF(B38="","",VLOOKUP(B38,Roadmap!$B$3:$C$100,2,FALSE()))</f>
         <v/>
       </c>
-      <c r="D38" s="14" t="inlineStr">
-        <is>
-          <t>Tổng hợp</t>
-        </is>
-      </c>
+      <c r="D38" s="14" t="n"/>
       <c r="E38" s="15" t="inlineStr">
         <is>
           <t>Tiếp nhận và và xử lý lỗi của Robot đang hoạt động tại các P&amp;L</t>
@@ -32998,46 +33023,43 @@
     <cfRule type="cellIs" priority="5" operator="equal" dxfId="11">
       <formula>"Wire Harness"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="6" operator="equal" dxfId="4">
-      <formula>"Tổng hợp"</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F58">
-    <cfRule type="cellIs" priority="7" operator="equal" dxfId="8">
+    <cfRule type="cellIs" priority="6" operator="equal" dxfId="8">
       <formula>"Task"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="8" operator="equal" dxfId="7">
+    <cfRule type="cellIs" priority="7" operator="equal" dxfId="7">
       <formula>"Issue"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I58">
-    <cfRule type="cellIs" priority="9" operator="equal" dxfId="6">
+    <cfRule type="cellIs" priority="8" operator="equal" dxfId="6">
       <formula>"Open"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="10" operator="equal" dxfId="1">
+    <cfRule type="cellIs" priority="9" operator="equal" dxfId="1">
       <formula>"Doing"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="11" operator="equal" dxfId="4">
+    <cfRule type="cellIs" priority="10" operator="equal" dxfId="4">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="12" operator="equal" dxfId="0">
+    <cfRule type="cellIs" priority="11" operator="equal" dxfId="0">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M58">
-    <cfRule type="cellIs" priority="13" operator="equal" dxfId="2">
+    <cfRule type="cellIs" priority="12" operator="equal" dxfId="2">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="14" operator="equal" dxfId="1">
+    <cfRule type="cellIs" priority="13" operator="equal" dxfId="1">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="15" operator="equal" dxfId="0">
+    <cfRule type="cellIs" priority="14" operator="equal" dxfId="0">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation sqref="D2:D58" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"PDU,LLB,Hub Ethernet,Hot Swap,Wire Harness,Tổng hợp"</formula1>
+    <dataValidation sqref="D2:D58" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Không hợp lệ" error="Board/Module chỉ áp dụng cho dự án MOT0200" type="list">
+      <formula1>=INDIRECT($B2)</formula1>
     </dataValidation>
     <dataValidation sqref="B2:B58" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>Roadmap!$B$3:$B$100</formula1>

</xml_diff>

<commit_message>
Add definition library for all dropdowns with colors
Create editable "THƯ VIỆN ĐỊNH NGHĨA" on Roadmap sheet (col AK+):

Section 1 - General Dropdowns (AK-AM):
  RASI:     R/A/S/C/I with descriptions and color-coded values
  Status:   Open/Doing/Pending/Done
  Type:     Task/Issue
  Priority: High/Medium/Low

Section 2 - Board/Module per Project (AO+):
  Each project has its own column with editable board list
  Dynamic named ranges (OFFSET+COUNTA) auto-expand when user adds items

All dropdowns now reference the library via named ranges:
  - RASI_List, Status_List, Type_List, Priority_List
  - Project-specific board lists (MOT0200, MOT0300, etc.)
  - Conditional formatting colors match library definitions

https://claude.ai/code/session_015Yj1rKpkcryqiDrxyhDemu
</commit_message>
<xml_diff>
--- a/EE_Project_Dashboard.xlsx
+++ b/EE_Project_Dashboard.xlsx
@@ -10,13 +10,17 @@
     <sheet name="Tasks" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="MOT0200">'Roadmap'!$AK$2:$AK$6</definedName>
-    <definedName name="MOT0300">'Roadmap'!$AL$2</definedName>
-    <definedName name="HSCR01">'Roadmap'!$AL$2</definedName>
-    <definedName name="HBR00">'Roadmap'!$AL$2</definedName>
-    <definedName name="EMBPC00">'Roadmap'!$AL$2</definedName>
-    <definedName name="HCR00">'Roadmap'!$AL$2</definedName>
-    <definedName name="BATERY00">'Roadmap'!$AL$2</definedName>
+    <definedName name="RASI_List">'Roadmap'!$AL$3:$AL$7</definedName>
+    <definedName name="Status_List">'Roadmap'!$AL$8:$AL$11</definedName>
+    <definedName name="Type_List">'Roadmap'!$AL$12:$AL$13</definedName>
+    <definedName name="Priority_List">'Roadmap'!$AL$14:$AL$16</definedName>
+    <definedName name="MOT0200">OFFSET('Roadmap'!$AO$3,0,0,MAX(COUNTA('Roadmap'!$AO$3:$AO$22),1),1)</definedName>
+    <definedName name="MOT0300">OFFSET('Roadmap'!$AP$3,0,0,MAX(COUNTA('Roadmap'!$AP$3:$AP$22),1),1)</definedName>
+    <definedName name="HSCR01">OFFSET('Roadmap'!$AQ$3,0,0,MAX(COUNTA('Roadmap'!$AQ$3:$AQ$22),1),1)</definedName>
+    <definedName name="HBR00">OFFSET('Roadmap'!$AR$3,0,0,MAX(COUNTA('Roadmap'!$AR$3:$AR$22),1),1)</definedName>
+    <definedName name="EMBPC00">OFFSET('Roadmap'!$AS$3,0,0,MAX(COUNTA('Roadmap'!$AS$3:$AS$22),1),1)</definedName>
+    <definedName name="HCR00">OFFSET('Roadmap'!$AT$3,0,0,MAX(COUNTA('Roadmap'!$AT$3:$AT$22),1),1)</definedName>
+    <definedName name="BATERY00">OFFSET('Roadmap'!$AU$3,0,0,MAX(COUNTA('Roadmap'!$AU$3:$AU$22),1),1)</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Tasks'!$A$1:$M$58</definedName>
   </definedNames>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -29,7 +33,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="18">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
@@ -73,8 +77,67 @@
       <color rgb="FF999999"/>
       <sz val="9"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <color rgb="FFFFFFFF"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <color rgb="FF4A148C"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <color rgb="FF1864AB"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <color rgb="FF0B6623"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <color rgb="FF9B1D1D"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <color rgb="FF7C5E00"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <i val="1"/>
+      <color rgb="FF888888"/>
+      <sz val="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <color rgb="FF0070C0"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FF666666"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <color rgb="FF495057"/>
+      <sz val="11"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="20">
     <fill>
       <patternFill/>
     </fill>
@@ -99,8 +162,98 @@
         <bgColor rgb="FF33C1FF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor rgb="FF0070C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDBEAFE"/>
+        <bgColor rgb="FFDBEAFE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE3F2FD"/>
+        <bgColor rgb="FFE3F2FD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD3F9D8"/>
+        <bgColor rgb="FFD3F9D8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD6D6"/>
+        <bgColor rgb="FFFFD6D6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF9DB"/>
+        <bgColor rgb="FFFFF9DB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8F9FA"/>
+        <bgColor rgb="FFF8F9FA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8F4FD"/>
+        <bgColor rgb="FFE8F4FD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6B6B"/>
+        <bgColor rgb="FFFF6B6B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFA94D"/>
+        <bgColor rgb="FFFFA94D"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF69DB7C"/>
+        <bgColor rgb="FF69DB7C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF74C0FC"/>
+        <bgColor rgb="FF74C0FC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB197FC"/>
+        <bgColor rgb="FFB197FC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD43B"/>
+        <bgColor rgb="FFFFD43B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDEE2E6"/>
+        <bgColor rgb="FFDEE2E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -243,11 +396,26 @@
         <color rgb="FF005A9E"/>
       </bottom>
     </border>
+    <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FFD0D0D0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD0D0D0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD0D0D0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD0D0D0"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -293,6 +461,65 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -840,7 +1067,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AL52"/>
+  <dimension ref="A1:BB52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
@@ -856,8 +1083,17 @@
     <col width="50" customWidth="1" min="3" max="3"/>
     <col width="6.81640625" customWidth="1" min="4" max="10"/>
     <col width="10" customWidth="1" min="11" max="34"/>
-    <col width="14" customWidth="1" min="37" max="37"/>
-    <col width="3" customWidth="1" min="38" max="38"/>
+    <col width="12" customWidth="1" min="37" max="37"/>
+    <col width="12" customWidth="1" min="38" max="38"/>
+    <col width="45" customWidth="1" min="39" max="39"/>
+    <col width="16" customWidth="1" min="40" max="40"/>
+    <col width="16" customWidth="1" min="41" max="41"/>
+    <col width="16" customWidth="1" min="42" max="42"/>
+    <col width="16" customWidth="1" min="43" max="43"/>
+    <col width="16" customWidth="1" min="44" max="44"/>
+    <col width="16" customWidth="1" min="45" max="45"/>
+    <col width="16" customWidth="1" min="46" max="46"/>
+    <col width="16" customWidth="1" min="47" max="47"/>
   </cols>
   <sheetData>
     <row r="1" ht="16" customHeight="1">
@@ -1007,11 +1243,32 @@
           <t>T12/2026</t>
         </is>
       </c>
-      <c r="AK1" s="19" t="inlineStr">
+      <c r="AK1" s="21" t="inlineStr">
         <is>
-          <t>Board List</t>
+          <t>THƯ VIỆN ĐỊNH NGHĨA</t>
         </is>
       </c>
+      <c r="AL1" s="22" t="n"/>
+      <c r="AM1" s="22" t="n"/>
+      <c r="AN1" s="23" t="n"/>
+      <c r="AO1" s="21" t="inlineStr">
+        <is>
+          <t>BOARD / MODULE CHO TỪNG DỰ ÁN</t>
+        </is>
+      </c>
+      <c r="AP1" s="22" t="n"/>
+      <c r="AQ1" s="22" t="n"/>
+      <c r="AR1" s="22" t="n"/>
+      <c r="AS1" s="22" t="n"/>
+      <c r="AT1" s="22" t="n"/>
+      <c r="AU1" s="22" t="n"/>
+      <c r="AV1" s="23" t="n"/>
+      <c r="AW1" s="23" t="n"/>
+      <c r="AX1" s="23" t="n"/>
+      <c r="AY1" s="23" t="n"/>
+      <c r="AZ1" s="23" t="n"/>
+      <c r="BA1" s="23" t="n"/>
+      <c r="BB1" s="23" t="n"/>
     </row>
     <row r="2" ht="58" customHeight="1">
       <c r="A2" s="11" t="n"/>
@@ -1076,16 +1333,64 @@
       <c r="AF2" s="11" t="n"/>
       <c r="AG2" s="11" t="n"/>
       <c r="AH2" s="11" t="n"/>
-      <c r="AK2" s="20" t="inlineStr">
+      <c r="AK2" s="24" t="inlineStr">
         <is>
-          <t>PDU</t>
+          <t>Loại</t>
         </is>
       </c>
-      <c r="AL2" s="20" t="inlineStr">
+      <c r="AL2" s="24" t="inlineStr">
         <is>
-          <t> </t>
+          <t>Giá trị</t>
         </is>
       </c>
+      <c r="AM2" s="24" t="inlineStr">
+        <is>
+          <t>Mô tả</t>
+        </is>
+      </c>
+      <c r="AN2" s="23" t="n"/>
+      <c r="AO2" s="24" t="inlineStr">
+        <is>
+          <t>MOT0200</t>
+        </is>
+      </c>
+      <c r="AP2" s="24" t="inlineStr">
+        <is>
+          <t>MOT0300</t>
+        </is>
+      </c>
+      <c r="AQ2" s="24" t="inlineStr">
+        <is>
+          <t>HSCR01</t>
+        </is>
+      </c>
+      <c r="AR2" s="24" t="inlineStr">
+        <is>
+          <t>HBR00</t>
+        </is>
+      </c>
+      <c r="AS2" s="24" t="inlineStr">
+        <is>
+          <t>EMBPC00</t>
+        </is>
+      </c>
+      <c r="AT2" s="24" t="inlineStr">
+        <is>
+          <t>HCR00</t>
+        </is>
+      </c>
+      <c r="AU2" s="24" t="inlineStr">
+        <is>
+          <t>BATERY00</t>
+        </is>
+      </c>
+      <c r="AV2" s="23" t="n"/>
+      <c r="AW2" s="23" t="n"/>
+      <c r="AX2" s="23" t="n"/>
+      <c r="AY2" s="23" t="n"/>
+      <c r="AZ2" s="23" t="n"/>
+      <c r="BA2" s="23" t="n"/>
+      <c r="BB2" s="23" t="n"/>
     </row>
     <row r="3" ht="45.5" customHeight="1">
       <c r="A3" s="5" t="n">
@@ -1160,11 +1465,40 @@
       <c r="AF3" s="5" t="n"/>
       <c r="AG3" s="5" t="n"/>
       <c r="AH3" s="5" t="n"/>
-      <c r="AK3" s="20" t="inlineStr">
+      <c r="AK3" s="32" t="inlineStr">
         <is>
-          <t>LLB</t>
+          <t>RASI</t>
         </is>
       </c>
+      <c r="AL3" s="33" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="AM3" s="34" t="inlineStr">
+        <is>
+          <t>Responsible - Chịu trách nhiệm thực hiện</t>
+        </is>
+      </c>
+      <c r="AN3" s="23" t="n"/>
+      <c r="AO3" s="25" t="inlineStr">
+        <is>
+          <t>PDU</t>
+        </is>
+      </c>
+      <c r="AP3" s="26" t="n"/>
+      <c r="AQ3" s="26" t="n"/>
+      <c r="AR3" s="26" t="n"/>
+      <c r="AS3" s="26" t="n"/>
+      <c r="AT3" s="26" t="n"/>
+      <c r="AU3" s="26" t="n"/>
+      <c r="AV3" s="23" t="n"/>
+      <c r="AW3" s="23" t="n"/>
+      <c r="AX3" s="23" t="n"/>
+      <c r="AY3" s="23" t="n"/>
+      <c r="AZ3" s="23" t="n"/>
+      <c r="BA3" s="23" t="n"/>
+      <c r="BB3" s="23" t="n"/>
     </row>
     <row r="4" ht="45.5" customHeight="1">
       <c r="A4" s="5" t="n">
@@ -1219,11 +1553,36 @@
       <c r="AF4" s="5" t="n"/>
       <c r="AG4" s="5" t="n"/>
       <c r="AH4" s="5" t="n"/>
-      <c r="AK4" s="20" t="inlineStr">
+      <c r="AK4" s="35" t="n"/>
+      <c r="AL4" s="36" t="inlineStr">
         <is>
-          <t>Hub Ethernet</t>
+          <t>A</t>
         </is>
       </c>
+      <c r="AM4" s="34" t="inlineStr">
+        <is>
+          <t>Accountable - Phê duyệt, chịu trách nhiệm cuối cùng</t>
+        </is>
+      </c>
+      <c r="AN4" s="23" t="n"/>
+      <c r="AO4" s="27" t="inlineStr">
+        <is>
+          <t>LLB</t>
+        </is>
+      </c>
+      <c r="AP4" s="26" t="n"/>
+      <c r="AQ4" s="26" t="n"/>
+      <c r="AR4" s="26" t="n"/>
+      <c r="AS4" s="26" t="n"/>
+      <c r="AT4" s="26" t="n"/>
+      <c r="AU4" s="26" t="n"/>
+      <c r="AV4" s="23" t="n"/>
+      <c r="AW4" s="23" t="n"/>
+      <c r="AX4" s="23" t="n"/>
+      <c r="AY4" s="23" t="n"/>
+      <c r="AZ4" s="23" t="n"/>
+      <c r="BA4" s="23" t="n"/>
+      <c r="BB4" s="23" t="n"/>
     </row>
     <row r="5" ht="45.5" customHeight="1">
       <c r="A5" s="5" t="n">
@@ -1282,11 +1641,36 @@
       <c r="AF5" s="5" t="n"/>
       <c r="AG5" s="5" t="n"/>
       <c r="AH5" s="5" t="n"/>
-      <c r="AK5" s="20" t="inlineStr">
+      <c r="AK5" s="35" t="n"/>
+      <c r="AL5" s="37" t="inlineStr">
         <is>
-          <t>Hot Swap</t>
+          <t>S</t>
         </is>
       </c>
+      <c r="AM5" s="34" t="inlineStr">
+        <is>
+          <t>Support - Hỗ trợ thực hiện</t>
+        </is>
+      </c>
+      <c r="AN5" s="23" t="n"/>
+      <c r="AO5" s="28" t="inlineStr">
+        <is>
+          <t>Hub Ethernet</t>
+        </is>
+      </c>
+      <c r="AP5" s="26" t="n"/>
+      <c r="AQ5" s="26" t="n"/>
+      <c r="AR5" s="26" t="n"/>
+      <c r="AS5" s="26" t="n"/>
+      <c r="AT5" s="26" t="n"/>
+      <c r="AU5" s="26" t="n"/>
+      <c r="AV5" s="23" t="n"/>
+      <c r="AW5" s="23" t="n"/>
+      <c r="AX5" s="23" t="n"/>
+      <c r="AY5" s="23" t="n"/>
+      <c r="AZ5" s="23" t="n"/>
+      <c r="BA5" s="23" t="n"/>
+      <c r="BB5" s="23" t="n"/>
     </row>
     <row r="6" ht="45.5" customHeight="1">
       <c r="A6" s="5" t="n">
@@ -1337,11 +1721,36 @@
       <c r="AF6" s="5" t="n"/>
       <c r="AG6" s="5" t="n"/>
       <c r="AH6" s="5" t="n"/>
-      <c r="AK6" s="20" t="inlineStr">
+      <c r="AK6" s="35" t="n"/>
+      <c r="AL6" s="38" t="inlineStr">
         <is>
-          <t>Wire Harness</t>
+          <t>C</t>
         </is>
       </c>
+      <c r="AM6" s="34" t="inlineStr">
+        <is>
+          <t>Consulted - Được tham vấn ý kiến</t>
+        </is>
+      </c>
+      <c r="AN6" s="23" t="n"/>
+      <c r="AO6" s="29" t="inlineStr">
+        <is>
+          <t>Hot Swap</t>
+        </is>
+      </c>
+      <c r="AP6" s="26" t="n"/>
+      <c r="AQ6" s="26" t="n"/>
+      <c r="AR6" s="26" t="n"/>
+      <c r="AS6" s="26" t="n"/>
+      <c r="AT6" s="26" t="n"/>
+      <c r="AU6" s="26" t="n"/>
+      <c r="AV6" s="23" t="n"/>
+      <c r="AW6" s="23" t="n"/>
+      <c r="AX6" s="23" t="n"/>
+      <c r="AY6" s="23" t="n"/>
+      <c r="AZ6" s="23" t="n"/>
+      <c r="BA6" s="23" t="n"/>
+      <c r="BB6" s="23" t="n"/>
     </row>
     <row r="7" ht="45.5" customHeight="1">
       <c r="A7" s="5" t="n">
@@ -1392,6 +1801,36 @@
       <c r="AF7" s="5" t="n"/>
       <c r="AG7" s="5" t="n"/>
       <c r="AH7" s="5" t="n"/>
+      <c r="AK7" s="35" t="n"/>
+      <c r="AL7" s="39" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="AM7" s="34" t="inlineStr">
+        <is>
+          <t>Informed - Được thông báo kết quả</t>
+        </is>
+      </c>
+      <c r="AN7" s="23" t="n"/>
+      <c r="AO7" s="30" t="inlineStr">
+        <is>
+          <t>Wire Harness</t>
+        </is>
+      </c>
+      <c r="AP7" s="26" t="n"/>
+      <c r="AQ7" s="26" t="n"/>
+      <c r="AR7" s="26" t="n"/>
+      <c r="AS7" s="26" t="n"/>
+      <c r="AT7" s="26" t="n"/>
+      <c r="AU7" s="26" t="n"/>
+      <c r="AV7" s="23" t="n"/>
+      <c r="AW7" s="23" t="n"/>
+      <c r="AX7" s="23" t="n"/>
+      <c r="AY7" s="23" t="n"/>
+      <c r="AZ7" s="23" t="n"/>
+      <c r="BA7" s="23" t="n"/>
+      <c r="BB7" s="23" t="n"/>
     </row>
     <row r="8" ht="45.5" customHeight="1">
       <c r="A8" s="5" t="n">
@@ -1450,6 +1889,36 @@
       <c r="AF8" s="5" t="n"/>
       <c r="AG8" s="5" t="n"/>
       <c r="AH8" s="5" t="n"/>
+      <c r="AK8" s="32" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="AL8" s="38" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="AM8" s="34" t="inlineStr">
+        <is>
+          <t>Chưa bắt đầu</t>
+        </is>
+      </c>
+      <c r="AN8" s="23" t="n"/>
+      <c r="AO8" s="26" t="n"/>
+      <c r="AP8" s="26" t="n"/>
+      <c r="AQ8" s="26" t="n"/>
+      <c r="AR8" s="26" t="n"/>
+      <c r="AS8" s="26" t="n"/>
+      <c r="AT8" s="26" t="n"/>
+      <c r="AU8" s="26" t="n"/>
+      <c r="AV8" s="23" t="n"/>
+      <c r="AW8" s="23" t="n"/>
+      <c r="AX8" s="23" t="n"/>
+      <c r="AY8" s="23" t="n"/>
+      <c r="AZ8" s="23" t="n"/>
+      <c r="BA8" s="23" t="n"/>
+      <c r="BB8" s="23" t="n"/>
     </row>
     <row r="9" ht="45.5" customHeight="1">
       <c r="A9" s="5" t="n">
@@ -1500,6 +1969,32 @@
       <c r="AF9" s="5" t="n"/>
       <c r="AG9" s="5" t="n"/>
       <c r="AH9" s="5" t="n"/>
+      <c r="AK9" s="35" t="n"/>
+      <c r="AL9" s="40" t="inlineStr">
+        <is>
+          <t>Doing</t>
+        </is>
+      </c>
+      <c r="AM9" s="34" t="inlineStr">
+        <is>
+          <t>Đang thực hiện</t>
+        </is>
+      </c>
+      <c r="AN9" s="23" t="n"/>
+      <c r="AO9" s="26" t="n"/>
+      <c r="AP9" s="26" t="n"/>
+      <c r="AQ9" s="26" t="n"/>
+      <c r="AR9" s="26" t="n"/>
+      <c r="AS9" s="26" t="n"/>
+      <c r="AT9" s="26" t="n"/>
+      <c r="AU9" s="26" t="n"/>
+      <c r="AV9" s="23" t="n"/>
+      <c r="AW9" s="23" t="n"/>
+      <c r="AX9" s="23" t="n"/>
+      <c r="AY9" s="23" t="n"/>
+      <c r="AZ9" s="23" t="n"/>
+      <c r="BA9" s="23" t="n"/>
+      <c r="BB9" s="23" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="5" t="n"/>
@@ -1536,6 +2031,32 @@
       <c r="AF10" s="5" t="n"/>
       <c r="AG10" s="5" t="n"/>
       <c r="AH10" s="5" t="n"/>
+      <c r="AK10" s="35" t="n"/>
+      <c r="AL10" s="41" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="AM10" s="34" t="inlineStr">
+        <is>
+          <t>Tạm dừng / Chờ xử lý</t>
+        </is>
+      </c>
+      <c r="AN10" s="23" t="n"/>
+      <c r="AO10" s="26" t="n"/>
+      <c r="AP10" s="26" t="n"/>
+      <c r="AQ10" s="26" t="n"/>
+      <c r="AR10" s="26" t="n"/>
+      <c r="AS10" s="26" t="n"/>
+      <c r="AT10" s="26" t="n"/>
+      <c r="AU10" s="26" t="n"/>
+      <c r="AV10" s="23" t="n"/>
+      <c r="AW10" s="23" t="n"/>
+      <c r="AX10" s="23" t="n"/>
+      <c r="AY10" s="23" t="n"/>
+      <c r="AZ10" s="23" t="n"/>
+      <c r="BA10" s="23" t="n"/>
+      <c r="BB10" s="23" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="5" t="n"/>
@@ -1572,6 +2093,32 @@
       <c r="AF11" s="5" t="n"/>
       <c r="AG11" s="5" t="n"/>
       <c r="AH11" s="5" t="n"/>
+      <c r="AK11" s="35" t="n"/>
+      <c r="AL11" s="37" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="AM11" s="34" t="inlineStr">
+        <is>
+          <t>Hoàn thành</t>
+        </is>
+      </c>
+      <c r="AN11" s="23" t="n"/>
+      <c r="AO11" s="26" t="n"/>
+      <c r="AP11" s="26" t="n"/>
+      <c r="AQ11" s="26" t="n"/>
+      <c r="AR11" s="26" t="n"/>
+      <c r="AS11" s="26" t="n"/>
+      <c r="AT11" s="26" t="n"/>
+      <c r="AU11" s="26" t="n"/>
+      <c r="AV11" s="23" t="n"/>
+      <c r="AW11" s="23" t="n"/>
+      <c r="AX11" s="23" t="n"/>
+      <c r="AY11" s="23" t="n"/>
+      <c r="AZ11" s="23" t="n"/>
+      <c r="BA11" s="23" t="n"/>
+      <c r="BB11" s="23" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="5" t="n"/>
@@ -1608,6 +2155,36 @@
       <c r="AF12" s="5" t="n"/>
       <c r="AG12" s="5" t="n"/>
       <c r="AH12" s="5" t="n"/>
+      <c r="AK12" s="32" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="AL12" s="27" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="AM12" s="34" t="inlineStr">
+        <is>
+          <t>Công việc thường</t>
+        </is>
+      </c>
+      <c r="AN12" s="23" t="n"/>
+      <c r="AO12" s="26" t="n"/>
+      <c r="AP12" s="26" t="n"/>
+      <c r="AQ12" s="26" t="n"/>
+      <c r="AR12" s="26" t="n"/>
+      <c r="AS12" s="26" t="n"/>
+      <c r="AT12" s="26" t="n"/>
+      <c r="AU12" s="26" t="n"/>
+      <c r="AV12" s="23" t="n"/>
+      <c r="AW12" s="23" t="n"/>
+      <c r="AX12" s="23" t="n"/>
+      <c r="AY12" s="23" t="n"/>
+      <c r="AZ12" s="23" t="n"/>
+      <c r="BA12" s="23" t="n"/>
+      <c r="BB12" s="23" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="5" t="n"/>
@@ -1644,6 +2221,32 @@
       <c r="AF13" s="5" t="n"/>
       <c r="AG13" s="5" t="n"/>
       <c r="AH13" s="5" t="n"/>
+      <c r="AK13" s="35" t="n"/>
+      <c r="AL13" s="29" t="inlineStr">
+        <is>
+          <t>Issue</t>
+        </is>
+      </c>
+      <c r="AM13" s="34" t="inlineStr">
+        <is>
+          <t>Vấn đề / Lỗi cần xử lý</t>
+        </is>
+      </c>
+      <c r="AN13" s="23" t="n"/>
+      <c r="AO13" s="26" t="n"/>
+      <c r="AP13" s="26" t="n"/>
+      <c r="AQ13" s="26" t="n"/>
+      <c r="AR13" s="26" t="n"/>
+      <c r="AS13" s="26" t="n"/>
+      <c r="AT13" s="26" t="n"/>
+      <c r="AU13" s="26" t="n"/>
+      <c r="AV13" s="23" t="n"/>
+      <c r="AW13" s="23" t="n"/>
+      <c r="AX13" s="23" t="n"/>
+      <c r="AY13" s="23" t="n"/>
+      <c r="AZ13" s="23" t="n"/>
+      <c r="BA13" s="23" t="n"/>
+      <c r="BB13" s="23" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="5" t="n"/>
@@ -1680,6 +2283,36 @@
       <c r="AF14" s="5" t="n"/>
       <c r="AG14" s="5" t="n"/>
       <c r="AH14" s="5" t="n"/>
+      <c r="AK14" s="32" t="inlineStr">
+        <is>
+          <t>Priority</t>
+        </is>
+      </c>
+      <c r="AL14" s="33" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="AM14" s="34" t="inlineStr">
+        <is>
+          <t>Ưu tiên cao - Cần xử lý gấp</t>
+        </is>
+      </c>
+      <c r="AN14" s="23" t="n"/>
+      <c r="AO14" s="26" t="n"/>
+      <c r="AP14" s="26" t="n"/>
+      <c r="AQ14" s="26" t="n"/>
+      <c r="AR14" s="26" t="n"/>
+      <c r="AS14" s="26" t="n"/>
+      <c r="AT14" s="26" t="n"/>
+      <c r="AU14" s="26" t="n"/>
+      <c r="AV14" s="23" t="n"/>
+      <c r="AW14" s="23" t="n"/>
+      <c r="AX14" s="23" t="n"/>
+      <c r="AY14" s="23" t="n"/>
+      <c r="AZ14" s="23" t="n"/>
+      <c r="BA14" s="23" t="n"/>
+      <c r="BB14" s="23" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="5" t="n"/>
@@ -1716,6 +2349,32 @@
       <c r="AF15" s="5" t="n"/>
       <c r="AG15" s="5" t="n"/>
       <c r="AH15" s="5" t="n"/>
+      <c r="AK15" s="35" t="n"/>
+      <c r="AL15" s="40" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="AM15" s="34" t="inlineStr">
+        <is>
+          <t>Ưu tiên trung bình</t>
+        </is>
+      </c>
+      <c r="AN15" s="23" t="n"/>
+      <c r="AO15" s="26" t="n"/>
+      <c r="AP15" s="26" t="n"/>
+      <c r="AQ15" s="26" t="n"/>
+      <c r="AR15" s="26" t="n"/>
+      <c r="AS15" s="26" t="n"/>
+      <c r="AT15" s="26" t="n"/>
+      <c r="AU15" s="26" t="n"/>
+      <c r="AV15" s="23" t="n"/>
+      <c r="AW15" s="23" t="n"/>
+      <c r="AX15" s="23" t="n"/>
+      <c r="AY15" s="23" t="n"/>
+      <c r="AZ15" s="23" t="n"/>
+      <c r="BA15" s="23" t="n"/>
+      <c r="BB15" s="23" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="5" t="n"/>
@@ -1752,6 +2411,32 @@
       <c r="AF16" s="5" t="n"/>
       <c r="AG16" s="5" t="n"/>
       <c r="AH16" s="5" t="n"/>
+      <c r="AK16" s="35" t="n"/>
+      <c r="AL16" s="37" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="AM16" s="34" t="inlineStr">
+        <is>
+          <t>Ưu tiên thấp</t>
+        </is>
+      </c>
+      <c r="AN16" s="23" t="n"/>
+      <c r="AO16" s="26" t="n"/>
+      <c r="AP16" s="26" t="n"/>
+      <c r="AQ16" s="26" t="n"/>
+      <c r="AR16" s="26" t="n"/>
+      <c r="AS16" s="26" t="n"/>
+      <c r="AT16" s="26" t="n"/>
+      <c r="AU16" s="26" t="n"/>
+      <c r="AV16" s="23" t="n"/>
+      <c r="AW16" s="23" t="n"/>
+      <c r="AX16" s="23" t="n"/>
+      <c r="AY16" s="23" t="n"/>
+      <c r="AZ16" s="23" t="n"/>
+      <c r="BA16" s="23" t="n"/>
+      <c r="BB16" s="23" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="5" t="n"/>
@@ -1788,6 +2473,24 @@
       <c r="AF17" s="5" t="n"/>
       <c r="AG17" s="5" t="n"/>
       <c r="AH17" s="5" t="n"/>
+      <c r="AK17" s="42" t="n"/>
+      <c r="AL17" s="42" t="n"/>
+      <c r="AM17" s="42" t="n"/>
+      <c r="AN17" s="23" t="n"/>
+      <c r="AO17" s="26" t="n"/>
+      <c r="AP17" s="26" t="n"/>
+      <c r="AQ17" s="26" t="n"/>
+      <c r="AR17" s="26" t="n"/>
+      <c r="AS17" s="26" t="n"/>
+      <c r="AT17" s="26" t="n"/>
+      <c r="AU17" s="26" t="n"/>
+      <c r="AV17" s="23" t="n"/>
+      <c r="AW17" s="23" t="n"/>
+      <c r="AX17" s="23" t="n"/>
+      <c r="AY17" s="23" t="n"/>
+      <c r="AZ17" s="23" t="n"/>
+      <c r="BA17" s="23" t="n"/>
+      <c r="BB17" s="23" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="5" t="n"/>
@@ -1824,6 +2527,24 @@
       <c r="AF18" s="5" t="n"/>
       <c r="AG18" s="5" t="n"/>
       <c r="AH18" s="5" t="n"/>
+      <c r="AK18" s="42" t="n"/>
+      <c r="AL18" s="42" t="n"/>
+      <c r="AM18" s="42" t="n"/>
+      <c r="AN18" s="23" t="n"/>
+      <c r="AO18" s="26" t="n"/>
+      <c r="AP18" s="26" t="n"/>
+      <c r="AQ18" s="26" t="n"/>
+      <c r="AR18" s="26" t="n"/>
+      <c r="AS18" s="26" t="n"/>
+      <c r="AT18" s="26" t="n"/>
+      <c r="AU18" s="26" t="n"/>
+      <c r="AV18" s="23" t="n"/>
+      <c r="AW18" s="23" t="n"/>
+      <c r="AX18" s="23" t="n"/>
+      <c r="AY18" s="23" t="n"/>
+      <c r="AZ18" s="23" t="n"/>
+      <c r="BA18" s="23" t="n"/>
+      <c r="BB18" s="23" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="5" t="n"/>
@@ -1860,6 +2581,24 @@
       <c r="AF19" s="5" t="n"/>
       <c r="AG19" s="5" t="n"/>
       <c r="AH19" s="5" t="n"/>
+      <c r="AK19" s="42" t="n"/>
+      <c r="AL19" s="42" t="n"/>
+      <c r="AM19" s="42" t="n"/>
+      <c r="AN19" s="23" t="n"/>
+      <c r="AO19" s="26" t="n"/>
+      <c r="AP19" s="26" t="n"/>
+      <c r="AQ19" s="26" t="n"/>
+      <c r="AR19" s="26" t="n"/>
+      <c r="AS19" s="26" t="n"/>
+      <c r="AT19" s="26" t="n"/>
+      <c r="AU19" s="26" t="n"/>
+      <c r="AV19" s="23" t="n"/>
+      <c r="AW19" s="23" t="n"/>
+      <c r="AX19" s="23" t="n"/>
+      <c r="AY19" s="23" t="n"/>
+      <c r="AZ19" s="23" t="n"/>
+      <c r="BA19" s="23" t="n"/>
+      <c r="BB19" s="23" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="5" t="n"/>
@@ -1896,6 +2635,24 @@
       <c r="AF20" s="5" t="n"/>
       <c r="AG20" s="5" t="n"/>
       <c r="AH20" s="5" t="n"/>
+      <c r="AK20" s="42" t="n"/>
+      <c r="AL20" s="42" t="n"/>
+      <c r="AM20" s="42" t="n"/>
+      <c r="AN20" s="23" t="n"/>
+      <c r="AO20" s="26" t="n"/>
+      <c r="AP20" s="26" t="n"/>
+      <c r="AQ20" s="26" t="n"/>
+      <c r="AR20" s="26" t="n"/>
+      <c r="AS20" s="26" t="n"/>
+      <c r="AT20" s="26" t="n"/>
+      <c r="AU20" s="26" t="n"/>
+      <c r="AV20" s="23" t="n"/>
+      <c r="AW20" s="23" t="n"/>
+      <c r="AX20" s="23" t="n"/>
+      <c r="AY20" s="23" t="n"/>
+      <c r="AZ20" s="23" t="n"/>
+      <c r="BA20" s="23" t="n"/>
+      <c r="BB20" s="23" t="n"/>
     </row>
     <row r="21">
       <c r="A21" s="5" t="n"/>
@@ -1932,6 +2689,24 @@
       <c r="AF21" s="5" t="n"/>
       <c r="AG21" s="5" t="n"/>
       <c r="AH21" s="5" t="n"/>
+      <c r="AK21" s="42" t="n"/>
+      <c r="AL21" s="42" t="n"/>
+      <c r="AM21" s="42" t="n"/>
+      <c r="AN21" s="23" t="n"/>
+      <c r="AO21" s="26" t="n"/>
+      <c r="AP21" s="26" t="n"/>
+      <c r="AQ21" s="26" t="n"/>
+      <c r="AR21" s="26" t="n"/>
+      <c r="AS21" s="26" t="n"/>
+      <c r="AT21" s="26" t="n"/>
+      <c r="AU21" s="26" t="n"/>
+      <c r="AV21" s="23" t="n"/>
+      <c r="AW21" s="23" t="n"/>
+      <c r="AX21" s="23" t="n"/>
+      <c r="AY21" s="23" t="n"/>
+      <c r="AZ21" s="23" t="n"/>
+      <c r="BA21" s="23" t="n"/>
+      <c r="BB21" s="23" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="5" t="n"/>
@@ -1968,6 +2743,26 @@
       <c r="AF22" s="5" t="n"/>
       <c r="AG22" s="5" t="n"/>
       <c r="AH22" s="5" t="n"/>
+      <c r="AK22" s="43" t="inlineStr">
+        <is>
+          <t>* Thêm giá trị mới vào các ô trống bên trên → tự cập nhật dropdown</t>
+        </is>
+      </c>
+      <c r="AN22" s="23" t="n"/>
+      <c r="AO22" s="26" t="n"/>
+      <c r="AP22" s="26" t="n"/>
+      <c r="AQ22" s="26" t="n"/>
+      <c r="AR22" s="26" t="n"/>
+      <c r="AS22" s="26" t="n"/>
+      <c r="AT22" s="26" t="n"/>
+      <c r="AU22" s="26" t="n"/>
+      <c r="AV22" s="23" t="n"/>
+      <c r="AW22" s="23" t="n"/>
+      <c r="AX22" s="23" t="n"/>
+      <c r="AY22" s="23" t="n"/>
+      <c r="AZ22" s="23" t="n"/>
+      <c r="BA22" s="23" t="n"/>
+      <c r="BB22" s="23" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="5" t="n"/>
@@ -2004,6 +2799,22 @@
       <c r="AF23" s="5" t="n"/>
       <c r="AG23" s="5" t="n"/>
       <c r="AH23" s="5" t="n"/>
+      <c r="AK23" s="23" t="n"/>
+      <c r="AL23" s="23" t="n"/>
+      <c r="AM23" s="23" t="n"/>
+      <c r="AN23" s="23" t="n"/>
+      <c r="AO23" s="43" t="inlineStr">
+        <is>
+          <t>* Thêm/xóa Board ở đây → tự cập nhật dropdown trong Tasks</t>
+        </is>
+      </c>
+      <c r="AV23" s="23" t="n"/>
+      <c r="AW23" s="23" t="n"/>
+      <c r="AX23" s="23" t="n"/>
+      <c r="AY23" s="23" t="n"/>
+      <c r="AZ23" s="23" t="n"/>
+      <c r="BA23" s="23" t="n"/>
+      <c r="BB23" s="23" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="5" t="n"/>
@@ -2040,6 +2851,24 @@
       <c r="AF24" s="5" t="n"/>
       <c r="AG24" s="5" t="n"/>
       <c r="AH24" s="5" t="n"/>
+      <c r="AK24" s="23" t="n"/>
+      <c r="AL24" s="23" t="n"/>
+      <c r="AM24" s="23" t="n"/>
+      <c r="AN24" s="23" t="n"/>
+      <c r="AO24" s="23" t="n"/>
+      <c r="AP24" s="23" t="n"/>
+      <c r="AQ24" s="23" t="n"/>
+      <c r="AR24" s="23" t="n"/>
+      <c r="AS24" s="23" t="n"/>
+      <c r="AT24" s="23" t="n"/>
+      <c r="AU24" s="23" t="n"/>
+      <c r="AV24" s="23" t="n"/>
+      <c r="AW24" s="23" t="n"/>
+      <c r="AX24" s="23" t="n"/>
+      <c r="AY24" s="23" t="n"/>
+      <c r="AZ24" s="23" t="n"/>
+      <c r="BA24" s="23" t="n"/>
+      <c r="BB24" s="23" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="5" t="n"/>
@@ -2076,6 +2905,24 @@
       <c r="AF25" s="5" t="n"/>
       <c r="AG25" s="5" t="n"/>
       <c r="AH25" s="5" t="n"/>
+      <c r="AK25" s="23" t="n"/>
+      <c r="AL25" s="23" t="n"/>
+      <c r="AM25" s="23" t="n"/>
+      <c r="AN25" s="23" t="n"/>
+      <c r="AO25" s="23" t="n"/>
+      <c r="AP25" s="23" t="n"/>
+      <c r="AQ25" s="23" t="n"/>
+      <c r="AR25" s="23" t="n"/>
+      <c r="AS25" s="23" t="n"/>
+      <c r="AT25" s="23" t="n"/>
+      <c r="AU25" s="23" t="n"/>
+      <c r="AV25" s="23" t="n"/>
+      <c r="AW25" s="23" t="n"/>
+      <c r="AX25" s="23" t="n"/>
+      <c r="AY25" s="23" t="n"/>
+      <c r="AZ25" s="23" t="n"/>
+      <c r="BA25" s="23" t="n"/>
+      <c r="BB25" s="23" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="5" t="n"/>
@@ -2112,6 +2959,24 @@
       <c r="AF26" s="5" t="n"/>
       <c r="AG26" s="5" t="n"/>
       <c r="AH26" s="5" t="n"/>
+      <c r="AK26" s="23" t="n"/>
+      <c r="AL26" s="23" t="n"/>
+      <c r="AM26" s="23" t="n"/>
+      <c r="AN26" s="23" t="n"/>
+      <c r="AO26" s="23" t="n"/>
+      <c r="AP26" s="23" t="n"/>
+      <c r="AQ26" s="23" t="n"/>
+      <c r="AR26" s="23" t="n"/>
+      <c r="AS26" s="23" t="n"/>
+      <c r="AT26" s="23" t="n"/>
+      <c r="AU26" s="23" t="n"/>
+      <c r="AV26" s="23" t="n"/>
+      <c r="AW26" s="23" t="n"/>
+      <c r="AX26" s="23" t="n"/>
+      <c r="AY26" s="23" t="n"/>
+      <c r="AZ26" s="23" t="n"/>
+      <c r="BA26" s="23" t="n"/>
+      <c r="BB26" s="23" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="5" t="n"/>
@@ -2148,6 +3013,24 @@
       <c r="AF27" s="5" t="n"/>
       <c r="AG27" s="5" t="n"/>
       <c r="AH27" s="5" t="n"/>
+      <c r="AK27" s="23" t="n"/>
+      <c r="AL27" s="23" t="n"/>
+      <c r="AM27" s="23" t="n"/>
+      <c r="AN27" s="23" t="n"/>
+      <c r="AO27" s="23" t="n"/>
+      <c r="AP27" s="23" t="n"/>
+      <c r="AQ27" s="23" t="n"/>
+      <c r="AR27" s="23" t="n"/>
+      <c r="AS27" s="23" t="n"/>
+      <c r="AT27" s="23" t="n"/>
+      <c r="AU27" s="23" t="n"/>
+      <c r="AV27" s="23" t="n"/>
+      <c r="AW27" s="23" t="n"/>
+      <c r="AX27" s="23" t="n"/>
+      <c r="AY27" s="23" t="n"/>
+      <c r="AZ27" s="23" t="n"/>
+      <c r="BA27" s="23" t="n"/>
+      <c r="BB27" s="23" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="5" t="n"/>
@@ -2184,6 +3067,24 @@
       <c r="AF28" s="5" t="n"/>
       <c r="AG28" s="5" t="n"/>
       <c r="AH28" s="5" t="n"/>
+      <c r="AK28" s="23" t="n"/>
+      <c r="AL28" s="23" t="n"/>
+      <c r="AM28" s="23" t="n"/>
+      <c r="AN28" s="23" t="n"/>
+      <c r="AO28" s="23" t="n"/>
+      <c r="AP28" s="23" t="n"/>
+      <c r="AQ28" s="23" t="n"/>
+      <c r="AR28" s="23" t="n"/>
+      <c r="AS28" s="23" t="n"/>
+      <c r="AT28" s="23" t="n"/>
+      <c r="AU28" s="23" t="n"/>
+      <c r="AV28" s="23" t="n"/>
+      <c r="AW28" s="23" t="n"/>
+      <c r="AX28" s="23" t="n"/>
+      <c r="AY28" s="23" t="n"/>
+      <c r="AZ28" s="23" t="n"/>
+      <c r="BA28" s="23" t="n"/>
+      <c r="BB28" s="23" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="5" t="n"/>
@@ -2220,6 +3121,24 @@
       <c r="AF29" s="5" t="n"/>
       <c r="AG29" s="5" t="n"/>
       <c r="AH29" s="5" t="n"/>
+      <c r="AK29" s="23" t="n"/>
+      <c r="AL29" s="23" t="n"/>
+      <c r="AM29" s="23" t="n"/>
+      <c r="AN29" s="23" t="n"/>
+      <c r="AO29" s="23" t="n"/>
+      <c r="AP29" s="23" t="n"/>
+      <c r="AQ29" s="23" t="n"/>
+      <c r="AR29" s="23" t="n"/>
+      <c r="AS29" s="23" t="n"/>
+      <c r="AT29" s="23" t="n"/>
+      <c r="AU29" s="23" t="n"/>
+      <c r="AV29" s="23" t="n"/>
+      <c r="AW29" s="23" t="n"/>
+      <c r="AX29" s="23" t="n"/>
+      <c r="AY29" s="23" t="n"/>
+      <c r="AZ29" s="23" t="n"/>
+      <c r="BA29" s="23" t="n"/>
+      <c r="BB29" s="23" t="n"/>
     </row>
     <row r="30">
       <c r="A30" s="5" t="n"/>
@@ -2256,6 +3175,24 @@
       <c r="AF30" s="5" t="n"/>
       <c r="AG30" s="5" t="n"/>
       <c r="AH30" s="5" t="n"/>
+      <c r="AK30" s="23" t="n"/>
+      <c r="AL30" s="23" t="n"/>
+      <c r="AM30" s="23" t="n"/>
+      <c r="AN30" s="23" t="n"/>
+      <c r="AO30" s="23" t="n"/>
+      <c r="AP30" s="23" t="n"/>
+      <c r="AQ30" s="23" t="n"/>
+      <c r="AR30" s="23" t="n"/>
+      <c r="AS30" s="23" t="n"/>
+      <c r="AT30" s="23" t="n"/>
+      <c r="AU30" s="23" t="n"/>
+      <c r="AV30" s="23" t="n"/>
+      <c r="AW30" s="23" t="n"/>
+      <c r="AX30" s="23" t="n"/>
+      <c r="AY30" s="23" t="n"/>
+      <c r="AZ30" s="23" t="n"/>
+      <c r="BA30" s="23" t="n"/>
+      <c r="BB30" s="23" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="5" t="n"/>
@@ -2292,6 +3229,24 @@
       <c r="AF31" s="5" t="n"/>
       <c r="AG31" s="5" t="n"/>
       <c r="AH31" s="5" t="n"/>
+      <c r="AK31" s="23" t="n"/>
+      <c r="AL31" s="23" t="n"/>
+      <c r="AM31" s="23" t="n"/>
+      <c r="AN31" s="23" t="n"/>
+      <c r="AO31" s="23" t="n"/>
+      <c r="AP31" s="23" t="n"/>
+      <c r="AQ31" s="23" t="n"/>
+      <c r="AR31" s="23" t="n"/>
+      <c r="AS31" s="23" t="n"/>
+      <c r="AT31" s="23" t="n"/>
+      <c r="AU31" s="23" t="n"/>
+      <c r="AV31" s="23" t="n"/>
+      <c r="AW31" s="23" t="n"/>
+      <c r="AX31" s="23" t="n"/>
+      <c r="AY31" s="23" t="n"/>
+      <c r="AZ31" s="23" t="n"/>
+      <c r="BA31" s="23" t="n"/>
+      <c r="BB31" s="23" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="5" t="n"/>
@@ -2328,6 +3283,24 @@
       <c r="AF32" s="5" t="n"/>
       <c r="AG32" s="5" t="n"/>
       <c r="AH32" s="5" t="n"/>
+      <c r="AK32" s="23" t="n"/>
+      <c r="AL32" s="23" t="n"/>
+      <c r="AM32" s="23" t="n"/>
+      <c r="AN32" s="23" t="n"/>
+      <c r="AO32" s="23" t="n"/>
+      <c r="AP32" s="23" t="n"/>
+      <c r="AQ32" s="23" t="n"/>
+      <c r="AR32" s="23" t="n"/>
+      <c r="AS32" s="23" t="n"/>
+      <c r="AT32" s="23" t="n"/>
+      <c r="AU32" s="23" t="n"/>
+      <c r="AV32" s="23" t="n"/>
+      <c r="AW32" s="23" t="n"/>
+      <c r="AX32" s="23" t="n"/>
+      <c r="AY32" s="23" t="n"/>
+      <c r="AZ32" s="23" t="n"/>
+      <c r="BA32" s="23" t="n"/>
+      <c r="BB32" s="23" t="n"/>
     </row>
     <row r="33">
       <c r="A33" s="5" t="n"/>
@@ -2364,6 +3337,24 @@
       <c r="AF33" s="5" t="n"/>
       <c r="AG33" s="5" t="n"/>
       <c r="AH33" s="5" t="n"/>
+      <c r="AK33" s="23" t="n"/>
+      <c r="AL33" s="23" t="n"/>
+      <c r="AM33" s="23" t="n"/>
+      <c r="AN33" s="23" t="n"/>
+      <c r="AO33" s="23" t="n"/>
+      <c r="AP33" s="23" t="n"/>
+      <c r="AQ33" s="23" t="n"/>
+      <c r="AR33" s="23" t="n"/>
+      <c r="AS33" s="23" t="n"/>
+      <c r="AT33" s="23" t="n"/>
+      <c r="AU33" s="23" t="n"/>
+      <c r="AV33" s="23" t="n"/>
+      <c r="AW33" s="23" t="n"/>
+      <c r="AX33" s="23" t="n"/>
+      <c r="AY33" s="23" t="n"/>
+      <c r="AZ33" s="23" t="n"/>
+      <c r="BA33" s="23" t="n"/>
+      <c r="BB33" s="23" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="5" t="n"/>
@@ -2400,6 +3391,24 @@
       <c r="AF34" s="5" t="n"/>
       <c r="AG34" s="5" t="n"/>
       <c r="AH34" s="5" t="n"/>
+      <c r="AK34" s="23" t="n"/>
+      <c r="AL34" s="23" t="n"/>
+      <c r="AM34" s="23" t="n"/>
+      <c r="AN34" s="23" t="n"/>
+      <c r="AO34" s="23" t="n"/>
+      <c r="AP34" s="23" t="n"/>
+      <c r="AQ34" s="23" t="n"/>
+      <c r="AR34" s="23" t="n"/>
+      <c r="AS34" s="23" t="n"/>
+      <c r="AT34" s="23" t="n"/>
+      <c r="AU34" s="23" t="n"/>
+      <c r="AV34" s="23" t="n"/>
+      <c r="AW34" s="23" t="n"/>
+      <c r="AX34" s="23" t="n"/>
+      <c r="AY34" s="23" t="n"/>
+      <c r="AZ34" s="23" t="n"/>
+      <c r="BA34" s="23" t="n"/>
+      <c r="BB34" s="23" t="n"/>
     </row>
     <row r="35">
       <c r="A35" s="5" t="n"/>
@@ -3050,7 +4059,8 @@
       <c r="AH52" s="5" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="32">
+    <mergeCell ref="AO1:AU1"/>
     <mergeCell ref="AB1:AB2"/>
     <mergeCell ref="AD1:AD2"/>
     <mergeCell ref="C1:C2"/>
@@ -3062,6 +4072,8 @@
     <mergeCell ref="W1:W2"/>
     <mergeCell ref="AH1:AH2"/>
     <mergeCell ref="Y1:Y2"/>
+    <mergeCell ref="AK1:AM1"/>
+    <mergeCell ref="AK22:AM22"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="D1:J1"/>
     <mergeCell ref="AC1:AC2"/>
@@ -3072,6 +4084,7 @@
     <mergeCell ref="T1:T2"/>
     <mergeCell ref="AF1:AF2"/>
     <mergeCell ref="X1:X2"/>
+    <mergeCell ref="AO23:AU23"/>
     <mergeCell ref="Z1:Z2"/>
     <mergeCell ref="S1:S2"/>
     <mergeCell ref="U1:U2"/>
@@ -3111,14 +4124,13 @@
       <formula>"Delay"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="3">
+  <dataValidations count="2">
     <dataValidation sqref="D3:J52" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"R,A,S,C,I"</formula1>
+      <formula1>=RASI_List</formula1>
     </dataValidation>
-    <dataValidation sqref="K10:AH52" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="K3:AH52" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"Plan,Active,Done,Delay"</formula1>
     </dataValidation>
-    <dataValidation sqref="K3:AH9" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1"/>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" paperSize="9"/>
@@ -33058,23 +34070,23 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation sqref="D2:D58" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Không hợp lệ" error="Board/Module chỉ áp dụng cho dự án MOT0200" type="list">
-      <formula1>=INDIRECT($B2)</formula1>
-    </dataValidation>
     <dataValidation sqref="B2:B58" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>Roadmap!$B$3:$B$100</formula1>
     </dataValidation>
+    <dataValidation sqref="D2:D58" showDropDown="0" showInputMessage="1" showErrorMessage="0" allowBlank="1" errorTitle="Board/Module" error="Board không hợp lệ. Kiểm tra thư viện định nghĩa trên Roadmap." promptTitle="Board/Module" prompt="Chọn Board/Module (cấu hình trên Roadmap)" type="list">
+      <formula1>=INDIRECT($B2)</formula1>
+    </dataValidation>
     <dataValidation sqref="F2:F58" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"Task,Issue"</formula1>
+      <formula1>=Type_List</formula1>
     </dataValidation>
     <dataValidation sqref="G2:G58" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"phudh2,kienlt44,hienpn2,khoavd11,anhlt25,huyldk,khanhttp"</formula1>
     </dataValidation>
     <dataValidation sqref="I2:I58" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"Open,Doing,Pending,Done"</formula1>
+      <formula1>=Status_List</formula1>
     </dataValidation>
     <dataValidation sqref="M2:M58" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"High,Medium,Low"</formula1>
+      <formula1>=Priority_List</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Fix Sub Project dependent dropdown, rename Board/Module -> Sub Project
Root cause: OFFSET formula in named ranges doesn't work reliably
with INDIRECT in Excel Data Validation.

Fix: Replace dynamic OFFSET named ranges with static cell references:
  - MOT0200 -> Roadmap!$AO$3:$AO$7 (5 sub-projects, exact range)
  - Other projects -> Roadmap!$BA$1 (empty cell, no dropdown items)

Also fixed: removed '=' prefix from INDIRECT formula in validation
(formula1='INDIRECT($B2)' instead of '=INDIRECT($B2)')

Other named ranges (Status_List, Type_List, Priority_List, RASI_List)
also cleaned up to use direct references without '=' prefix.

Renamed "Board/Module" -> "Sub Project" in Tasks header and Roadmap
library title.

https://claude.ai/code/session_015Yj1rKpkcryqiDrxyhDemu
</commit_message>
<xml_diff>
--- a/EE_Project_Dashboard.xlsx
+++ b/EE_Project_Dashboard.xlsx
@@ -10,17 +10,17 @@
     <sheet name="Tasks" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="MOT0200">'Roadmap'!$AO$3:$AO$7</definedName>
+    <definedName name="MOT0300">'Roadmap'!$BA$1</definedName>
+    <definedName name="HSCR01">'Roadmap'!$BA$1</definedName>
+    <definedName name="HBR00">'Roadmap'!$BA$1</definedName>
+    <definedName name="EMBPC00">'Roadmap'!$BA$1</definedName>
+    <definedName name="HCR00">'Roadmap'!$BA$1</definedName>
+    <definedName name="BATERY00">'Roadmap'!$BA$1</definedName>
     <definedName name="RASI_List">'Roadmap'!$AL$3:$AL$7</definedName>
     <definedName name="Status_List">'Roadmap'!$AL$8:$AL$11</definedName>
     <definedName name="Type_List">'Roadmap'!$AL$12:$AL$13</definedName>
     <definedName name="Priority_List">'Roadmap'!$AL$14:$AL$16</definedName>
-    <definedName name="MOT0200">OFFSET('Roadmap'!$AO$3,0,0,MAX(COUNTA('Roadmap'!$AO$3:$AO$22),1),1)</definedName>
-    <definedName name="MOT0300">OFFSET('Roadmap'!$AP$3,0,0,MAX(COUNTA('Roadmap'!$AP$3:$AP$22),1),1)</definedName>
-    <definedName name="HSCR01">OFFSET('Roadmap'!$AQ$3,0,0,MAX(COUNTA('Roadmap'!$AQ$3:$AQ$22),1),1)</definedName>
-    <definedName name="HBR00">OFFSET('Roadmap'!$AR$3,0,0,MAX(COUNTA('Roadmap'!$AR$3:$AR$22),1),1)</definedName>
-    <definedName name="EMBPC00">OFFSET('Roadmap'!$AS$3,0,0,MAX(COUNTA('Roadmap'!$AS$3:$AS$22),1),1)</definedName>
-    <definedName name="HCR00">OFFSET('Roadmap'!$AT$3,0,0,MAX(COUNTA('Roadmap'!$AT$3:$AT$22),1),1)</definedName>
-    <definedName name="BATERY00">OFFSET('Roadmap'!$AU$3,0,0,MAX(COUNTA('Roadmap'!$AU$3:$AU$22),1),1)</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Tasks'!$A$1:$M$58</definedName>
   </definedNames>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -33,7 +33,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
@@ -135,6 +135,11 @@
       <b val="1"/>
       <color rgb="FF495057"/>
       <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FFFFFFFF"/>
+      <sz val="1"/>
     </font>
   </fonts>
   <fills count="20">
@@ -415,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -520,6 +525,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1248,26 +1254,30 @@
           <t>THƯ VIỆN ĐỊNH NGHĨA</t>
         </is>
       </c>
-      <c r="AL1" s="22" t="n"/>
-      <c r="AM1" s="22" t="n"/>
+      <c r="AL1" s="12" t="n"/>
+      <c r="AM1" s="13" t="n"/>
       <c r="AN1" s="23" t="n"/>
       <c r="AO1" s="21" t="inlineStr">
         <is>
-          <t>BOARD / MODULE CHO TỪNG DỰ ÁN</t>
+          <t>SUB PROJECT CHO TỪNG DỰ ÁN</t>
         </is>
       </c>
-      <c r="AP1" s="22" t="n"/>
-      <c r="AQ1" s="22" t="n"/>
-      <c r="AR1" s="22" t="n"/>
-      <c r="AS1" s="22" t="n"/>
-      <c r="AT1" s="22" t="n"/>
-      <c r="AU1" s="22" t="n"/>
+      <c r="AP1" s="12" t="n"/>
+      <c r="AQ1" s="12" t="n"/>
+      <c r="AR1" s="12" t="n"/>
+      <c r="AS1" s="12" t="n"/>
+      <c r="AT1" s="12" t="n"/>
+      <c r="AU1" s="13" t="n"/>
       <c r="AV1" s="23" t="n"/>
       <c r="AW1" s="23" t="n"/>
       <c r="AX1" s="23" t="n"/>
       <c r="AY1" s="23" t="n"/>
       <c r="AZ1" s="23" t="n"/>
-      <c r="BA1" s="23" t="n"/>
+      <c r="BA1" s="44" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="BB1" s="23" t="n"/>
     </row>
     <row r="2" ht="58" customHeight="1">
@@ -2805,7 +2815,7 @@
       <c r="AN23" s="23" t="n"/>
       <c r="AO23" s="43" t="inlineStr">
         <is>
-          <t>* Thêm/xóa Board ở đây → tự cập nhật dropdown trong Tasks</t>
+          <t>* Thêm/xóa Sub Project ở đây. Sau khi thêm, vào Name Manager để mở rộng range.</t>
         </is>
       </c>
       <c r="AV23" s="23" t="n"/>
@@ -4126,7 +4136,7 @@
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation sqref="D3:J52" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>=RASI_List</formula1>
+      <formula1>RASI_List</formula1>
     </dataValidation>
     <dataValidation sqref="K3:AH52" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"Plan,Active,Done,Delay"</formula1>
@@ -4186,7 +4196,7 @@
       </c>
       <c r="D1" s="18" t="inlineStr">
         <is>
-          <t>Board/Module</t>
+          <t>Sub Project</t>
         </is>
       </c>
       <c r="E1" s="18" t="inlineStr">
@@ -34073,20 +34083,20 @@
     <dataValidation sqref="B2:B58" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>Roadmap!$B$3:$B$100</formula1>
     </dataValidation>
-    <dataValidation sqref="D2:D58" showDropDown="0" showInputMessage="1" showErrorMessage="0" allowBlank="1" errorTitle="Board/Module" error="Board không hợp lệ. Kiểm tra thư viện định nghĩa trên Roadmap." promptTitle="Board/Module" prompt="Chọn Board/Module (cấu hình trên Roadmap)" type="list">
-      <formula1>=INDIRECT($B2)</formula1>
+    <dataValidation sqref="D2:D58" showDropDown="0" showInputMessage="1" showErrorMessage="0" allowBlank="1" errorTitle="Sub Project" error="Sub Project không hợp lệ. Kiểm tra thư viện trên Roadmap." promptTitle="Sub Project" prompt="Chọn Sub Project (chỉ áp dụng cho dự án có sub-project)" type="list">
+      <formula1>INDIRECT($B2)</formula1>
     </dataValidation>
     <dataValidation sqref="F2:F58" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>=Type_List</formula1>
+      <formula1>Type_List</formula1>
     </dataValidation>
     <dataValidation sqref="G2:G58" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"phudh2,kienlt44,hienpn2,khoavd11,anhlt25,huyldk,khanhttp"</formula1>
     </dataValidation>
     <dataValidation sqref="I2:I58" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>=Status_List</formula1>
+      <formula1>Status_List</formula1>
     </dataValidation>
     <dataValidation sqref="M2:M58" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>=Priority_List</formula1>
+      <formula1>Priority_List</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Improve Definitions layout: color change guide, clearer Sub Project slots
- Add color change instructions (row 20-21): explains that colors are
  a visual reference only, and how to change conditional formatting
  colors via Home → Conditional Formatting → Manage Rules
- Add "(thêm ở đây)" placeholder in first empty slot of each project's
  Sub Project column to make it obvious where to add new values
- Rewrite hint text with numbered steps for adding new Sub Projects

https://claude.ai/code/session_015Yj1rKpkcryqiDrxyhDemu
</commit_message>
<xml_diff>
--- a/EE_Project_Dashboard.xlsx
+++ b/EE_Project_Dashboard.xlsx
@@ -34,7 +34,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="21">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
@@ -141,6 +141,18 @@
       <name val="Calibri"/>
       <color rgb="FFFFFFFF"/>
       <sz val="1"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <i val="1"/>
+      <color rgb="FF0070C0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <i val="1"/>
+      <color rgb="FFCCCCCC"/>
+      <sz val="9"/>
     </font>
   </fonts>
   <fills count="20">
@@ -421,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -528,6 +540,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -33935,19 +33954,19 @@
           <t>DROPDOWN DEFINITIONS</t>
         </is>
       </c>
-      <c r="B1" s="22" t="n"/>
-      <c r="C1" s="22" t="n"/>
+      <c r="B1" s="12" t="n"/>
+      <c r="C1" s="13" t="n"/>
       <c r="E1" s="21" t="inlineStr">
         <is>
           <t>SUB PROJECT THEO DỰ ÁN</t>
         </is>
       </c>
-      <c r="F1" s="22" t="n"/>
-      <c r="G1" s="22" t="n"/>
-      <c r="H1" s="22" t="n"/>
-      <c r="I1" s="22" t="n"/>
-      <c r="J1" s="22" t="n"/>
-      <c r="K1" s="22" t="n"/>
+      <c r="F1" s="12" t="n"/>
+      <c r="G1" s="12" t="n"/>
+      <c r="H1" s="12" t="n"/>
+      <c r="I1" s="12" t="n"/>
+      <c r="J1" s="12" t="n"/>
+      <c r="K1" s="13" t="n"/>
       <c r="Z1" s="45" t="inlineStr">
         <is>
           <t> </t>
@@ -34027,12 +34046,36 @@
           <t>PDU</t>
         </is>
       </c>
-      <c r="F3" s="26" t="n"/>
-      <c r="G3" s="26" t="n"/>
-      <c r="H3" s="26" t="n"/>
-      <c r="I3" s="26" t="n"/>
-      <c r="J3" s="26" t="n"/>
-      <c r="K3" s="26" t="n"/>
+      <c r="F3" s="46" t="inlineStr">
+        <is>
+          <t>(thêm ở đây)</t>
+        </is>
+      </c>
+      <c r="G3" s="46" t="inlineStr">
+        <is>
+          <t>(thêm ở đây)</t>
+        </is>
+      </c>
+      <c r="H3" s="46" t="inlineStr">
+        <is>
+          <t>(thêm ở đây)</t>
+        </is>
+      </c>
+      <c r="I3" s="46" t="inlineStr">
+        <is>
+          <t>(thêm ở đây)</t>
+        </is>
+      </c>
+      <c r="J3" s="46" t="inlineStr">
+        <is>
+          <t>(thêm ở đây)</t>
+        </is>
+      </c>
+      <c r="K3" s="46" t="inlineStr">
+        <is>
+          <t>(thêm ở đây)</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="35" t="n"/>
@@ -34146,7 +34189,11 @@
           <t>Chưa bắt đầu</t>
         </is>
       </c>
-      <c r="E8" s="26" t="n"/>
+      <c r="E8" s="46" t="inlineStr">
+        <is>
+          <t>(thêm ở đây)</t>
+        </is>
+      </c>
       <c r="F8" s="26" t="n"/>
       <c r="G8" s="26" t="n"/>
       <c r="H8" s="26" t="n"/>
@@ -34359,6 +34406,11 @@
       <c r="K19" s="26" t="n"/>
     </row>
     <row r="20">
+      <c r="A20" s="47" t="inlineStr">
+        <is>
+          <t>Lưu ý: Màu sắc ở đây là bảng tham chiếu. Để đổi màu hiển thị trên Roadmap/Tasks:</t>
+        </is>
+      </c>
       <c r="E20" s="26" t="n"/>
       <c r="F20" s="26" t="n"/>
       <c r="G20" s="26" t="n"/>
@@ -34368,6 +34420,11 @@
       <c r="K20" s="26" t="n"/>
     </row>
     <row r="21">
+      <c r="A21" s="47" t="inlineStr">
+        <is>
+          <t>→ Home → Conditional Formatting → Manage Rules → chọn rule cần sửa → Edit Rule → Format</t>
+        </is>
+      </c>
       <c r="E21" s="26" t="n"/>
       <c r="F21" s="26" t="n"/>
       <c r="G21" s="26" t="n"/>
@@ -34385,17 +34442,20 @@
       <c r="J22" s="26" t="n"/>
       <c r="K22" s="26" t="n"/>
     </row>
-    <row r="23">
-      <c r="E23" s="19" t="inlineStr">
+    <row r="23" ht="30" customHeight="1">
+      <c r="E23" s="48" t="inlineStr">
         <is>
-          <t>* Thêm Sub Project → gõ vào ô trống bên dưới. Nếu cần mở rộng, chỉnh Named Range trong Name Manager.</t>
+          <t>① Xóa text "(thêm ở đây)" → gõ tên Sub Project mới vào ô đó
+② Vào Formulas → Name Manager → chọn PRJ_&lt;mã dự án&gt; → sửa Refers to cho khớp</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
+    <mergeCell ref="E23:K23"/>
+    <mergeCell ref="A20:C20"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E23:K23"/>
+    <mergeCell ref="A21:C21"/>
     <mergeCell ref="E1:K1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Restructure Roadmap: replace monthly timeline with date-based versions
Replace 24 monthly columns (T1/2025-T12/2026) with structured columns:
  - Version (A, B, C...) - supports multiple versions per project
  - Start Date (DD/MM/YYYY)
  - End Date (DD/MM/YYYY)
  - Status (Plan/Active/Done/Delay) with conditional formatting
  - Notes

New layout:
  No | Project ID | Project Name | Version | RASI (7 employees) |
  Start Date | End Date | Status | Notes

MOT0200 (Motion 2) now has 3 version rows (A, B, C) as example.
Other projects have single rows (add versions as needed).

RASI shifted from D-J to E-K (to make room for Version column).
Freeze panes at E3 (freeze headers + first 4 columns).
Auto filter on row 2 for all columns.

https://claude.ai/code/session_015Yj1rKpkcryqiDrxyhDemu
</commit_message>
<xml_diff>
--- a/EE_Project_Dashboard.xlsx
+++ b/EE_Project_Dashboard.xlsx
@@ -22,6 +22,7 @@
     <definedName name="PRJ_EMBPC00">'Definitions'!$Z$1</definedName>
     <definedName name="PRJ_HCR00">'Definitions'!$Z$1</definedName>
     <definedName name="PRJ_BATERY00">'Definitions'!$Z$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Roadmap'!$A$2:$O$50</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Tasks'!$A$1:$M$58</definedName>
   </definedNames>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -433,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -546,6 +547,20 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="11" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1094,11 +1109,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BB52"/>
+  <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
       <selection pane="bottomRight" activeCell="M4" sqref="M4"/>
     </sheetView>
@@ -1107,9 +1124,19 @@
   <cols>
     <col width="5" customWidth="1" min="1" max="1"/>
     <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="50" customWidth="1" min="3" max="3"/>
-    <col width="6.81640625" customWidth="1" min="4" max="10"/>
+    <col width="48" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="10"/>
+    <col width="10" customWidth="1" min="5" max="5"/>
+    <col width="10" customWidth="1" min="6" max="6"/>
+    <col width="10" customWidth="1" min="7" max="7"/>
+    <col width="10" customWidth="1" min="8" max="8"/>
+    <col width="10" customWidth="1" min="9" max="9"/>
+    <col width="10" customWidth="1" min="10" max="10"/>
     <col width="10" customWidth="1" min="11" max="34"/>
+    <col width="14" customWidth="1" min="12" max="12"/>
+    <col width="14" customWidth="1" min="13" max="13"/>
+    <col width="12" customWidth="1" min="14" max="14"/>
+    <col width="40" customWidth="1" min="15" max="15"/>
     <col width="12" customWidth="1" min="37" max="37"/>
     <col width="12" customWidth="1" min="38" max="38"/>
     <col width="45" customWidth="1" min="39" max="39"/>
@@ -1123,153 +1150,79 @@
     <col width="16" customWidth="1" min="47" max="47"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16" customHeight="1">
-      <c r="A1" s="10" t="inlineStr">
+    <row r="1" ht="22" customHeight="1">
+      <c r="A1" s="18" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="B1" s="10" t="inlineStr">
+      <c r="B1" s="18" t="inlineStr">
         <is>
           <t>Project ID</t>
         </is>
       </c>
-      <c r="C1" s="10" t="inlineStr">
+      <c r="C1" s="18" t="inlineStr">
         <is>
           <t>Project Name</t>
         </is>
       </c>
-      <c r="D1" s="10" t="inlineStr">
+      <c r="D1" s="18" t="inlineStr">
+        <is>
+          <t>Version</t>
+        </is>
+      </c>
+      <c r="E1" s="18" t="inlineStr">
         <is>
           <t>RASI</t>
         </is>
       </c>
-      <c r="E1" s="12" t="n"/>
-      <c r="F1" s="12" t="n"/>
-      <c r="G1" s="12" t="n"/>
-      <c r="H1" s="12" t="n"/>
-      <c r="I1" s="12" t="n"/>
-      <c r="J1" s="13" t="n"/>
-      <c r="K1" s="10" t="inlineStr">
+      <c r="F1" s="49" t="n"/>
+      <c r="G1" s="49" t="n"/>
+      <c r="H1" s="49" t="n"/>
+      <c r="I1" s="49" t="n"/>
+      <c r="J1" s="49" t="n"/>
+      <c r="K1" s="49" t="n"/>
+      <c r="L1" s="18" t="inlineStr">
         <is>
-          <t>T1/2025</t>
+          <t>Start Date</t>
         </is>
       </c>
-      <c r="L1" s="10" t="inlineStr">
+      <c r="M1" s="18" t="inlineStr">
         <is>
-          <t>T2/2025</t>
+          <t>End Date</t>
         </is>
       </c>
-      <c r="M1" s="10" t="inlineStr">
+      <c r="N1" s="18" t="inlineStr">
         <is>
-          <t>T3/2025</t>
+          <t>Status</t>
         </is>
       </c>
-      <c r="N1" s="10" t="inlineStr">
+      <c r="O1" s="18" t="inlineStr">
         <is>
-          <t>T4/2025</t>
+          <t>Notes</t>
         </is>
       </c>
-      <c r="O1" s="10" t="inlineStr">
-        <is>
-          <t>T5/2025</t>
-        </is>
-      </c>
-      <c r="P1" s="10" t="inlineStr">
-        <is>
-          <t>T6/2025</t>
-        </is>
-      </c>
-      <c r="Q1" s="10" t="inlineStr">
-        <is>
-          <t>T7/2025</t>
-        </is>
-      </c>
-      <c r="R1" s="10" t="inlineStr">
-        <is>
-          <t>T8/2025</t>
-        </is>
-      </c>
-      <c r="S1" s="10" t="inlineStr">
-        <is>
-          <t>T9/2025</t>
-        </is>
-      </c>
-      <c r="T1" s="10" t="inlineStr">
-        <is>
-          <t>T10/2025</t>
-        </is>
-      </c>
-      <c r="U1" s="10" t="inlineStr">
-        <is>
-          <t>T11/2025</t>
-        </is>
-      </c>
-      <c r="V1" s="10" t="inlineStr">
-        <is>
-          <t>T12/2025</t>
-        </is>
-      </c>
-      <c r="W1" s="10" t="inlineStr">
-        <is>
-          <t>T1/2026</t>
-        </is>
-      </c>
-      <c r="X1" s="10" t="inlineStr">
-        <is>
-          <t>T2/2026</t>
-        </is>
-      </c>
-      <c r="Y1" s="10" t="inlineStr">
-        <is>
-          <t>T3/2026</t>
-        </is>
-      </c>
-      <c r="Z1" s="10" t="inlineStr">
-        <is>
-          <t>T4/2026</t>
-        </is>
-      </c>
-      <c r="AA1" s="10" t="inlineStr">
-        <is>
-          <t>T5/2026</t>
-        </is>
-      </c>
-      <c r="AB1" s="10" t="inlineStr">
-        <is>
-          <t>T6/2026</t>
-        </is>
-      </c>
-      <c r="AC1" s="10" t="inlineStr">
-        <is>
-          <t>T7/2026</t>
-        </is>
-      </c>
-      <c r="AD1" s="10" t="inlineStr">
-        <is>
-          <t>T8/2026</t>
-        </is>
-      </c>
-      <c r="AE1" s="10" t="inlineStr">
-        <is>
-          <t>T9/2026</t>
-        </is>
-      </c>
-      <c r="AF1" s="10" t="inlineStr">
-        <is>
-          <t>T10/2026</t>
-        </is>
-      </c>
-      <c r="AG1" s="10" t="inlineStr">
-        <is>
-          <t>T11/2026</t>
-        </is>
-      </c>
-      <c r="AH1" s="10" t="inlineStr">
-        <is>
-          <t>T12/2026</t>
-        </is>
-      </c>
+      <c r="P1" s="23" t="n"/>
+      <c r="Q1" s="23" t="n"/>
+      <c r="R1" s="23" t="n"/>
+      <c r="S1" s="23" t="n"/>
+      <c r="T1" s="23" t="n"/>
+      <c r="U1" s="23" t="n"/>
+      <c r="V1" s="23" t="n"/>
+      <c r="W1" s="23" t="n"/>
+      <c r="X1" s="23" t="n"/>
+      <c r="Y1" s="23" t="n"/>
+      <c r="Z1" s="23" t="n"/>
+      <c r="AA1" s="23" t="n"/>
+      <c r="AB1" s="23" t="n"/>
+      <c r="AC1" s="23" t="n"/>
+      <c r="AD1" s="23" t="n"/>
+      <c r="AE1" s="23" t="n"/>
+      <c r="AF1" s="23" t="n"/>
+      <c r="AG1" s="23" t="n"/>
+      <c r="AH1" s="23" t="n"/>
+      <c r="AI1" s="23" t="n"/>
+      <c r="AJ1" s="23" t="n"/>
       <c r="AK1" s="23" t="n"/>
       <c r="AL1" s="23" t="n"/>
       <c r="AM1" s="23" t="n"/>
@@ -1289,69 +1242,71 @@
       <c r="BA1" s="23" t="n"/>
       <c r="BB1" s="23" t="n"/>
     </row>
-    <row r="2" ht="58" customHeight="1">
-      <c r="A2" s="11" t="n"/>
-      <c r="B2" s="11" t="n"/>
-      <c r="C2" s="11" t="n"/>
-      <c r="D2" s="8" t="inlineStr">
+    <row r="2" ht="30" customHeight="1">
+      <c r="A2" s="50" t="n"/>
+      <c r="B2" s="50" t="n"/>
+      <c r="C2" s="50" t="n"/>
+      <c r="D2" s="50" t="n"/>
+      <c r="E2" s="51" t="inlineStr">
         <is>
           <t>Đinh Hoàng Phú</t>
         </is>
       </c>
-      <c r="E2" s="8" t="inlineStr">
+      <c r="F2" s="51" t="inlineStr">
         <is>
           <t>Lê Trí Kiên</t>
         </is>
       </c>
-      <c r="F2" s="8" t="inlineStr">
+      <c r="G2" s="51" t="inlineStr">
         <is>
           <t>Phạm Nam Hiền</t>
         </is>
       </c>
-      <c r="G2" s="8" t="inlineStr">
+      <c r="H2" s="51" t="inlineStr">
         <is>
           <t>Vũ Đăng Khoa</t>
         </is>
       </c>
-      <c r="H2" s="8" t="inlineStr">
+      <c r="I2" s="51" t="inlineStr">
         <is>
           <t>Lê Tiến Anh</t>
         </is>
       </c>
-      <c r="I2" s="8" t="inlineStr">
+      <c r="J2" s="51" t="inlineStr">
         <is>
           <t>Lê Dương Khánh Huy</t>
         </is>
       </c>
-      <c r="J2" s="8" t="inlineStr">
+      <c r="K2" s="51" t="inlineStr">
         <is>
           <t>Tôn Thất Phúc Khánh</t>
         </is>
       </c>
-      <c r="K2" s="11" t="n"/>
-      <c r="L2" s="11" t="n"/>
-      <c r="M2" s="11" t="n"/>
-      <c r="N2" s="11" t="n"/>
-      <c r="O2" s="11" t="n"/>
-      <c r="P2" s="11" t="n"/>
-      <c r="Q2" s="11" t="n"/>
-      <c r="R2" s="11" t="n"/>
-      <c r="S2" s="11" t="n"/>
-      <c r="T2" s="11" t="n"/>
-      <c r="U2" s="11" t="n"/>
-      <c r="V2" s="11" t="n"/>
-      <c r="W2" s="11" t="n"/>
-      <c r="X2" s="11" t="n"/>
-      <c r="Y2" s="11" t="n"/>
-      <c r="Z2" s="11" t="n"/>
-      <c r="AA2" s="11" t="n"/>
-      <c r="AB2" s="11" t="n"/>
-      <c r="AC2" s="11" t="n"/>
-      <c r="AD2" s="11" t="n"/>
-      <c r="AE2" s="11" t="n"/>
-      <c r="AF2" s="11" t="n"/>
-      <c r="AG2" s="11" t="n"/>
-      <c r="AH2" s="11" t="n"/>
+      <c r="L2" s="50" t="n"/>
+      <c r="M2" s="50" t="n"/>
+      <c r="N2" s="50" t="n"/>
+      <c r="O2" s="50" t="n"/>
+      <c r="P2" s="23" t="n"/>
+      <c r="Q2" s="23" t="n"/>
+      <c r="R2" s="23" t="n"/>
+      <c r="S2" s="23" t="n"/>
+      <c r="T2" s="23" t="n"/>
+      <c r="U2" s="23" t="n"/>
+      <c r="V2" s="23" t="n"/>
+      <c r="W2" s="23" t="n"/>
+      <c r="X2" s="23" t="n"/>
+      <c r="Y2" s="23" t="n"/>
+      <c r="Z2" s="23" t="n"/>
+      <c r="AA2" s="23" t="n"/>
+      <c r="AB2" s="23" t="n"/>
+      <c r="AC2" s="23" t="n"/>
+      <c r="AD2" s="23" t="n"/>
+      <c r="AE2" s="23" t="n"/>
+      <c r="AF2" s="23" t="n"/>
+      <c r="AG2" s="23" t="n"/>
+      <c r="AH2" s="23" t="n"/>
+      <c r="AI2" s="23" t="n"/>
+      <c r="AJ2" s="23" t="n"/>
       <c r="AK2" s="23" t="n"/>
       <c r="AL2" s="23" t="n"/>
       <c r="AM2" s="23" t="n"/>
@@ -1372,78 +1327,88 @@
       <c r="BB2" s="23" t="n"/>
     </row>
     <row r="3" ht="45.5" customHeight="1">
-      <c r="A3" s="5" t="n">
+      <c r="A3" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="inlineStr">
+      <c r="B3" s="14" t="inlineStr">
         <is>
           <t>MOT0200</t>
         </is>
       </c>
-      <c r="C3" s="6" t="inlineStr">
+      <c r="C3" s="15" t="inlineStr">
         <is>
           <t>Dự án phát triển Motion 2</t>
         </is>
       </c>
-      <c r="D3" s="5" t="inlineStr">
+      <c r="D3" s="14" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E3" s="14" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="E3" s="5" t="inlineStr">
+      <c r="F3" s="14" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="F3" s="5" t="inlineStr">
+      <c r="G3" s="14" t="inlineStr">
         <is>
           <t>S</t>
         </is>
       </c>
-      <c r="G3" s="9" t="inlineStr">
+      <c r="H3" s="14" t="inlineStr">
         <is>
           <t>S</t>
         </is>
       </c>
-      <c r="H3" s="5" t="inlineStr">
+      <c r="I3" s="14" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="I3" s="5" t="inlineStr">
+      <c r="J3" s="14" t="inlineStr">
         <is>
           <t>S</t>
         </is>
       </c>
-      <c r="J3" s="5" t="inlineStr">
+      <c r="K3" s="14" t="inlineStr">
         <is>
           <t>S</t>
         </is>
       </c>
-      <c r="K3" s="5" t="n"/>
-      <c r="L3" s="5" t="n"/>
-      <c r="M3" s="5" t="n"/>
-      <c r="N3" s="5" t="n"/>
-      <c r="O3" s="5" t="n"/>
-      <c r="P3" s="5" t="n"/>
-      <c r="Q3" s="5" t="n"/>
-      <c r="R3" s="5" t="n"/>
-      <c r="S3" s="5" t="n"/>
-      <c r="T3" s="5" t="n"/>
-      <c r="U3" s="5" t="n"/>
-      <c r="V3" s="5" t="n"/>
-      <c r="W3" s="5" t="n"/>
-      <c r="X3" s="5" t="n"/>
-      <c r="Y3" s="5" t="n"/>
-      <c r="Z3" s="5" t="n"/>
-      <c r="AA3" s="5" t="n"/>
-      <c r="AB3" s="5" t="n"/>
-      <c r="AC3" s="5" t="n"/>
-      <c r="AD3" s="5" t="n"/>
-      <c r="AE3" s="5" t="n"/>
-      <c r="AF3" s="5" t="n"/>
-      <c r="AG3" s="5" t="n"/>
-      <c r="AH3" s="5" t="n"/>
+      <c r="L3" s="16" t="n"/>
+      <c r="M3" s="16" t="n"/>
+      <c r="N3" s="14" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="O3" s="15" t="n"/>
+      <c r="P3" s="23" t="n"/>
+      <c r="Q3" s="23" t="n"/>
+      <c r="R3" s="23" t="n"/>
+      <c r="S3" s="23" t="n"/>
+      <c r="T3" s="23" t="n"/>
+      <c r="U3" s="23" t="n"/>
+      <c r="V3" s="23" t="n"/>
+      <c r="W3" s="23" t="n"/>
+      <c r="X3" s="23" t="n"/>
+      <c r="Y3" s="23" t="n"/>
+      <c r="Z3" s="23" t="n"/>
+      <c r="AA3" s="23" t="n"/>
+      <c r="AB3" s="23" t="n"/>
+      <c r="AC3" s="23" t="n"/>
+      <c r="AD3" s="23" t="n"/>
+      <c r="AE3" s="23" t="n"/>
+      <c r="AF3" s="23" t="n"/>
+      <c r="AG3" s="23" t="n"/>
+      <c r="AH3" s="23" t="n"/>
+      <c r="AI3" s="23" t="n"/>
+      <c r="AJ3" s="23" t="n"/>
       <c r="AK3" s="23" t="n"/>
       <c r="AL3" s="23" t="n"/>
       <c r="AM3" s="23" t="n"/>
@@ -1464,58 +1429,60 @@
       <c r="BB3" s="23" t="n"/>
     </row>
     <row r="4" ht="45.5" customHeight="1">
-      <c r="A4" s="5" t="n">
+      <c r="A4" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="inlineStr">
+      <c r="B4" s="14" t="inlineStr">
         <is>
-          <t>MOT0300</t>
+          <t>MOT0200</t>
         </is>
       </c>
-      <c r="C4" s="6" t="inlineStr">
+      <c r="C4" s="15" t="inlineStr">
         <is>
-          <t>Dự án phát triển Motion 3</t>
+          <t>Dự án phát triển Motion 2</t>
         </is>
       </c>
-      <c r="D4" s="9" t="n"/>
-      <c r="E4" s="9" t="inlineStr">
+      <c r="D4" s="14" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>B</t>
         </is>
       </c>
-      <c r="F4" s="9" t="inlineStr">
+      <c r="E4" s="14" t="n"/>
+      <c r="F4" s="14" t="n"/>
+      <c r="G4" s="14" t="n"/>
+      <c r="H4" s="14" t="n"/>
+      <c r="I4" s="14" t="n"/>
+      <c r="J4" s="14" t="n"/>
+      <c r="K4" s="14" t="n"/>
+      <c r="L4" s="16" t="n"/>
+      <c r="M4" s="16" t="n"/>
+      <c r="N4" s="14" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>Plan</t>
         </is>
       </c>
-      <c r="G4" s="9" t="n"/>
-      <c r="H4" s="9" t="n"/>
-      <c r="I4" s="9" t="n"/>
-      <c r="J4" s="9" t="n"/>
-      <c r="K4" s="5" t="n"/>
-      <c r="L4" s="5" t="n"/>
-      <c r="M4" s="5" t="n"/>
-      <c r="N4" s="5" t="n"/>
-      <c r="O4" s="5" t="n"/>
-      <c r="P4" s="5" t="n"/>
-      <c r="Q4" s="5" t="n"/>
-      <c r="R4" s="5" t="n"/>
-      <c r="S4" s="5" t="n"/>
-      <c r="T4" s="5" t="n"/>
-      <c r="U4" s="5" t="n"/>
-      <c r="V4" s="5" t="n"/>
-      <c r="W4" s="5" t="n"/>
-      <c r="X4" s="5" t="n"/>
-      <c r="Y4" s="5" t="n"/>
-      <c r="Z4" s="5" t="n"/>
-      <c r="AA4" s="5" t="n"/>
-      <c r="AB4" s="5" t="n"/>
-      <c r="AC4" s="5" t="n"/>
-      <c r="AD4" s="5" t="n"/>
-      <c r="AE4" s="5" t="n"/>
-      <c r="AF4" s="5" t="n"/>
-      <c r="AG4" s="5" t="n"/>
-      <c r="AH4" s="5" t="n"/>
+      <c r="O4" s="15" t="n"/>
+      <c r="P4" s="23" t="n"/>
+      <c r="Q4" s="23" t="n"/>
+      <c r="R4" s="23" t="n"/>
+      <c r="S4" s="23" t="n"/>
+      <c r="T4" s="23" t="n"/>
+      <c r="U4" s="23" t="n"/>
+      <c r="V4" s="23" t="n"/>
+      <c r="W4" s="23" t="n"/>
+      <c r="X4" s="23" t="n"/>
+      <c r="Y4" s="23" t="n"/>
+      <c r="Z4" s="23" t="n"/>
+      <c r="AA4" s="23" t="n"/>
+      <c r="AB4" s="23" t="n"/>
+      <c r="AC4" s="23" t="n"/>
+      <c r="AD4" s="23" t="n"/>
+      <c r="AE4" s="23" t="n"/>
+      <c r="AF4" s="23" t="n"/>
+      <c r="AG4" s="23" t="n"/>
+      <c r="AH4" s="23" t="n"/>
+      <c r="AI4" s="23" t="n"/>
+      <c r="AJ4" s="23" t="n"/>
       <c r="AK4" s="23" t="n"/>
       <c r="AL4" s="23" t="n"/>
       <c r="AM4" s="23" t="n"/>
@@ -1536,62 +1503,60 @@
       <c r="BB4" s="23" t="n"/>
     </row>
     <row r="5" ht="45.5" customHeight="1">
-      <c r="A5" s="5" t="n">
+      <c r="A5" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="inlineStr">
+      <c r="B5" s="14" t="inlineStr">
         <is>
-          <t>HSCR01</t>
+          <t>MOT0200</t>
         </is>
       </c>
-      <c r="C5" s="6" t="inlineStr">
+      <c r="C5" s="15" t="inlineStr">
         <is>
-          <t>Dự án NC trạm sạc và thay pin cho Robot VMO</t>
+          <t>Dự án phát triển Motion 2</t>
         </is>
       </c>
-      <c r="D5" s="9" t="n"/>
-      <c r="E5" s="5" t="inlineStr">
+      <c r="D5" s="14" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>C</t>
         </is>
       </c>
-      <c r="F5" s="5" t="inlineStr">
+      <c r="E5" s="14" t="n"/>
+      <c r="F5" s="14" t="n"/>
+      <c r="G5" s="14" t="n"/>
+      <c r="H5" s="14" t="n"/>
+      <c r="I5" s="14" t="n"/>
+      <c r="J5" s="14" t="n"/>
+      <c r="K5" s="14" t="n"/>
+      <c r="L5" s="16" t="n"/>
+      <c r="M5" s="16" t="n"/>
+      <c r="N5" s="14" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>Plan</t>
         </is>
       </c>
-      <c r="G5" s="9" t="n"/>
-      <c r="H5" s="9" t="n"/>
-      <c r="I5" s="5" t="inlineStr">
-        <is>
-          <t>S</t>
-        </is>
-      </c>
-      <c r="J5" s="9" t="n"/>
-      <c r="K5" s="5" t="n"/>
-      <c r="L5" s="5" t="n"/>
-      <c r="M5" s="5" t="n"/>
-      <c r="N5" s="5" t="n"/>
-      <c r="O5" s="5" t="n"/>
-      <c r="P5" s="5" t="n"/>
-      <c r="Q5" s="5" t="n"/>
-      <c r="R5" s="5" t="n"/>
-      <c r="S5" s="5" t="n"/>
-      <c r="T5" s="5" t="n"/>
-      <c r="U5" s="5" t="n"/>
-      <c r="V5" s="5" t="n"/>
-      <c r="W5" s="5" t="n"/>
-      <c r="X5" s="5" t="n"/>
-      <c r="Y5" s="5" t="n"/>
-      <c r="Z5" s="5" t="n"/>
-      <c r="AA5" s="5" t="n"/>
-      <c r="AB5" s="5" t="n"/>
-      <c r="AC5" s="5" t="n"/>
-      <c r="AD5" s="5" t="n"/>
-      <c r="AE5" s="5" t="n"/>
-      <c r="AF5" s="5" t="n"/>
-      <c r="AG5" s="5" t="n"/>
-      <c r="AH5" s="5" t="n"/>
+      <c r="O5" s="15" t="n"/>
+      <c r="P5" s="23" t="n"/>
+      <c r="Q5" s="23" t="n"/>
+      <c r="R5" s="23" t="n"/>
+      <c r="S5" s="23" t="n"/>
+      <c r="T5" s="23" t="n"/>
+      <c r="U5" s="23" t="n"/>
+      <c r="V5" s="23" t="n"/>
+      <c r="W5" s="23" t="n"/>
+      <c r="X5" s="23" t="n"/>
+      <c r="Y5" s="23" t="n"/>
+      <c r="Z5" s="23" t="n"/>
+      <c r="AA5" s="23" t="n"/>
+      <c r="AB5" s="23" t="n"/>
+      <c r="AC5" s="23" t="n"/>
+      <c r="AD5" s="23" t="n"/>
+      <c r="AE5" s="23" t="n"/>
+      <c r="AF5" s="23" t="n"/>
+      <c r="AG5" s="23" t="n"/>
+      <c r="AH5" s="23" t="n"/>
+      <c r="AI5" s="23" t="n"/>
+      <c r="AJ5" s="23" t="n"/>
       <c r="AK5" s="23" t="n"/>
       <c r="AL5" s="23" t="n"/>
       <c r="AM5" s="23" t="n"/>
@@ -1612,54 +1577,64 @@
       <c r="BB5" s="23" t="n"/>
     </row>
     <row r="6" ht="45.5" customHeight="1">
-      <c r="A6" s="5" t="n">
+      <c r="A6" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="5" t="inlineStr">
+      <c r="B6" s="14" t="inlineStr">
         <is>
-          <t>HBR00</t>
+          <t>MOT0300</t>
         </is>
       </c>
-      <c r="C6" s="6" t="inlineStr">
+      <c r="C6" s="15" t="inlineStr">
         <is>
-          <t>Dự án NC bàn tay Robot VMO</t>
+          <t>Dự án phát triển Motion 3</t>
         </is>
       </c>
-      <c r="D6" s="9" t="n"/>
-      <c r="E6" s="9" t="n"/>
-      <c r="F6" s="9" t="n"/>
-      <c r="G6" s="5" t="inlineStr">
+      <c r="D6" s="14" t="n"/>
+      <c r="E6" s="14" t="n"/>
+      <c r="F6" s="14" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="H6" s="9" t="n"/>
-      <c r="I6" s="9" t="n"/>
-      <c r="J6" s="9" t="n"/>
-      <c r="K6" s="5" t="n"/>
-      <c r="L6" s="5" t="n"/>
-      <c r="M6" s="5" t="n"/>
-      <c r="N6" s="5" t="n"/>
-      <c r="O6" s="5" t="n"/>
-      <c r="P6" s="5" t="n"/>
-      <c r="Q6" s="5" t="n"/>
-      <c r="R6" s="5" t="n"/>
-      <c r="S6" s="5" t="n"/>
-      <c r="T6" s="5" t="n"/>
-      <c r="U6" s="5" t="n"/>
-      <c r="V6" s="5" t="n"/>
-      <c r="W6" s="5" t="n"/>
-      <c r="X6" s="5" t="n"/>
-      <c r="Y6" s="5" t="n"/>
-      <c r="Z6" s="5" t="n"/>
-      <c r="AA6" s="5" t="n"/>
-      <c r="AB6" s="5" t="n"/>
-      <c r="AC6" s="5" t="n"/>
-      <c r="AD6" s="5" t="n"/>
-      <c r="AE6" s="5" t="n"/>
-      <c r="AF6" s="5" t="n"/>
-      <c r="AG6" s="5" t="n"/>
-      <c r="AH6" s="5" t="n"/>
+      <c r="G6" s="14" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="H6" s="14" t="n"/>
+      <c r="I6" s="14" t="n"/>
+      <c r="J6" s="14" t="n"/>
+      <c r="K6" s="14" t="n"/>
+      <c r="L6" s="16" t="n"/>
+      <c r="M6" s="16" t="n"/>
+      <c r="N6" s="14" t="inlineStr">
+        <is>
+          <t>Plan</t>
+        </is>
+      </c>
+      <c r="O6" s="15" t="n"/>
+      <c r="P6" s="23" t="n"/>
+      <c r="Q6" s="23" t="n"/>
+      <c r="R6" s="23" t="n"/>
+      <c r="S6" s="23" t="n"/>
+      <c r="T6" s="23" t="n"/>
+      <c r="U6" s="23" t="n"/>
+      <c r="V6" s="23" t="n"/>
+      <c r="W6" s="23" t="n"/>
+      <c r="X6" s="23" t="n"/>
+      <c r="Y6" s="23" t="n"/>
+      <c r="Z6" s="23" t="n"/>
+      <c r="AA6" s="23" t="n"/>
+      <c r="AB6" s="23" t="n"/>
+      <c r="AC6" s="23" t="n"/>
+      <c r="AD6" s="23" t="n"/>
+      <c r="AE6" s="23" t="n"/>
+      <c r="AF6" s="23" t="n"/>
+      <c r="AG6" s="23" t="n"/>
+      <c r="AH6" s="23" t="n"/>
+      <c r="AI6" s="23" t="n"/>
+      <c r="AJ6" s="23" t="n"/>
       <c r="AK6" s="23" t="n"/>
       <c r="AL6" s="23" t="n"/>
       <c r="AM6" s="23" t="n"/>
@@ -1680,54 +1655,68 @@
       <c r="BB6" s="23" t="n"/>
     </row>
     <row r="7" ht="45.5" customHeight="1">
-      <c r="A7" s="5" t="n">
+      <c r="A7" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="5" t="inlineStr">
+      <c r="B7" s="14" t="inlineStr">
         <is>
-          <t>EMBPC00</t>
+          <t>HSCR01</t>
         </is>
       </c>
-      <c r="C7" s="6" t="inlineStr">
+      <c r="C7" s="15" t="inlineStr">
         <is>
-          <t>Dự án máy tính nhúng VMO</t>
+          <t>Dự án NC trạm sạc và thay pin cho Robot VMO</t>
         </is>
       </c>
-      <c r="D7" s="5" t="inlineStr">
+      <c r="D7" s="14" t="n"/>
+      <c r="E7" s="14" t="n"/>
+      <c r="F7" s="14" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="E7" s="9" t="n"/>
-      <c r="F7" s="9" t="n"/>
-      <c r="G7" s="9" t="n"/>
-      <c r="H7" s="9" t="n"/>
-      <c r="I7" s="9" t="n"/>
-      <c r="J7" s="9" t="n"/>
-      <c r="K7" s="5" t="n"/>
-      <c r="L7" s="5" t="n"/>
-      <c r="M7" s="5" t="n"/>
-      <c r="N7" s="5" t="n"/>
-      <c r="O7" s="5" t="n"/>
-      <c r="P7" s="5" t="n"/>
-      <c r="Q7" s="5" t="n"/>
-      <c r="R7" s="5" t="n"/>
-      <c r="S7" s="5" t="n"/>
-      <c r="T7" s="5" t="n"/>
-      <c r="U7" s="5" t="n"/>
-      <c r="V7" s="5" t="n"/>
-      <c r="W7" s="5" t="n"/>
-      <c r="X7" s="5" t="n"/>
-      <c r="Y7" s="5" t="n"/>
-      <c r="Z7" s="5" t="n"/>
-      <c r="AA7" s="5" t="n"/>
-      <c r="AB7" s="5" t="n"/>
-      <c r="AC7" s="5" t="n"/>
-      <c r="AD7" s="5" t="n"/>
-      <c r="AE7" s="5" t="n"/>
-      <c r="AF7" s="5" t="n"/>
-      <c r="AG7" s="5" t="n"/>
-      <c r="AH7" s="5" t="n"/>
+      <c r="G7" s="14" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="H7" s="14" t="n"/>
+      <c r="I7" s="14" t="n"/>
+      <c r="J7" s="14" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="K7" s="14" t="n"/>
+      <c r="L7" s="16" t="n"/>
+      <c r="M7" s="16" t="n"/>
+      <c r="N7" s="14" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="O7" s="15" t="n"/>
+      <c r="P7" s="23" t="n"/>
+      <c r="Q7" s="23" t="n"/>
+      <c r="R7" s="23" t="n"/>
+      <c r="S7" s="23" t="n"/>
+      <c r="T7" s="23" t="n"/>
+      <c r="U7" s="23" t="n"/>
+      <c r="V7" s="23" t="n"/>
+      <c r="W7" s="23" t="n"/>
+      <c r="X7" s="23" t="n"/>
+      <c r="Y7" s="23" t="n"/>
+      <c r="Z7" s="23" t="n"/>
+      <c r="AA7" s="23" t="n"/>
+      <c r="AB7" s="23" t="n"/>
+      <c r="AC7" s="23" t="n"/>
+      <c r="AD7" s="23" t="n"/>
+      <c r="AE7" s="23" t="n"/>
+      <c r="AF7" s="23" t="n"/>
+      <c r="AG7" s="23" t="n"/>
+      <c r="AH7" s="23" t="n"/>
+      <c r="AI7" s="23" t="n"/>
+      <c r="AJ7" s="23" t="n"/>
       <c r="AK7" s="23" t="n"/>
       <c r="AL7" s="23" t="n"/>
       <c r="AM7" s="23" t="n"/>
@@ -1748,62 +1737,60 @@
       <c r="BB7" s="23" t="n"/>
     </row>
     <row r="8" ht="45.5" customHeight="1">
-      <c r="A8" s="5" t="n">
+      <c r="A8" s="14" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="5" t="inlineStr">
+      <c r="B8" s="14" t="inlineStr">
         <is>
-          <t>HCR00</t>
+          <t>HBR00</t>
         </is>
       </c>
-      <c r="C8" s="6" t="inlineStr">
+      <c r="C8" s="15" t="inlineStr">
         <is>
-          <t>Dự án tay cầm điều khiển từ xa VMO</t>
+          <t>Dự án NC bàn tay Robot VMO</t>
         </is>
       </c>
-      <c r="D8" s="9" t="n"/>
-      <c r="E8" s="5" t="inlineStr">
+      <c r="D8" s="14" t="n"/>
+      <c r="E8" s="14" t="n"/>
+      <c r="F8" s="14" t="n"/>
+      <c r="G8" s="14" t="n"/>
+      <c r="H8" s="14" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="F8" s="9" t="inlineStr">
+      <c r="I8" s="14" t="n"/>
+      <c r="J8" s="14" t="n"/>
+      <c r="K8" s="14" t="n"/>
+      <c r="L8" s="16" t="n"/>
+      <c r="M8" s="16" t="n"/>
+      <c r="N8" s="14" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>Active</t>
         </is>
       </c>
-      <c r="G8" s="9" t="inlineStr">
-        <is>
-          <t>S</t>
-        </is>
-      </c>
-      <c r="H8" s="9" t="n"/>
-      <c r="I8" s="9" t="n"/>
-      <c r="J8" s="9" t="n"/>
-      <c r="K8" s="5" t="n"/>
-      <c r="L8" s="5" t="n"/>
-      <c r="M8" s="5" t="n"/>
-      <c r="N8" s="5" t="n"/>
-      <c r="O8" s="5" t="n"/>
-      <c r="P8" s="5" t="n"/>
-      <c r="Q8" s="5" t="n"/>
-      <c r="R8" s="5" t="n"/>
-      <c r="S8" s="5" t="n"/>
-      <c r="T8" s="5" t="n"/>
-      <c r="U8" s="5" t="n"/>
-      <c r="V8" s="5" t="n"/>
-      <c r="W8" s="5" t="n"/>
-      <c r="X8" s="5" t="n"/>
-      <c r="Y8" s="5" t="n"/>
-      <c r="Z8" s="5" t="n"/>
-      <c r="AA8" s="5" t="n"/>
-      <c r="AB8" s="5" t="n"/>
-      <c r="AC8" s="5" t="n"/>
-      <c r="AD8" s="5" t="n"/>
-      <c r="AE8" s="5" t="n"/>
-      <c r="AF8" s="5" t="n"/>
-      <c r="AG8" s="5" t="n"/>
-      <c r="AH8" s="5" t="n"/>
+      <c r="O8" s="15" t="n"/>
+      <c r="P8" s="23" t="n"/>
+      <c r="Q8" s="23" t="n"/>
+      <c r="R8" s="23" t="n"/>
+      <c r="S8" s="23" t="n"/>
+      <c r="T8" s="23" t="n"/>
+      <c r="U8" s="23" t="n"/>
+      <c r="V8" s="23" t="n"/>
+      <c r="W8" s="23" t="n"/>
+      <c r="X8" s="23" t="n"/>
+      <c r="Y8" s="23" t="n"/>
+      <c r="Z8" s="23" t="n"/>
+      <c r="AA8" s="23" t="n"/>
+      <c r="AB8" s="23" t="n"/>
+      <c r="AC8" s="23" t="n"/>
+      <c r="AD8" s="23" t="n"/>
+      <c r="AE8" s="23" t="n"/>
+      <c r="AF8" s="23" t="n"/>
+      <c r="AG8" s="23" t="n"/>
+      <c r="AH8" s="23" t="n"/>
+      <c r="AI8" s="23" t="n"/>
+      <c r="AJ8" s="23" t="n"/>
       <c r="AK8" s="23" t="n"/>
       <c r="AL8" s="23" t="n"/>
       <c r="AM8" s="23" t="n"/>
@@ -1824,54 +1811,60 @@
       <c r="BB8" s="23" t="n"/>
     </row>
     <row r="9" ht="45.5" customHeight="1">
-      <c r="A9" s="5" t="n">
+      <c r="A9" s="14" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="5" t="inlineStr">
+      <c r="B9" s="14" t="inlineStr">
         <is>
-          <t>BATERY00</t>
+          <t>EMBPC00</t>
         </is>
       </c>
-      <c r="C9" s="6" t="inlineStr">
+      <c r="C9" s="15" t="inlineStr">
         <is>
-          <t>Dự án Pack pin cho Robot VMO</t>
+          <t>Dự án máy tính nhúng VMO</t>
         </is>
       </c>
-      <c r="D9" s="9" t="n"/>
-      <c r="E9" s="5" t="inlineStr">
+      <c r="D9" s="14" t="n"/>
+      <c r="E9" s="14" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="F9" s="9" t="n"/>
-      <c r="G9" s="9" t="n"/>
-      <c r="H9" s="9" t="n"/>
-      <c r="I9" s="9" t="n"/>
-      <c r="J9" s="9" t="n"/>
-      <c r="K9" s="5" t="n"/>
-      <c r="L9" s="5" t="n"/>
-      <c r="M9" s="5" t="n"/>
-      <c r="N9" s="5" t="n"/>
-      <c r="O9" s="5" t="n"/>
-      <c r="P9" s="5" t="n"/>
-      <c r="Q9" s="5" t="n"/>
-      <c r="R9" s="5" t="n"/>
-      <c r="S9" s="5" t="n"/>
-      <c r="T9" s="5" t="n"/>
-      <c r="U9" s="5" t="n"/>
-      <c r="V9" s="5" t="n"/>
-      <c r="W9" s="5" t="n"/>
-      <c r="X9" s="5" t="n"/>
-      <c r="Y9" s="5" t="n"/>
-      <c r="Z9" s="5" t="n"/>
-      <c r="AA9" s="5" t="n"/>
-      <c r="AB9" s="5" t="n"/>
-      <c r="AC9" s="5" t="n"/>
-      <c r="AD9" s="5" t="n"/>
-      <c r="AE9" s="5" t="n"/>
-      <c r="AF9" s="5" t="n"/>
-      <c r="AG9" s="5" t="n"/>
-      <c r="AH9" s="5" t="n"/>
+      <c r="F9" s="14" t="n"/>
+      <c r="G9" s="14" t="n"/>
+      <c r="H9" s="14" t="n"/>
+      <c r="I9" s="14" t="n"/>
+      <c r="J9" s="14" t="n"/>
+      <c r="K9" s="14" t="n"/>
+      <c r="L9" s="16" t="n"/>
+      <c r="M9" s="16" t="n"/>
+      <c r="N9" s="14" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="O9" s="15" t="n"/>
+      <c r="P9" s="23" t="n"/>
+      <c r="Q9" s="23" t="n"/>
+      <c r="R9" s="23" t="n"/>
+      <c r="S9" s="23" t="n"/>
+      <c r="T9" s="23" t="n"/>
+      <c r="U9" s="23" t="n"/>
+      <c r="V9" s="23" t="n"/>
+      <c r="W9" s="23" t="n"/>
+      <c r="X9" s="23" t="n"/>
+      <c r="Y9" s="23" t="n"/>
+      <c r="Z9" s="23" t="n"/>
+      <c r="AA9" s="23" t="n"/>
+      <c r="AB9" s="23" t="n"/>
+      <c r="AC9" s="23" t="n"/>
+      <c r="AD9" s="23" t="n"/>
+      <c r="AE9" s="23" t="n"/>
+      <c r="AF9" s="23" t="n"/>
+      <c r="AG9" s="23" t="n"/>
+      <c r="AH9" s="23" t="n"/>
+      <c r="AI9" s="23" t="n"/>
+      <c r="AJ9" s="23" t="n"/>
       <c r="AK9" s="23" t="n"/>
       <c r="AL9" s="23" t="n"/>
       <c r="AM9" s="23" t="n"/>
@@ -1892,40 +1885,68 @@
       <c r="BB9" s="23" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="5" t="n"/>
-      <c r="B10" s="6" t="n"/>
-      <c r="C10" s="6" t="n"/>
-      <c r="D10" s="5" t="n"/>
-      <c r="E10" s="5" t="n"/>
-      <c r="F10" s="5" t="n"/>
-      <c r="G10" s="5" t="n"/>
-      <c r="H10" s="5" t="n"/>
-      <c r="I10" s="5" t="n"/>
-      <c r="J10" s="5" t="n"/>
-      <c r="K10" s="5" t="n"/>
-      <c r="L10" s="5" t="n"/>
-      <c r="M10" s="5" t="n"/>
-      <c r="N10" s="5" t="n"/>
-      <c r="O10" s="5" t="n"/>
-      <c r="P10" s="5" t="n"/>
-      <c r="Q10" s="5" t="n"/>
-      <c r="R10" s="5" t="n"/>
-      <c r="S10" s="5" t="n"/>
-      <c r="T10" s="5" t="n"/>
-      <c r="U10" s="5" t="n"/>
-      <c r="V10" s="5" t="n"/>
-      <c r="W10" s="5" t="n"/>
-      <c r="X10" s="5" t="n"/>
-      <c r="Y10" s="5" t="n"/>
-      <c r="Z10" s="5" t="n"/>
-      <c r="AA10" s="5" t="n"/>
-      <c r="AB10" s="5" t="n"/>
-      <c r="AC10" s="5" t="n"/>
-      <c r="AD10" s="5" t="n"/>
-      <c r="AE10" s="5" t="n"/>
-      <c r="AF10" s="5" t="n"/>
-      <c r="AG10" s="5" t="n"/>
-      <c r="AH10" s="5" t="n"/>
+      <c r="A10" s="14" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" s="14" t="inlineStr">
+        <is>
+          <t>HCR00</t>
+        </is>
+      </c>
+      <c r="C10" s="15" t="inlineStr">
+        <is>
+          <t>Dự án tay cầm điều khiển từ xa VMO</t>
+        </is>
+      </c>
+      <c r="D10" s="14" t="n"/>
+      <c r="E10" s="14" t="n"/>
+      <c r="F10" s="14" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="G10" s="14" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="H10" s="14" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="I10" s="14" t="n"/>
+      <c r="J10" s="14" t="n"/>
+      <c r="K10" s="14" t="n"/>
+      <c r="L10" s="16" t="n"/>
+      <c r="M10" s="16" t="n"/>
+      <c r="N10" s="14" t="inlineStr">
+        <is>
+          <t>Plan</t>
+        </is>
+      </c>
+      <c r="O10" s="15" t="n"/>
+      <c r="P10" s="23" t="n"/>
+      <c r="Q10" s="23" t="n"/>
+      <c r="R10" s="23" t="n"/>
+      <c r="S10" s="23" t="n"/>
+      <c r="T10" s="23" t="n"/>
+      <c r="U10" s="23" t="n"/>
+      <c r="V10" s="23" t="n"/>
+      <c r="W10" s="23" t="n"/>
+      <c r="X10" s="23" t="n"/>
+      <c r="Y10" s="23" t="n"/>
+      <c r="Z10" s="23" t="n"/>
+      <c r="AA10" s="23" t="n"/>
+      <c r="AB10" s="23" t="n"/>
+      <c r="AC10" s="23" t="n"/>
+      <c r="AD10" s="23" t="n"/>
+      <c r="AE10" s="23" t="n"/>
+      <c r="AF10" s="23" t="n"/>
+      <c r="AG10" s="23" t="n"/>
+      <c r="AH10" s="23" t="n"/>
+      <c r="AI10" s="23" t="n"/>
+      <c r="AJ10" s="23" t="n"/>
       <c r="AK10" s="23" t="n"/>
       <c r="AL10" s="23" t="n"/>
       <c r="AM10" s="23" t="n"/>
@@ -1946,40 +1967,60 @@
       <c r="BB10" s="23" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="5" t="n"/>
-      <c r="B11" s="6" t="n"/>
-      <c r="C11" s="6" t="n"/>
-      <c r="D11" s="5" t="n"/>
-      <c r="E11" s="5" t="n"/>
-      <c r="F11" s="5" t="n"/>
-      <c r="G11" s="5" t="n"/>
-      <c r="H11" s="5" t="n"/>
-      <c r="I11" s="5" t="n"/>
-      <c r="J11" s="5" t="n"/>
-      <c r="K11" s="5" t="n"/>
-      <c r="L11" s="5" t="n"/>
-      <c r="M11" s="5" t="n"/>
-      <c r="N11" s="5" t="n"/>
-      <c r="O11" s="5" t="n"/>
-      <c r="P11" s="5" t="n"/>
-      <c r="Q11" s="5" t="n"/>
-      <c r="R11" s="5" t="n"/>
-      <c r="S11" s="5" t="n"/>
-      <c r="T11" s="5" t="n"/>
-      <c r="U11" s="5" t="n"/>
-      <c r="V11" s="5" t="n"/>
-      <c r="W11" s="5" t="n"/>
-      <c r="X11" s="5" t="n"/>
-      <c r="Y11" s="5" t="n"/>
-      <c r="Z11" s="5" t="n"/>
-      <c r="AA11" s="5" t="n"/>
-      <c r="AB11" s="5" t="n"/>
-      <c r="AC11" s="5" t="n"/>
-      <c r="AD11" s="5" t="n"/>
-      <c r="AE11" s="5" t="n"/>
-      <c r="AF11" s="5" t="n"/>
-      <c r="AG11" s="5" t="n"/>
-      <c r="AH11" s="5" t="n"/>
+      <c r="A11" s="14" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" s="14" t="inlineStr">
+        <is>
+          <t>BATERY00</t>
+        </is>
+      </c>
+      <c r="C11" s="15" t="inlineStr">
+        <is>
+          <t>Dự án Pack pin cho Robot VMO</t>
+        </is>
+      </c>
+      <c r="D11" s="14" t="n"/>
+      <c r="E11" s="14" t="n"/>
+      <c r="F11" s="14" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="G11" s="14" t="n"/>
+      <c r="H11" s="14" t="n"/>
+      <c r="I11" s="14" t="n"/>
+      <c r="J11" s="14" t="n"/>
+      <c r="K11" s="14" t="n"/>
+      <c r="L11" s="16" t="n"/>
+      <c r="M11" s="16" t="n"/>
+      <c r="N11" s="14" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="O11" s="15" t="n"/>
+      <c r="P11" s="23" t="n"/>
+      <c r="Q11" s="23" t="n"/>
+      <c r="R11" s="23" t="n"/>
+      <c r="S11" s="23" t="n"/>
+      <c r="T11" s="23" t="n"/>
+      <c r="U11" s="23" t="n"/>
+      <c r="V11" s="23" t="n"/>
+      <c r="W11" s="23" t="n"/>
+      <c r="X11" s="23" t="n"/>
+      <c r="Y11" s="23" t="n"/>
+      <c r="Z11" s="23" t="n"/>
+      <c r="AA11" s="23" t="n"/>
+      <c r="AB11" s="23" t="n"/>
+      <c r="AC11" s="23" t="n"/>
+      <c r="AD11" s="23" t="n"/>
+      <c r="AE11" s="23" t="n"/>
+      <c r="AF11" s="23" t="n"/>
+      <c r="AG11" s="23" t="n"/>
+      <c r="AH11" s="23" t="n"/>
+      <c r="AI11" s="23" t="n"/>
+      <c r="AJ11" s="23" t="n"/>
       <c r="AK11" s="23" t="n"/>
       <c r="AL11" s="23" t="n"/>
       <c r="AM11" s="23" t="n"/>
@@ -2000,40 +2041,42 @@
       <c r="BB11" s="23" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="5" t="n"/>
-      <c r="B12" s="6" t="n"/>
-      <c r="C12" s="6" t="n"/>
-      <c r="D12" s="5" t="n"/>
-      <c r="E12" s="5" t="n"/>
-      <c r="F12" s="5" t="n"/>
-      <c r="G12" s="5" t="n"/>
-      <c r="H12" s="5" t="n"/>
-      <c r="I12" s="5" t="n"/>
-      <c r="J12" s="5" t="n"/>
-      <c r="K12" s="5" t="n"/>
-      <c r="L12" s="5" t="n"/>
-      <c r="M12" s="5" t="n"/>
-      <c r="N12" s="5" t="n"/>
-      <c r="O12" s="5" t="n"/>
-      <c r="P12" s="5" t="n"/>
-      <c r="Q12" s="5" t="n"/>
-      <c r="R12" s="5" t="n"/>
-      <c r="S12" s="5" t="n"/>
-      <c r="T12" s="5" t="n"/>
-      <c r="U12" s="5" t="n"/>
-      <c r="V12" s="5" t="n"/>
-      <c r="W12" s="5" t="n"/>
-      <c r="X12" s="5" t="n"/>
-      <c r="Y12" s="5" t="n"/>
-      <c r="Z12" s="5" t="n"/>
-      <c r="AA12" s="5" t="n"/>
-      <c r="AB12" s="5" t="n"/>
-      <c r="AC12" s="5" t="n"/>
-      <c r="AD12" s="5" t="n"/>
-      <c r="AE12" s="5" t="n"/>
-      <c r="AF12" s="5" t="n"/>
-      <c r="AG12" s="5" t="n"/>
-      <c r="AH12" s="5" t="n"/>
+      <c r="A12" s="52" t="n"/>
+      <c r="B12" s="52" t="n"/>
+      <c r="C12" s="53" t="n"/>
+      <c r="D12" s="52" t="n"/>
+      <c r="E12" s="52" t="n"/>
+      <c r="F12" s="52" t="n"/>
+      <c r="G12" s="52" t="n"/>
+      <c r="H12" s="52" t="n"/>
+      <c r="I12" s="52" t="n"/>
+      <c r="J12" s="52" t="n"/>
+      <c r="K12" s="52" t="n"/>
+      <c r="L12" s="54" t="n"/>
+      <c r="M12" s="54" t="n"/>
+      <c r="N12" s="52" t="n"/>
+      <c r="O12" s="53" t="n"/>
+      <c r="P12" s="23" t="n"/>
+      <c r="Q12" s="23" t="n"/>
+      <c r="R12" s="23" t="n"/>
+      <c r="S12" s="23" t="n"/>
+      <c r="T12" s="23" t="n"/>
+      <c r="U12" s="23" t="n"/>
+      <c r="V12" s="23" t="n"/>
+      <c r="W12" s="23" t="n"/>
+      <c r="X12" s="23" t="n"/>
+      <c r="Y12" s="23" t="n"/>
+      <c r="Z12" s="23" t="n"/>
+      <c r="AA12" s="23" t="n"/>
+      <c r="AB12" s="23" t="n"/>
+      <c r="AC12" s="23" t="n"/>
+      <c r="AD12" s="23" t="n"/>
+      <c r="AE12" s="23" t="n"/>
+      <c r="AF12" s="23" t="n"/>
+      <c r="AG12" s="23" t="n"/>
+      <c r="AH12" s="23" t="n"/>
+      <c r="AI12" s="23" t="n"/>
+      <c r="AJ12" s="23" t="n"/>
       <c r="AK12" s="23" t="n"/>
       <c r="AL12" s="23" t="n"/>
       <c r="AM12" s="23" t="n"/>
@@ -2054,40 +2097,42 @@
       <c r="BB12" s="23" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="5" t="n"/>
-      <c r="B13" s="6" t="n"/>
-      <c r="C13" s="6" t="n"/>
-      <c r="D13" s="5" t="n"/>
-      <c r="E13" s="5" t="n"/>
-      <c r="F13" s="5" t="n"/>
-      <c r="G13" s="5" t="n"/>
-      <c r="H13" s="5" t="n"/>
-      <c r="I13" s="5" t="n"/>
-      <c r="J13" s="5" t="n"/>
-      <c r="K13" s="5" t="n"/>
-      <c r="L13" s="5" t="n"/>
-      <c r="M13" s="5" t="n"/>
-      <c r="N13" s="5" t="n"/>
-      <c r="O13" s="5" t="n"/>
-      <c r="P13" s="5" t="n"/>
-      <c r="Q13" s="5" t="n"/>
-      <c r="R13" s="5" t="n"/>
-      <c r="S13" s="5" t="n"/>
-      <c r="T13" s="5" t="n"/>
-      <c r="U13" s="5" t="n"/>
-      <c r="V13" s="5" t="n"/>
-      <c r="W13" s="5" t="n"/>
-      <c r="X13" s="5" t="n"/>
-      <c r="Y13" s="5" t="n"/>
-      <c r="Z13" s="5" t="n"/>
-      <c r="AA13" s="5" t="n"/>
-      <c r="AB13" s="5" t="n"/>
-      <c r="AC13" s="5" t="n"/>
-      <c r="AD13" s="5" t="n"/>
-      <c r="AE13" s="5" t="n"/>
-      <c r="AF13" s="5" t="n"/>
-      <c r="AG13" s="5" t="n"/>
-      <c r="AH13" s="5" t="n"/>
+      <c r="A13" s="52" t="n"/>
+      <c r="B13" s="52" t="n"/>
+      <c r="C13" s="53" t="n"/>
+      <c r="D13" s="52" t="n"/>
+      <c r="E13" s="52" t="n"/>
+      <c r="F13" s="52" t="n"/>
+      <c r="G13" s="52" t="n"/>
+      <c r="H13" s="52" t="n"/>
+      <c r="I13" s="52" t="n"/>
+      <c r="J13" s="52" t="n"/>
+      <c r="K13" s="52" t="n"/>
+      <c r="L13" s="54" t="n"/>
+      <c r="M13" s="54" t="n"/>
+      <c r="N13" s="52" t="n"/>
+      <c r="O13" s="53" t="n"/>
+      <c r="P13" s="23" t="n"/>
+      <c r="Q13" s="23" t="n"/>
+      <c r="R13" s="23" t="n"/>
+      <c r="S13" s="23" t="n"/>
+      <c r="T13" s="23" t="n"/>
+      <c r="U13" s="23" t="n"/>
+      <c r="V13" s="23" t="n"/>
+      <c r="W13" s="23" t="n"/>
+      <c r="X13" s="23" t="n"/>
+      <c r="Y13" s="23" t="n"/>
+      <c r="Z13" s="23" t="n"/>
+      <c r="AA13" s="23" t="n"/>
+      <c r="AB13" s="23" t="n"/>
+      <c r="AC13" s="23" t="n"/>
+      <c r="AD13" s="23" t="n"/>
+      <c r="AE13" s="23" t="n"/>
+      <c r="AF13" s="23" t="n"/>
+      <c r="AG13" s="23" t="n"/>
+      <c r="AH13" s="23" t="n"/>
+      <c r="AI13" s="23" t="n"/>
+      <c r="AJ13" s="23" t="n"/>
       <c r="AK13" s="23" t="n"/>
       <c r="AL13" s="23" t="n"/>
       <c r="AM13" s="23" t="n"/>
@@ -2108,40 +2153,42 @@
       <c r="BB13" s="23" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="5" t="n"/>
-      <c r="B14" s="6" t="n"/>
-      <c r="C14" s="6" t="n"/>
-      <c r="D14" s="5" t="n"/>
-      <c r="E14" s="5" t="n"/>
-      <c r="F14" s="5" t="n"/>
-      <c r="G14" s="5" t="n"/>
-      <c r="H14" s="5" t="n"/>
-      <c r="I14" s="5" t="n"/>
-      <c r="J14" s="5" t="n"/>
-      <c r="K14" s="5" t="n"/>
-      <c r="L14" s="5" t="n"/>
-      <c r="M14" s="5" t="n"/>
-      <c r="N14" s="5" t="n"/>
-      <c r="O14" s="5" t="n"/>
-      <c r="P14" s="5" t="n"/>
-      <c r="Q14" s="5" t="n"/>
-      <c r="R14" s="5" t="n"/>
-      <c r="S14" s="5" t="n"/>
-      <c r="T14" s="5" t="n"/>
-      <c r="U14" s="5" t="n"/>
-      <c r="V14" s="5" t="n"/>
-      <c r="W14" s="5" t="n"/>
-      <c r="X14" s="5" t="n"/>
-      <c r="Y14" s="5" t="n"/>
-      <c r="Z14" s="5" t="n"/>
-      <c r="AA14" s="5" t="n"/>
-      <c r="AB14" s="5" t="n"/>
-      <c r="AC14" s="5" t="n"/>
-      <c r="AD14" s="5" t="n"/>
-      <c r="AE14" s="5" t="n"/>
-      <c r="AF14" s="5" t="n"/>
-      <c r="AG14" s="5" t="n"/>
-      <c r="AH14" s="5" t="n"/>
+      <c r="A14" s="52" t="n"/>
+      <c r="B14" s="52" t="n"/>
+      <c r="C14" s="53" t="n"/>
+      <c r="D14" s="52" t="n"/>
+      <c r="E14" s="52" t="n"/>
+      <c r="F14" s="52" t="n"/>
+      <c r="G14" s="52" t="n"/>
+      <c r="H14" s="52" t="n"/>
+      <c r="I14" s="52" t="n"/>
+      <c r="J14" s="52" t="n"/>
+      <c r="K14" s="52" t="n"/>
+      <c r="L14" s="54" t="n"/>
+      <c r="M14" s="54" t="n"/>
+      <c r="N14" s="52" t="n"/>
+      <c r="O14" s="53" t="n"/>
+      <c r="P14" s="23" t="n"/>
+      <c r="Q14" s="23" t="n"/>
+      <c r="R14" s="23" t="n"/>
+      <c r="S14" s="23" t="n"/>
+      <c r="T14" s="23" t="n"/>
+      <c r="U14" s="23" t="n"/>
+      <c r="V14" s="23" t="n"/>
+      <c r="W14" s="23" t="n"/>
+      <c r="X14" s="23" t="n"/>
+      <c r="Y14" s="23" t="n"/>
+      <c r="Z14" s="23" t="n"/>
+      <c r="AA14" s="23" t="n"/>
+      <c r="AB14" s="23" t="n"/>
+      <c r="AC14" s="23" t="n"/>
+      <c r="AD14" s="23" t="n"/>
+      <c r="AE14" s="23" t="n"/>
+      <c r="AF14" s="23" t="n"/>
+      <c r="AG14" s="23" t="n"/>
+      <c r="AH14" s="23" t="n"/>
+      <c r="AI14" s="23" t="n"/>
+      <c r="AJ14" s="23" t="n"/>
       <c r="AK14" s="23" t="n"/>
       <c r="AL14" s="23" t="n"/>
       <c r="AM14" s="23" t="n"/>
@@ -2162,40 +2209,42 @@
       <c r="BB14" s="23" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="5" t="n"/>
-      <c r="B15" s="6" t="n"/>
-      <c r="C15" s="6" t="n"/>
-      <c r="D15" s="5" t="n"/>
-      <c r="E15" s="5" t="n"/>
-      <c r="F15" s="5" t="n"/>
-      <c r="G15" s="5" t="n"/>
-      <c r="H15" s="5" t="n"/>
-      <c r="I15" s="5" t="n"/>
-      <c r="J15" s="5" t="n"/>
-      <c r="K15" s="5" t="n"/>
-      <c r="L15" s="5" t="n"/>
-      <c r="M15" s="5" t="n"/>
-      <c r="N15" s="5" t="n"/>
-      <c r="O15" s="5" t="n"/>
-      <c r="P15" s="5" t="n"/>
-      <c r="Q15" s="5" t="n"/>
-      <c r="R15" s="5" t="n"/>
-      <c r="S15" s="5" t="n"/>
-      <c r="T15" s="5" t="n"/>
-      <c r="U15" s="5" t="n"/>
-      <c r="V15" s="5" t="n"/>
-      <c r="W15" s="5" t="n"/>
-      <c r="X15" s="5" t="n"/>
-      <c r="Y15" s="5" t="n"/>
-      <c r="Z15" s="5" t="n"/>
-      <c r="AA15" s="5" t="n"/>
-      <c r="AB15" s="5" t="n"/>
-      <c r="AC15" s="5" t="n"/>
-      <c r="AD15" s="5" t="n"/>
-      <c r="AE15" s="5" t="n"/>
-      <c r="AF15" s="5" t="n"/>
-      <c r="AG15" s="5" t="n"/>
-      <c r="AH15" s="5" t="n"/>
+      <c r="A15" s="52" t="n"/>
+      <c r="B15" s="52" t="n"/>
+      <c r="C15" s="53" t="n"/>
+      <c r="D15" s="52" t="n"/>
+      <c r="E15" s="52" t="n"/>
+      <c r="F15" s="52" t="n"/>
+      <c r="G15" s="52" t="n"/>
+      <c r="H15" s="52" t="n"/>
+      <c r="I15" s="52" t="n"/>
+      <c r="J15" s="52" t="n"/>
+      <c r="K15" s="52" t="n"/>
+      <c r="L15" s="54" t="n"/>
+      <c r="M15" s="54" t="n"/>
+      <c r="N15" s="52" t="n"/>
+      <c r="O15" s="53" t="n"/>
+      <c r="P15" s="23" t="n"/>
+      <c r="Q15" s="23" t="n"/>
+      <c r="R15" s="23" t="n"/>
+      <c r="S15" s="23" t="n"/>
+      <c r="T15" s="23" t="n"/>
+      <c r="U15" s="23" t="n"/>
+      <c r="V15" s="23" t="n"/>
+      <c r="W15" s="23" t="n"/>
+      <c r="X15" s="23" t="n"/>
+      <c r="Y15" s="23" t="n"/>
+      <c r="Z15" s="23" t="n"/>
+      <c r="AA15" s="23" t="n"/>
+      <c r="AB15" s="23" t="n"/>
+      <c r="AC15" s="23" t="n"/>
+      <c r="AD15" s="23" t="n"/>
+      <c r="AE15" s="23" t="n"/>
+      <c r="AF15" s="23" t="n"/>
+      <c r="AG15" s="23" t="n"/>
+      <c r="AH15" s="23" t="n"/>
+      <c r="AI15" s="23" t="n"/>
+      <c r="AJ15" s="23" t="n"/>
       <c r="AK15" s="23" t="n"/>
       <c r="AL15" s="23" t="n"/>
       <c r="AM15" s="23" t="n"/>
@@ -2216,40 +2265,42 @@
       <c r="BB15" s="23" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="5" t="n"/>
-      <c r="B16" s="6" t="n"/>
-      <c r="C16" s="6" t="n"/>
-      <c r="D16" s="5" t="n"/>
-      <c r="E16" s="5" t="n"/>
-      <c r="F16" s="5" t="n"/>
-      <c r="G16" s="5" t="n"/>
-      <c r="H16" s="5" t="n"/>
-      <c r="I16" s="5" t="n"/>
-      <c r="J16" s="5" t="n"/>
-      <c r="K16" s="5" t="n"/>
-      <c r="L16" s="5" t="n"/>
-      <c r="M16" s="5" t="n"/>
-      <c r="N16" s="5" t="n"/>
-      <c r="O16" s="5" t="n"/>
-      <c r="P16" s="5" t="n"/>
-      <c r="Q16" s="5" t="n"/>
-      <c r="R16" s="5" t="n"/>
-      <c r="S16" s="5" t="n"/>
-      <c r="T16" s="5" t="n"/>
-      <c r="U16" s="5" t="n"/>
-      <c r="V16" s="5" t="n"/>
-      <c r="W16" s="5" t="n"/>
-      <c r="X16" s="5" t="n"/>
-      <c r="Y16" s="5" t="n"/>
-      <c r="Z16" s="5" t="n"/>
-      <c r="AA16" s="5" t="n"/>
-      <c r="AB16" s="5" t="n"/>
-      <c r="AC16" s="5" t="n"/>
-      <c r="AD16" s="5" t="n"/>
-      <c r="AE16" s="5" t="n"/>
-      <c r="AF16" s="5" t="n"/>
-      <c r="AG16" s="5" t="n"/>
-      <c r="AH16" s="5" t="n"/>
+      <c r="A16" s="52" t="n"/>
+      <c r="B16" s="52" t="n"/>
+      <c r="C16" s="53" t="n"/>
+      <c r="D16" s="52" t="n"/>
+      <c r="E16" s="52" t="n"/>
+      <c r="F16" s="52" t="n"/>
+      <c r="G16" s="52" t="n"/>
+      <c r="H16" s="52" t="n"/>
+      <c r="I16" s="52" t="n"/>
+      <c r="J16" s="52" t="n"/>
+      <c r="K16" s="52" t="n"/>
+      <c r="L16" s="54" t="n"/>
+      <c r="M16" s="54" t="n"/>
+      <c r="N16" s="52" t="n"/>
+      <c r="O16" s="53" t="n"/>
+      <c r="P16" s="23" t="n"/>
+      <c r="Q16" s="23" t="n"/>
+      <c r="R16" s="23" t="n"/>
+      <c r="S16" s="23" t="n"/>
+      <c r="T16" s="23" t="n"/>
+      <c r="U16" s="23" t="n"/>
+      <c r="V16" s="23" t="n"/>
+      <c r="W16" s="23" t="n"/>
+      <c r="X16" s="23" t="n"/>
+      <c r="Y16" s="23" t="n"/>
+      <c r="Z16" s="23" t="n"/>
+      <c r="AA16" s="23" t="n"/>
+      <c r="AB16" s="23" t="n"/>
+      <c r="AC16" s="23" t="n"/>
+      <c r="AD16" s="23" t="n"/>
+      <c r="AE16" s="23" t="n"/>
+      <c r="AF16" s="23" t="n"/>
+      <c r="AG16" s="23" t="n"/>
+      <c r="AH16" s="23" t="n"/>
+      <c r="AI16" s="23" t="n"/>
+      <c r="AJ16" s="23" t="n"/>
       <c r="AK16" s="23" t="n"/>
       <c r="AL16" s="23" t="n"/>
       <c r="AM16" s="23" t="n"/>
@@ -2270,40 +2321,42 @@
       <c r="BB16" s="23" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="5" t="n"/>
-      <c r="B17" s="6" t="n"/>
-      <c r="C17" s="6" t="n"/>
-      <c r="D17" s="5" t="n"/>
-      <c r="E17" s="5" t="n"/>
-      <c r="F17" s="5" t="n"/>
-      <c r="G17" s="5" t="n"/>
-      <c r="H17" s="5" t="n"/>
-      <c r="I17" s="5" t="n"/>
-      <c r="J17" s="5" t="n"/>
-      <c r="K17" s="5" t="n"/>
-      <c r="L17" s="5" t="n"/>
-      <c r="M17" s="5" t="n"/>
-      <c r="N17" s="5" t="n"/>
-      <c r="O17" s="5" t="n"/>
-      <c r="P17" s="5" t="n"/>
-      <c r="Q17" s="5" t="n"/>
-      <c r="R17" s="5" t="n"/>
-      <c r="S17" s="5" t="n"/>
-      <c r="T17" s="5" t="n"/>
-      <c r="U17" s="5" t="n"/>
-      <c r="V17" s="5" t="n"/>
-      <c r="W17" s="5" t="n"/>
-      <c r="X17" s="5" t="n"/>
-      <c r="Y17" s="5" t="n"/>
-      <c r="Z17" s="5" t="n"/>
-      <c r="AA17" s="5" t="n"/>
-      <c r="AB17" s="5" t="n"/>
-      <c r="AC17" s="5" t="n"/>
-      <c r="AD17" s="5" t="n"/>
-      <c r="AE17" s="5" t="n"/>
-      <c r="AF17" s="5" t="n"/>
-      <c r="AG17" s="5" t="n"/>
-      <c r="AH17" s="5" t="n"/>
+      <c r="A17" s="52" t="n"/>
+      <c r="B17" s="52" t="n"/>
+      <c r="C17" s="53" t="n"/>
+      <c r="D17" s="52" t="n"/>
+      <c r="E17" s="52" t="n"/>
+      <c r="F17" s="52" t="n"/>
+      <c r="G17" s="52" t="n"/>
+      <c r="H17" s="52" t="n"/>
+      <c r="I17" s="52" t="n"/>
+      <c r="J17" s="52" t="n"/>
+      <c r="K17" s="52" t="n"/>
+      <c r="L17" s="54" t="n"/>
+      <c r="M17" s="54" t="n"/>
+      <c r="N17" s="52" t="n"/>
+      <c r="O17" s="53" t="n"/>
+      <c r="P17" s="23" t="n"/>
+      <c r="Q17" s="23" t="n"/>
+      <c r="R17" s="23" t="n"/>
+      <c r="S17" s="23" t="n"/>
+      <c r="T17" s="23" t="n"/>
+      <c r="U17" s="23" t="n"/>
+      <c r="V17" s="23" t="n"/>
+      <c r="W17" s="23" t="n"/>
+      <c r="X17" s="23" t="n"/>
+      <c r="Y17" s="23" t="n"/>
+      <c r="Z17" s="23" t="n"/>
+      <c r="AA17" s="23" t="n"/>
+      <c r="AB17" s="23" t="n"/>
+      <c r="AC17" s="23" t="n"/>
+      <c r="AD17" s="23" t="n"/>
+      <c r="AE17" s="23" t="n"/>
+      <c r="AF17" s="23" t="n"/>
+      <c r="AG17" s="23" t="n"/>
+      <c r="AH17" s="23" t="n"/>
+      <c r="AI17" s="23" t="n"/>
+      <c r="AJ17" s="23" t="n"/>
       <c r="AK17" s="23" t="n"/>
       <c r="AL17" s="23" t="n"/>
       <c r="AM17" s="23" t="n"/>
@@ -2324,40 +2377,42 @@
       <c r="BB17" s="23" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="5" t="n"/>
-      <c r="B18" s="6" t="n"/>
-      <c r="C18" s="6" t="n"/>
-      <c r="D18" s="5" t="n"/>
-      <c r="E18" s="5" t="n"/>
-      <c r="F18" s="5" t="n"/>
-      <c r="G18" s="5" t="n"/>
-      <c r="H18" s="5" t="n"/>
-      <c r="I18" s="5" t="n"/>
-      <c r="J18" s="5" t="n"/>
-      <c r="K18" s="5" t="n"/>
-      <c r="L18" s="5" t="n"/>
-      <c r="M18" s="5" t="n"/>
-      <c r="N18" s="5" t="n"/>
-      <c r="O18" s="5" t="n"/>
-      <c r="P18" s="5" t="n"/>
-      <c r="Q18" s="5" t="n"/>
-      <c r="R18" s="5" t="n"/>
-      <c r="S18" s="5" t="n"/>
-      <c r="T18" s="5" t="n"/>
-      <c r="U18" s="5" t="n"/>
-      <c r="V18" s="5" t="n"/>
-      <c r="W18" s="5" t="n"/>
-      <c r="X18" s="5" t="n"/>
-      <c r="Y18" s="5" t="n"/>
-      <c r="Z18" s="5" t="n"/>
-      <c r="AA18" s="5" t="n"/>
-      <c r="AB18" s="5" t="n"/>
-      <c r="AC18" s="5" t="n"/>
-      <c r="AD18" s="5" t="n"/>
-      <c r="AE18" s="5" t="n"/>
-      <c r="AF18" s="5" t="n"/>
-      <c r="AG18" s="5" t="n"/>
-      <c r="AH18" s="5" t="n"/>
+      <c r="A18" s="52" t="n"/>
+      <c r="B18" s="52" t="n"/>
+      <c r="C18" s="53" t="n"/>
+      <c r="D18" s="52" t="n"/>
+      <c r="E18" s="52" t="n"/>
+      <c r="F18" s="52" t="n"/>
+      <c r="G18" s="52" t="n"/>
+      <c r="H18" s="52" t="n"/>
+      <c r="I18" s="52" t="n"/>
+      <c r="J18" s="52" t="n"/>
+      <c r="K18" s="52" t="n"/>
+      <c r="L18" s="54" t="n"/>
+      <c r="M18" s="54" t="n"/>
+      <c r="N18" s="52" t="n"/>
+      <c r="O18" s="53" t="n"/>
+      <c r="P18" s="23" t="n"/>
+      <c r="Q18" s="23" t="n"/>
+      <c r="R18" s="23" t="n"/>
+      <c r="S18" s="23" t="n"/>
+      <c r="T18" s="23" t="n"/>
+      <c r="U18" s="23" t="n"/>
+      <c r="V18" s="23" t="n"/>
+      <c r="W18" s="23" t="n"/>
+      <c r="X18" s="23" t="n"/>
+      <c r="Y18" s="23" t="n"/>
+      <c r="Z18" s="23" t="n"/>
+      <c r="AA18" s="23" t="n"/>
+      <c r="AB18" s="23" t="n"/>
+      <c r="AC18" s="23" t="n"/>
+      <c r="AD18" s="23" t="n"/>
+      <c r="AE18" s="23" t="n"/>
+      <c r="AF18" s="23" t="n"/>
+      <c r="AG18" s="23" t="n"/>
+      <c r="AH18" s="23" t="n"/>
+      <c r="AI18" s="23" t="n"/>
+      <c r="AJ18" s="23" t="n"/>
       <c r="AK18" s="23" t="n"/>
       <c r="AL18" s="23" t="n"/>
       <c r="AM18" s="23" t="n"/>
@@ -2378,40 +2433,42 @@
       <c r="BB18" s="23" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="5" t="n"/>
-      <c r="B19" s="6" t="n"/>
-      <c r="C19" s="6" t="n"/>
-      <c r="D19" s="5" t="n"/>
-      <c r="E19" s="5" t="n"/>
-      <c r="F19" s="5" t="n"/>
-      <c r="G19" s="5" t="n"/>
-      <c r="H19" s="5" t="n"/>
-      <c r="I19" s="5" t="n"/>
-      <c r="J19" s="5" t="n"/>
-      <c r="K19" s="5" t="n"/>
-      <c r="L19" s="5" t="n"/>
-      <c r="M19" s="5" t="n"/>
-      <c r="N19" s="5" t="n"/>
-      <c r="O19" s="5" t="n"/>
-      <c r="P19" s="5" t="n"/>
-      <c r="Q19" s="5" t="n"/>
-      <c r="R19" s="5" t="n"/>
-      <c r="S19" s="5" t="n"/>
-      <c r="T19" s="5" t="n"/>
-      <c r="U19" s="5" t="n"/>
-      <c r="V19" s="5" t="n"/>
-      <c r="W19" s="5" t="n"/>
-      <c r="X19" s="5" t="n"/>
-      <c r="Y19" s="5" t="n"/>
-      <c r="Z19" s="5" t="n"/>
-      <c r="AA19" s="5" t="n"/>
-      <c r="AB19" s="5" t="n"/>
-      <c r="AC19" s="5" t="n"/>
-      <c r="AD19" s="5" t="n"/>
-      <c r="AE19" s="5" t="n"/>
-      <c r="AF19" s="5" t="n"/>
-      <c r="AG19" s="5" t="n"/>
-      <c r="AH19" s="5" t="n"/>
+      <c r="A19" s="52" t="n"/>
+      <c r="B19" s="52" t="n"/>
+      <c r="C19" s="53" t="n"/>
+      <c r="D19" s="52" t="n"/>
+      <c r="E19" s="52" t="n"/>
+      <c r="F19" s="52" t="n"/>
+      <c r="G19" s="52" t="n"/>
+      <c r="H19" s="52" t="n"/>
+      <c r="I19" s="52" t="n"/>
+      <c r="J19" s="52" t="n"/>
+      <c r="K19" s="52" t="n"/>
+      <c r="L19" s="54" t="n"/>
+      <c r="M19" s="54" t="n"/>
+      <c r="N19" s="52" t="n"/>
+      <c r="O19" s="53" t="n"/>
+      <c r="P19" s="23" t="n"/>
+      <c r="Q19" s="23" t="n"/>
+      <c r="R19" s="23" t="n"/>
+      <c r="S19" s="23" t="n"/>
+      <c r="T19" s="23" t="n"/>
+      <c r="U19" s="23" t="n"/>
+      <c r="V19" s="23" t="n"/>
+      <c r="W19" s="23" t="n"/>
+      <c r="X19" s="23" t="n"/>
+      <c r="Y19" s="23" t="n"/>
+      <c r="Z19" s="23" t="n"/>
+      <c r="AA19" s="23" t="n"/>
+      <c r="AB19" s="23" t="n"/>
+      <c r="AC19" s="23" t="n"/>
+      <c r="AD19" s="23" t="n"/>
+      <c r="AE19" s="23" t="n"/>
+      <c r="AF19" s="23" t="n"/>
+      <c r="AG19" s="23" t="n"/>
+      <c r="AH19" s="23" t="n"/>
+      <c r="AI19" s="23" t="n"/>
+      <c r="AJ19" s="23" t="n"/>
       <c r="AK19" s="23" t="n"/>
       <c r="AL19" s="23" t="n"/>
       <c r="AM19" s="23" t="n"/>
@@ -2432,40 +2489,42 @@
       <c r="BB19" s="23" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" s="5" t="n"/>
-      <c r="B20" s="6" t="n"/>
-      <c r="C20" s="6" t="n"/>
-      <c r="D20" s="5" t="n"/>
-      <c r="E20" s="5" t="n"/>
-      <c r="F20" s="5" t="n"/>
-      <c r="G20" s="5" t="n"/>
-      <c r="H20" s="5" t="n"/>
-      <c r="I20" s="5" t="n"/>
-      <c r="J20" s="5" t="n"/>
-      <c r="K20" s="5" t="n"/>
-      <c r="L20" s="5" t="n"/>
-      <c r="M20" s="5" t="n"/>
-      <c r="N20" s="5" t="n"/>
-      <c r="O20" s="5" t="n"/>
-      <c r="P20" s="5" t="n"/>
-      <c r="Q20" s="5" t="n"/>
-      <c r="R20" s="5" t="n"/>
-      <c r="S20" s="5" t="n"/>
-      <c r="T20" s="5" t="n"/>
-      <c r="U20" s="5" t="n"/>
-      <c r="V20" s="5" t="n"/>
-      <c r="W20" s="5" t="n"/>
-      <c r="X20" s="5" t="n"/>
-      <c r="Y20" s="5" t="n"/>
-      <c r="Z20" s="5" t="n"/>
-      <c r="AA20" s="5" t="n"/>
-      <c r="AB20" s="5" t="n"/>
-      <c r="AC20" s="5" t="n"/>
-      <c r="AD20" s="5" t="n"/>
-      <c r="AE20" s="5" t="n"/>
-      <c r="AF20" s="5" t="n"/>
-      <c r="AG20" s="5" t="n"/>
-      <c r="AH20" s="5" t="n"/>
+      <c r="A20" s="52" t="n"/>
+      <c r="B20" s="52" t="n"/>
+      <c r="C20" s="53" t="n"/>
+      <c r="D20" s="52" t="n"/>
+      <c r="E20" s="52" t="n"/>
+      <c r="F20" s="52" t="n"/>
+      <c r="G20" s="52" t="n"/>
+      <c r="H20" s="52" t="n"/>
+      <c r="I20" s="52" t="n"/>
+      <c r="J20" s="52" t="n"/>
+      <c r="K20" s="52" t="n"/>
+      <c r="L20" s="54" t="n"/>
+      <c r="M20" s="54" t="n"/>
+      <c r="N20" s="52" t="n"/>
+      <c r="O20" s="53" t="n"/>
+      <c r="P20" s="23" t="n"/>
+      <c r="Q20" s="23" t="n"/>
+      <c r="R20" s="23" t="n"/>
+      <c r="S20" s="23" t="n"/>
+      <c r="T20" s="23" t="n"/>
+      <c r="U20" s="23" t="n"/>
+      <c r="V20" s="23" t="n"/>
+      <c r="W20" s="23" t="n"/>
+      <c r="X20" s="23" t="n"/>
+      <c r="Y20" s="23" t="n"/>
+      <c r="Z20" s="23" t="n"/>
+      <c r="AA20" s="23" t="n"/>
+      <c r="AB20" s="23" t="n"/>
+      <c r="AC20" s="23" t="n"/>
+      <c r="AD20" s="23" t="n"/>
+      <c r="AE20" s="23" t="n"/>
+      <c r="AF20" s="23" t="n"/>
+      <c r="AG20" s="23" t="n"/>
+      <c r="AH20" s="23" t="n"/>
+      <c r="AI20" s="23" t="n"/>
+      <c r="AJ20" s="23" t="n"/>
       <c r="AK20" s="23" t="n"/>
       <c r="AL20" s="23" t="n"/>
       <c r="AM20" s="23" t="n"/>
@@ -2486,40 +2545,42 @@
       <c r="BB20" s="23" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="5" t="n"/>
-      <c r="B21" s="6" t="n"/>
-      <c r="C21" s="6" t="n"/>
-      <c r="D21" s="5" t="n"/>
-      <c r="E21" s="5" t="n"/>
-      <c r="F21" s="5" t="n"/>
-      <c r="G21" s="5" t="n"/>
-      <c r="H21" s="5" t="n"/>
-      <c r="I21" s="5" t="n"/>
-      <c r="J21" s="5" t="n"/>
-      <c r="K21" s="5" t="n"/>
-      <c r="L21" s="5" t="n"/>
-      <c r="M21" s="5" t="n"/>
-      <c r="N21" s="5" t="n"/>
-      <c r="O21" s="5" t="n"/>
-      <c r="P21" s="5" t="n"/>
-      <c r="Q21" s="5" t="n"/>
-      <c r="R21" s="5" t="n"/>
-      <c r="S21" s="5" t="n"/>
-      <c r="T21" s="5" t="n"/>
-      <c r="U21" s="5" t="n"/>
-      <c r="V21" s="5" t="n"/>
-      <c r="W21" s="5" t="n"/>
-      <c r="X21" s="5" t="n"/>
-      <c r="Y21" s="5" t="n"/>
-      <c r="Z21" s="5" t="n"/>
-      <c r="AA21" s="5" t="n"/>
-      <c r="AB21" s="5" t="n"/>
-      <c r="AC21" s="5" t="n"/>
-      <c r="AD21" s="5" t="n"/>
-      <c r="AE21" s="5" t="n"/>
-      <c r="AF21" s="5" t="n"/>
-      <c r="AG21" s="5" t="n"/>
-      <c r="AH21" s="5" t="n"/>
+      <c r="A21" s="52" t="n"/>
+      <c r="B21" s="52" t="n"/>
+      <c r="C21" s="53" t="n"/>
+      <c r="D21" s="52" t="n"/>
+      <c r="E21" s="52" t="n"/>
+      <c r="F21" s="52" t="n"/>
+      <c r="G21" s="52" t="n"/>
+      <c r="H21" s="52" t="n"/>
+      <c r="I21" s="52" t="n"/>
+      <c r="J21" s="52" t="n"/>
+      <c r="K21" s="52" t="n"/>
+      <c r="L21" s="54" t="n"/>
+      <c r="M21" s="54" t="n"/>
+      <c r="N21" s="52" t="n"/>
+      <c r="O21" s="53" t="n"/>
+      <c r="P21" s="23" t="n"/>
+      <c r="Q21" s="23" t="n"/>
+      <c r="R21" s="23" t="n"/>
+      <c r="S21" s="23" t="n"/>
+      <c r="T21" s="23" t="n"/>
+      <c r="U21" s="23" t="n"/>
+      <c r="V21" s="23" t="n"/>
+      <c r="W21" s="23" t="n"/>
+      <c r="X21" s="23" t="n"/>
+      <c r="Y21" s="23" t="n"/>
+      <c r="Z21" s="23" t="n"/>
+      <c r="AA21" s="23" t="n"/>
+      <c r="AB21" s="23" t="n"/>
+      <c r="AC21" s="23" t="n"/>
+      <c r="AD21" s="23" t="n"/>
+      <c r="AE21" s="23" t="n"/>
+      <c r="AF21" s="23" t="n"/>
+      <c r="AG21" s="23" t="n"/>
+      <c r="AH21" s="23" t="n"/>
+      <c r="AI21" s="23" t="n"/>
+      <c r="AJ21" s="23" t="n"/>
       <c r="AK21" s="23" t="n"/>
       <c r="AL21" s="23" t="n"/>
       <c r="AM21" s="23" t="n"/>
@@ -2540,40 +2601,42 @@
       <c r="BB21" s="23" t="n"/>
     </row>
     <row r="22">
-      <c r="A22" s="5" t="n"/>
-      <c r="B22" s="6" t="n"/>
-      <c r="C22" s="6" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
-      <c r="I22" s="5" t="n"/>
-      <c r="J22" s="5" t="n"/>
-      <c r="K22" s="5" t="n"/>
-      <c r="L22" s="5" t="n"/>
-      <c r="M22" s="5" t="n"/>
-      <c r="N22" s="5" t="n"/>
-      <c r="O22" s="5" t="n"/>
-      <c r="P22" s="5" t="n"/>
-      <c r="Q22" s="5" t="n"/>
-      <c r="R22" s="5" t="n"/>
-      <c r="S22" s="5" t="n"/>
-      <c r="T22" s="5" t="n"/>
-      <c r="U22" s="5" t="n"/>
-      <c r="V22" s="5" t="n"/>
-      <c r="W22" s="5" t="n"/>
-      <c r="X22" s="5" t="n"/>
-      <c r="Y22" s="5" t="n"/>
-      <c r="Z22" s="5" t="n"/>
-      <c r="AA22" s="5" t="n"/>
-      <c r="AB22" s="5" t="n"/>
-      <c r="AC22" s="5" t="n"/>
-      <c r="AD22" s="5" t="n"/>
-      <c r="AE22" s="5" t="n"/>
-      <c r="AF22" s="5" t="n"/>
-      <c r="AG22" s="5" t="n"/>
-      <c r="AH22" s="5" t="n"/>
+      <c r="A22" s="52" t="n"/>
+      <c r="B22" s="52" t="n"/>
+      <c r="C22" s="53" t="n"/>
+      <c r="D22" s="52" t="n"/>
+      <c r="E22" s="52" t="n"/>
+      <c r="F22" s="52" t="n"/>
+      <c r="G22" s="52" t="n"/>
+      <c r="H22" s="52" t="n"/>
+      <c r="I22" s="52" t="n"/>
+      <c r="J22" s="52" t="n"/>
+      <c r="K22" s="52" t="n"/>
+      <c r="L22" s="54" t="n"/>
+      <c r="M22" s="54" t="n"/>
+      <c r="N22" s="52" t="n"/>
+      <c r="O22" s="53" t="n"/>
+      <c r="P22" s="23" t="n"/>
+      <c r="Q22" s="23" t="n"/>
+      <c r="R22" s="23" t="n"/>
+      <c r="S22" s="23" t="n"/>
+      <c r="T22" s="23" t="n"/>
+      <c r="U22" s="23" t="n"/>
+      <c r="V22" s="23" t="n"/>
+      <c r="W22" s="23" t="n"/>
+      <c r="X22" s="23" t="n"/>
+      <c r="Y22" s="23" t="n"/>
+      <c r="Z22" s="23" t="n"/>
+      <c r="AA22" s="23" t="n"/>
+      <c r="AB22" s="23" t="n"/>
+      <c r="AC22" s="23" t="n"/>
+      <c r="AD22" s="23" t="n"/>
+      <c r="AE22" s="23" t="n"/>
+      <c r="AF22" s="23" t="n"/>
+      <c r="AG22" s="23" t="n"/>
+      <c r="AH22" s="23" t="n"/>
+      <c r="AI22" s="23" t="n"/>
+      <c r="AJ22" s="23" t="n"/>
       <c r="AK22" s="23" t="n"/>
       <c r="AL22" s="23" t="n"/>
       <c r="AM22" s="23" t="n"/>
@@ -2594,40 +2657,42 @@
       <c r="BB22" s="23" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="5" t="n"/>
-      <c r="B23" s="6" t="n"/>
-      <c r="C23" s="6" t="n"/>
-      <c r="D23" s="5" t="n"/>
-      <c r="E23" s="5" t="n"/>
-      <c r="F23" s="5" t="n"/>
-      <c r="G23" s="5" t="n"/>
-      <c r="H23" s="5" t="n"/>
-      <c r="I23" s="5" t="n"/>
-      <c r="J23" s="5" t="n"/>
-      <c r="K23" s="5" t="n"/>
-      <c r="L23" s="5" t="n"/>
-      <c r="M23" s="5" t="n"/>
-      <c r="N23" s="5" t="n"/>
-      <c r="O23" s="5" t="n"/>
-      <c r="P23" s="5" t="n"/>
-      <c r="Q23" s="5" t="n"/>
-      <c r="R23" s="5" t="n"/>
-      <c r="S23" s="5" t="n"/>
-      <c r="T23" s="5" t="n"/>
-      <c r="U23" s="5" t="n"/>
-      <c r="V23" s="5" t="n"/>
-      <c r="W23" s="5" t="n"/>
-      <c r="X23" s="5" t="n"/>
-      <c r="Y23" s="5" t="n"/>
-      <c r="Z23" s="5" t="n"/>
-      <c r="AA23" s="5" t="n"/>
-      <c r="AB23" s="5" t="n"/>
-      <c r="AC23" s="5" t="n"/>
-      <c r="AD23" s="5" t="n"/>
-      <c r="AE23" s="5" t="n"/>
-      <c r="AF23" s="5" t="n"/>
-      <c r="AG23" s="5" t="n"/>
-      <c r="AH23" s="5" t="n"/>
+      <c r="A23" s="52" t="n"/>
+      <c r="B23" s="52" t="n"/>
+      <c r="C23" s="53" t="n"/>
+      <c r="D23" s="52" t="n"/>
+      <c r="E23" s="52" t="n"/>
+      <c r="F23" s="52" t="n"/>
+      <c r="G23" s="52" t="n"/>
+      <c r="H23" s="52" t="n"/>
+      <c r="I23" s="52" t="n"/>
+      <c r="J23" s="52" t="n"/>
+      <c r="K23" s="52" t="n"/>
+      <c r="L23" s="54" t="n"/>
+      <c r="M23" s="54" t="n"/>
+      <c r="N23" s="52" t="n"/>
+      <c r="O23" s="53" t="n"/>
+      <c r="P23" s="23" t="n"/>
+      <c r="Q23" s="23" t="n"/>
+      <c r="R23" s="23" t="n"/>
+      <c r="S23" s="23" t="n"/>
+      <c r="T23" s="23" t="n"/>
+      <c r="U23" s="23" t="n"/>
+      <c r="V23" s="23" t="n"/>
+      <c r="W23" s="23" t="n"/>
+      <c r="X23" s="23" t="n"/>
+      <c r="Y23" s="23" t="n"/>
+      <c r="Z23" s="23" t="n"/>
+      <c r="AA23" s="23" t="n"/>
+      <c r="AB23" s="23" t="n"/>
+      <c r="AC23" s="23" t="n"/>
+      <c r="AD23" s="23" t="n"/>
+      <c r="AE23" s="23" t="n"/>
+      <c r="AF23" s="23" t="n"/>
+      <c r="AG23" s="23" t="n"/>
+      <c r="AH23" s="23" t="n"/>
+      <c r="AI23" s="23" t="n"/>
+      <c r="AJ23" s="23" t="n"/>
       <c r="AK23" s="23" t="n"/>
       <c r="AL23" s="23" t="n"/>
       <c r="AM23" s="23" t="n"/>
@@ -2648,40 +2713,42 @@
       <c r="BB23" s="23" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="5" t="n"/>
-      <c r="B24" s="6" t="n"/>
-      <c r="C24" s="6" t="n"/>
-      <c r="D24" s="5" t="n"/>
-      <c r="E24" s="5" t="n"/>
-      <c r="F24" s="5" t="n"/>
-      <c r="G24" s="5" t="n"/>
-      <c r="H24" s="5" t="n"/>
-      <c r="I24" s="5" t="n"/>
-      <c r="J24" s="5" t="n"/>
-      <c r="K24" s="5" t="n"/>
-      <c r="L24" s="5" t="n"/>
-      <c r="M24" s="5" t="n"/>
-      <c r="N24" s="5" t="n"/>
-      <c r="O24" s="5" t="n"/>
-      <c r="P24" s="5" t="n"/>
-      <c r="Q24" s="5" t="n"/>
-      <c r="R24" s="5" t="n"/>
-      <c r="S24" s="5" t="n"/>
-      <c r="T24" s="5" t="n"/>
-      <c r="U24" s="5" t="n"/>
-      <c r="V24" s="5" t="n"/>
-      <c r="W24" s="5" t="n"/>
-      <c r="X24" s="5" t="n"/>
-      <c r="Y24" s="5" t="n"/>
-      <c r="Z24" s="5" t="n"/>
-      <c r="AA24" s="5" t="n"/>
-      <c r="AB24" s="5" t="n"/>
-      <c r="AC24" s="5" t="n"/>
-      <c r="AD24" s="5" t="n"/>
-      <c r="AE24" s="5" t="n"/>
-      <c r="AF24" s="5" t="n"/>
-      <c r="AG24" s="5" t="n"/>
-      <c r="AH24" s="5" t="n"/>
+      <c r="A24" s="52" t="n"/>
+      <c r="B24" s="52" t="n"/>
+      <c r="C24" s="53" t="n"/>
+      <c r="D24" s="52" t="n"/>
+      <c r="E24" s="52" t="n"/>
+      <c r="F24" s="52" t="n"/>
+      <c r="G24" s="52" t="n"/>
+      <c r="H24" s="52" t="n"/>
+      <c r="I24" s="52" t="n"/>
+      <c r="J24" s="52" t="n"/>
+      <c r="K24" s="52" t="n"/>
+      <c r="L24" s="54" t="n"/>
+      <c r="M24" s="54" t="n"/>
+      <c r="N24" s="52" t="n"/>
+      <c r="O24" s="53" t="n"/>
+      <c r="P24" s="23" t="n"/>
+      <c r="Q24" s="23" t="n"/>
+      <c r="R24" s="23" t="n"/>
+      <c r="S24" s="23" t="n"/>
+      <c r="T24" s="23" t="n"/>
+      <c r="U24" s="23" t="n"/>
+      <c r="V24" s="23" t="n"/>
+      <c r="W24" s="23" t="n"/>
+      <c r="X24" s="23" t="n"/>
+      <c r="Y24" s="23" t="n"/>
+      <c r="Z24" s="23" t="n"/>
+      <c r="AA24" s="23" t="n"/>
+      <c r="AB24" s="23" t="n"/>
+      <c r="AC24" s="23" t="n"/>
+      <c r="AD24" s="23" t="n"/>
+      <c r="AE24" s="23" t="n"/>
+      <c r="AF24" s="23" t="n"/>
+      <c r="AG24" s="23" t="n"/>
+      <c r="AH24" s="23" t="n"/>
+      <c r="AI24" s="23" t="n"/>
+      <c r="AJ24" s="23" t="n"/>
       <c r="AK24" s="23" t="n"/>
       <c r="AL24" s="23" t="n"/>
       <c r="AM24" s="23" t="n"/>
@@ -2702,40 +2769,42 @@
       <c r="BB24" s="23" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="5" t="n"/>
-      <c r="B25" s="6" t="n"/>
-      <c r="C25" s="6" t="n"/>
-      <c r="D25" s="5" t="n"/>
-      <c r="E25" s="5" t="n"/>
-      <c r="F25" s="5" t="n"/>
-      <c r="G25" s="5" t="n"/>
-      <c r="H25" s="5" t="n"/>
-      <c r="I25" s="5" t="n"/>
-      <c r="J25" s="5" t="n"/>
-      <c r="K25" s="5" t="n"/>
-      <c r="L25" s="5" t="n"/>
-      <c r="M25" s="5" t="n"/>
-      <c r="N25" s="5" t="n"/>
-      <c r="O25" s="5" t="n"/>
-      <c r="P25" s="5" t="n"/>
-      <c r="Q25" s="5" t="n"/>
-      <c r="R25" s="5" t="n"/>
-      <c r="S25" s="5" t="n"/>
-      <c r="T25" s="5" t="n"/>
-      <c r="U25" s="5" t="n"/>
-      <c r="V25" s="5" t="n"/>
-      <c r="W25" s="5" t="n"/>
-      <c r="X25" s="5" t="n"/>
-      <c r="Y25" s="5" t="n"/>
-      <c r="Z25" s="5" t="n"/>
-      <c r="AA25" s="5" t="n"/>
-      <c r="AB25" s="5" t="n"/>
-      <c r="AC25" s="5" t="n"/>
-      <c r="AD25" s="5" t="n"/>
-      <c r="AE25" s="5" t="n"/>
-      <c r="AF25" s="5" t="n"/>
-      <c r="AG25" s="5" t="n"/>
-      <c r="AH25" s="5" t="n"/>
+      <c r="A25" s="52" t="n"/>
+      <c r="B25" s="52" t="n"/>
+      <c r="C25" s="53" t="n"/>
+      <c r="D25" s="52" t="n"/>
+      <c r="E25" s="52" t="n"/>
+      <c r="F25" s="52" t="n"/>
+      <c r="G25" s="52" t="n"/>
+      <c r="H25" s="52" t="n"/>
+      <c r="I25" s="52" t="n"/>
+      <c r="J25" s="52" t="n"/>
+      <c r="K25" s="52" t="n"/>
+      <c r="L25" s="54" t="n"/>
+      <c r="M25" s="54" t="n"/>
+      <c r="N25" s="52" t="n"/>
+      <c r="O25" s="53" t="n"/>
+      <c r="P25" s="23" t="n"/>
+      <c r="Q25" s="23" t="n"/>
+      <c r="R25" s="23" t="n"/>
+      <c r="S25" s="23" t="n"/>
+      <c r="T25" s="23" t="n"/>
+      <c r="U25" s="23" t="n"/>
+      <c r="V25" s="23" t="n"/>
+      <c r="W25" s="23" t="n"/>
+      <c r="X25" s="23" t="n"/>
+      <c r="Y25" s="23" t="n"/>
+      <c r="Z25" s="23" t="n"/>
+      <c r="AA25" s="23" t="n"/>
+      <c r="AB25" s="23" t="n"/>
+      <c r="AC25" s="23" t="n"/>
+      <c r="AD25" s="23" t="n"/>
+      <c r="AE25" s="23" t="n"/>
+      <c r="AF25" s="23" t="n"/>
+      <c r="AG25" s="23" t="n"/>
+      <c r="AH25" s="23" t="n"/>
+      <c r="AI25" s="23" t="n"/>
+      <c r="AJ25" s="23" t="n"/>
       <c r="AK25" s="23" t="n"/>
       <c r="AL25" s="23" t="n"/>
       <c r="AM25" s="23" t="n"/>
@@ -2756,40 +2825,42 @@
       <c r="BB25" s="23" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="5" t="n"/>
-      <c r="B26" s="6" t="n"/>
-      <c r="C26" s="6" t="n"/>
-      <c r="D26" s="5" t="n"/>
-      <c r="E26" s="5" t="n"/>
-      <c r="F26" s="5" t="n"/>
-      <c r="G26" s="5" t="n"/>
-      <c r="H26" s="5" t="n"/>
-      <c r="I26" s="5" t="n"/>
-      <c r="J26" s="5" t="n"/>
-      <c r="K26" s="5" t="n"/>
-      <c r="L26" s="5" t="n"/>
-      <c r="M26" s="5" t="n"/>
-      <c r="N26" s="5" t="n"/>
-      <c r="O26" s="5" t="n"/>
-      <c r="P26" s="5" t="n"/>
-      <c r="Q26" s="5" t="n"/>
-      <c r="R26" s="5" t="n"/>
-      <c r="S26" s="5" t="n"/>
-      <c r="T26" s="5" t="n"/>
-      <c r="U26" s="5" t="n"/>
-      <c r="V26" s="5" t="n"/>
-      <c r="W26" s="5" t="n"/>
-      <c r="X26" s="5" t="n"/>
-      <c r="Y26" s="5" t="n"/>
-      <c r="Z26" s="5" t="n"/>
-      <c r="AA26" s="5" t="n"/>
-      <c r="AB26" s="5" t="n"/>
-      <c r="AC26" s="5" t="n"/>
-      <c r="AD26" s="5" t="n"/>
-      <c r="AE26" s="5" t="n"/>
-      <c r="AF26" s="5" t="n"/>
-      <c r="AG26" s="5" t="n"/>
-      <c r="AH26" s="5" t="n"/>
+      <c r="A26" s="52" t="n"/>
+      <c r="B26" s="52" t="n"/>
+      <c r="C26" s="53" t="n"/>
+      <c r="D26" s="52" t="n"/>
+      <c r="E26" s="52" t="n"/>
+      <c r="F26" s="52" t="n"/>
+      <c r="G26" s="52" t="n"/>
+      <c r="H26" s="52" t="n"/>
+      <c r="I26" s="52" t="n"/>
+      <c r="J26" s="52" t="n"/>
+      <c r="K26" s="52" t="n"/>
+      <c r="L26" s="54" t="n"/>
+      <c r="M26" s="54" t="n"/>
+      <c r="N26" s="52" t="n"/>
+      <c r="O26" s="53" t="n"/>
+      <c r="P26" s="23" t="n"/>
+      <c r="Q26" s="23" t="n"/>
+      <c r="R26" s="23" t="n"/>
+      <c r="S26" s="23" t="n"/>
+      <c r="T26" s="23" t="n"/>
+      <c r="U26" s="23" t="n"/>
+      <c r="V26" s="23" t="n"/>
+      <c r="W26" s="23" t="n"/>
+      <c r="X26" s="23" t="n"/>
+      <c r="Y26" s="23" t="n"/>
+      <c r="Z26" s="23" t="n"/>
+      <c r="AA26" s="23" t="n"/>
+      <c r="AB26" s="23" t="n"/>
+      <c r="AC26" s="23" t="n"/>
+      <c r="AD26" s="23" t="n"/>
+      <c r="AE26" s="23" t="n"/>
+      <c r="AF26" s="23" t="n"/>
+      <c r="AG26" s="23" t="n"/>
+      <c r="AH26" s="23" t="n"/>
+      <c r="AI26" s="23" t="n"/>
+      <c r="AJ26" s="23" t="n"/>
       <c r="AK26" s="23" t="n"/>
       <c r="AL26" s="23" t="n"/>
       <c r="AM26" s="23" t="n"/>
@@ -2810,40 +2881,42 @@
       <c r="BB26" s="23" t="n"/>
     </row>
     <row r="27">
-      <c r="A27" s="5" t="n"/>
-      <c r="B27" s="6" t="n"/>
-      <c r="C27" s="6" t="n"/>
-      <c r="D27" s="5" t="n"/>
-      <c r="E27" s="5" t="n"/>
-      <c r="F27" s="5" t="n"/>
-      <c r="G27" s="5" t="n"/>
-      <c r="H27" s="5" t="n"/>
-      <c r="I27" s="5" t="n"/>
-      <c r="J27" s="5" t="n"/>
-      <c r="K27" s="5" t="n"/>
-      <c r="L27" s="5" t="n"/>
-      <c r="M27" s="5" t="n"/>
-      <c r="N27" s="5" t="n"/>
-      <c r="O27" s="5" t="n"/>
-      <c r="P27" s="5" t="n"/>
-      <c r="Q27" s="5" t="n"/>
-      <c r="R27" s="5" t="n"/>
-      <c r="S27" s="5" t="n"/>
-      <c r="T27" s="5" t="n"/>
-      <c r="U27" s="5" t="n"/>
-      <c r="V27" s="5" t="n"/>
-      <c r="W27" s="5" t="n"/>
-      <c r="X27" s="5" t="n"/>
-      <c r="Y27" s="5" t="n"/>
-      <c r="Z27" s="5" t="n"/>
-      <c r="AA27" s="5" t="n"/>
-      <c r="AB27" s="5" t="n"/>
-      <c r="AC27" s="5" t="n"/>
-      <c r="AD27" s="5" t="n"/>
-      <c r="AE27" s="5" t="n"/>
-      <c r="AF27" s="5" t="n"/>
-      <c r="AG27" s="5" t="n"/>
-      <c r="AH27" s="5" t="n"/>
+      <c r="A27" s="52" t="n"/>
+      <c r="B27" s="52" t="n"/>
+      <c r="C27" s="53" t="n"/>
+      <c r="D27" s="52" t="n"/>
+      <c r="E27" s="52" t="n"/>
+      <c r="F27" s="52" t="n"/>
+      <c r="G27" s="52" t="n"/>
+      <c r="H27" s="52" t="n"/>
+      <c r="I27" s="52" t="n"/>
+      <c r="J27" s="52" t="n"/>
+      <c r="K27" s="52" t="n"/>
+      <c r="L27" s="54" t="n"/>
+      <c r="M27" s="54" t="n"/>
+      <c r="N27" s="52" t="n"/>
+      <c r="O27" s="53" t="n"/>
+      <c r="P27" s="23" t="n"/>
+      <c r="Q27" s="23" t="n"/>
+      <c r="R27" s="23" t="n"/>
+      <c r="S27" s="23" t="n"/>
+      <c r="T27" s="23" t="n"/>
+      <c r="U27" s="23" t="n"/>
+      <c r="V27" s="23" t="n"/>
+      <c r="W27" s="23" t="n"/>
+      <c r="X27" s="23" t="n"/>
+      <c r="Y27" s="23" t="n"/>
+      <c r="Z27" s="23" t="n"/>
+      <c r="AA27" s="23" t="n"/>
+      <c r="AB27" s="23" t="n"/>
+      <c r="AC27" s="23" t="n"/>
+      <c r="AD27" s="23" t="n"/>
+      <c r="AE27" s="23" t="n"/>
+      <c r="AF27" s="23" t="n"/>
+      <c r="AG27" s="23" t="n"/>
+      <c r="AH27" s="23" t="n"/>
+      <c r="AI27" s="23" t="n"/>
+      <c r="AJ27" s="23" t="n"/>
       <c r="AK27" s="23" t="n"/>
       <c r="AL27" s="23" t="n"/>
       <c r="AM27" s="23" t="n"/>
@@ -2864,40 +2937,42 @@
       <c r="BB27" s="23" t="n"/>
     </row>
     <row r="28">
-      <c r="A28" s="5" t="n"/>
-      <c r="B28" s="6" t="n"/>
-      <c r="C28" s="6" t="n"/>
-      <c r="D28" s="5" t="n"/>
-      <c r="E28" s="5" t="n"/>
-      <c r="F28" s="5" t="n"/>
-      <c r="G28" s="5" t="n"/>
-      <c r="H28" s="5" t="n"/>
-      <c r="I28" s="5" t="n"/>
-      <c r="J28" s="5" t="n"/>
-      <c r="K28" s="5" t="n"/>
-      <c r="L28" s="5" t="n"/>
-      <c r="M28" s="5" t="n"/>
-      <c r="N28" s="5" t="n"/>
-      <c r="O28" s="5" t="n"/>
-      <c r="P28" s="5" t="n"/>
-      <c r="Q28" s="5" t="n"/>
-      <c r="R28" s="5" t="n"/>
-      <c r="S28" s="5" t="n"/>
-      <c r="T28" s="5" t="n"/>
-      <c r="U28" s="5" t="n"/>
-      <c r="V28" s="5" t="n"/>
-      <c r="W28" s="5" t="n"/>
-      <c r="X28" s="5" t="n"/>
-      <c r="Y28" s="5" t="n"/>
-      <c r="Z28" s="5" t="n"/>
-      <c r="AA28" s="5" t="n"/>
-      <c r="AB28" s="5" t="n"/>
-      <c r="AC28" s="5" t="n"/>
-      <c r="AD28" s="5" t="n"/>
-      <c r="AE28" s="5" t="n"/>
-      <c r="AF28" s="5" t="n"/>
-      <c r="AG28" s="5" t="n"/>
-      <c r="AH28" s="5" t="n"/>
+      <c r="A28" s="52" t="n"/>
+      <c r="B28" s="52" t="n"/>
+      <c r="C28" s="53" t="n"/>
+      <c r="D28" s="52" t="n"/>
+      <c r="E28" s="52" t="n"/>
+      <c r="F28" s="52" t="n"/>
+      <c r="G28" s="52" t="n"/>
+      <c r="H28" s="52" t="n"/>
+      <c r="I28" s="52" t="n"/>
+      <c r="J28" s="52" t="n"/>
+      <c r="K28" s="52" t="n"/>
+      <c r="L28" s="54" t="n"/>
+      <c r="M28" s="54" t="n"/>
+      <c r="N28" s="52" t="n"/>
+      <c r="O28" s="53" t="n"/>
+      <c r="P28" s="23" t="n"/>
+      <c r="Q28" s="23" t="n"/>
+      <c r="R28" s="23" t="n"/>
+      <c r="S28" s="23" t="n"/>
+      <c r="T28" s="23" t="n"/>
+      <c r="U28" s="23" t="n"/>
+      <c r="V28" s="23" t="n"/>
+      <c r="W28" s="23" t="n"/>
+      <c r="X28" s="23" t="n"/>
+      <c r="Y28" s="23" t="n"/>
+      <c r="Z28" s="23" t="n"/>
+      <c r="AA28" s="23" t="n"/>
+      <c r="AB28" s="23" t="n"/>
+      <c r="AC28" s="23" t="n"/>
+      <c r="AD28" s="23" t="n"/>
+      <c r="AE28" s="23" t="n"/>
+      <c r="AF28" s="23" t="n"/>
+      <c r="AG28" s="23" t="n"/>
+      <c r="AH28" s="23" t="n"/>
+      <c r="AI28" s="23" t="n"/>
+      <c r="AJ28" s="23" t="n"/>
       <c r="AK28" s="23" t="n"/>
       <c r="AL28" s="23" t="n"/>
       <c r="AM28" s="23" t="n"/>
@@ -2918,40 +2993,42 @@
       <c r="BB28" s="23" t="n"/>
     </row>
     <row r="29">
-      <c r="A29" s="5" t="n"/>
-      <c r="B29" s="6" t="n"/>
-      <c r="C29" s="6" t="n"/>
-      <c r="D29" s="5" t="n"/>
-      <c r="E29" s="5" t="n"/>
-      <c r="F29" s="5" t="n"/>
-      <c r="G29" s="5" t="n"/>
-      <c r="H29" s="5" t="n"/>
-      <c r="I29" s="5" t="n"/>
-      <c r="J29" s="5" t="n"/>
-      <c r="K29" s="5" t="n"/>
-      <c r="L29" s="5" t="n"/>
-      <c r="M29" s="5" t="n"/>
-      <c r="N29" s="5" t="n"/>
-      <c r="O29" s="5" t="n"/>
-      <c r="P29" s="5" t="n"/>
-      <c r="Q29" s="5" t="n"/>
-      <c r="R29" s="5" t="n"/>
-      <c r="S29" s="5" t="n"/>
-      <c r="T29" s="5" t="n"/>
-      <c r="U29" s="5" t="n"/>
-      <c r="V29" s="5" t="n"/>
-      <c r="W29" s="5" t="n"/>
-      <c r="X29" s="5" t="n"/>
-      <c r="Y29" s="5" t="n"/>
-      <c r="Z29" s="5" t="n"/>
-      <c r="AA29" s="5" t="n"/>
-      <c r="AB29" s="5" t="n"/>
-      <c r="AC29" s="5" t="n"/>
-      <c r="AD29" s="5" t="n"/>
-      <c r="AE29" s="5" t="n"/>
-      <c r="AF29" s="5" t="n"/>
-      <c r="AG29" s="5" t="n"/>
-      <c r="AH29" s="5" t="n"/>
+      <c r="A29" s="52" t="n"/>
+      <c r="B29" s="52" t="n"/>
+      <c r="C29" s="53" t="n"/>
+      <c r="D29" s="52" t="n"/>
+      <c r="E29" s="52" t="n"/>
+      <c r="F29" s="52" t="n"/>
+      <c r="G29" s="52" t="n"/>
+      <c r="H29" s="52" t="n"/>
+      <c r="I29" s="52" t="n"/>
+      <c r="J29" s="52" t="n"/>
+      <c r="K29" s="52" t="n"/>
+      <c r="L29" s="54" t="n"/>
+      <c r="M29" s="54" t="n"/>
+      <c r="N29" s="52" t="n"/>
+      <c r="O29" s="53" t="n"/>
+      <c r="P29" s="23" t="n"/>
+      <c r="Q29" s="23" t="n"/>
+      <c r="R29" s="23" t="n"/>
+      <c r="S29" s="23" t="n"/>
+      <c r="T29" s="23" t="n"/>
+      <c r="U29" s="23" t="n"/>
+      <c r="V29" s="23" t="n"/>
+      <c r="W29" s="23" t="n"/>
+      <c r="X29" s="23" t="n"/>
+      <c r="Y29" s="23" t="n"/>
+      <c r="Z29" s="23" t="n"/>
+      <c r="AA29" s="23" t="n"/>
+      <c r="AB29" s="23" t="n"/>
+      <c r="AC29" s="23" t="n"/>
+      <c r="AD29" s="23" t="n"/>
+      <c r="AE29" s="23" t="n"/>
+      <c r="AF29" s="23" t="n"/>
+      <c r="AG29" s="23" t="n"/>
+      <c r="AH29" s="23" t="n"/>
+      <c r="AI29" s="23" t="n"/>
+      <c r="AJ29" s="23" t="n"/>
       <c r="AK29" s="23" t="n"/>
       <c r="AL29" s="23" t="n"/>
       <c r="AM29" s="23" t="n"/>
@@ -2972,40 +3049,42 @@
       <c r="BB29" s="23" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" s="5" t="n"/>
-      <c r="B30" s="6" t="n"/>
-      <c r="C30" s="6" t="n"/>
-      <c r="D30" s="5" t="n"/>
-      <c r="E30" s="5" t="n"/>
-      <c r="F30" s="5" t="n"/>
-      <c r="G30" s="5" t="n"/>
-      <c r="H30" s="5" t="n"/>
-      <c r="I30" s="5" t="n"/>
-      <c r="J30" s="5" t="n"/>
-      <c r="K30" s="5" t="n"/>
-      <c r="L30" s="5" t="n"/>
-      <c r="M30" s="5" t="n"/>
-      <c r="N30" s="5" t="n"/>
-      <c r="O30" s="5" t="n"/>
-      <c r="P30" s="5" t="n"/>
-      <c r="Q30" s="5" t="n"/>
-      <c r="R30" s="5" t="n"/>
-      <c r="S30" s="5" t="n"/>
-      <c r="T30" s="5" t="n"/>
-      <c r="U30" s="5" t="n"/>
-      <c r="V30" s="5" t="n"/>
-      <c r="W30" s="5" t="n"/>
-      <c r="X30" s="5" t="n"/>
-      <c r="Y30" s="5" t="n"/>
-      <c r="Z30" s="5" t="n"/>
-      <c r="AA30" s="5" t="n"/>
-      <c r="AB30" s="5" t="n"/>
-      <c r="AC30" s="5" t="n"/>
-      <c r="AD30" s="5" t="n"/>
-      <c r="AE30" s="5" t="n"/>
-      <c r="AF30" s="5" t="n"/>
-      <c r="AG30" s="5" t="n"/>
-      <c r="AH30" s="5" t="n"/>
+      <c r="A30" s="52" t="n"/>
+      <c r="B30" s="52" t="n"/>
+      <c r="C30" s="53" t="n"/>
+      <c r="D30" s="52" t="n"/>
+      <c r="E30" s="52" t="n"/>
+      <c r="F30" s="52" t="n"/>
+      <c r="G30" s="52" t="n"/>
+      <c r="H30" s="52" t="n"/>
+      <c r="I30" s="52" t="n"/>
+      <c r="J30" s="52" t="n"/>
+      <c r="K30" s="52" t="n"/>
+      <c r="L30" s="54" t="n"/>
+      <c r="M30" s="54" t="n"/>
+      <c r="N30" s="52" t="n"/>
+      <c r="O30" s="53" t="n"/>
+      <c r="P30" s="23" t="n"/>
+      <c r="Q30" s="23" t="n"/>
+      <c r="R30" s="23" t="n"/>
+      <c r="S30" s="23" t="n"/>
+      <c r="T30" s="23" t="n"/>
+      <c r="U30" s="23" t="n"/>
+      <c r="V30" s="23" t="n"/>
+      <c r="W30" s="23" t="n"/>
+      <c r="X30" s="23" t="n"/>
+      <c r="Y30" s="23" t="n"/>
+      <c r="Z30" s="23" t="n"/>
+      <c r="AA30" s="23" t="n"/>
+      <c r="AB30" s="23" t="n"/>
+      <c r="AC30" s="23" t="n"/>
+      <c r="AD30" s="23" t="n"/>
+      <c r="AE30" s="23" t="n"/>
+      <c r="AF30" s="23" t="n"/>
+      <c r="AG30" s="23" t="n"/>
+      <c r="AH30" s="23" t="n"/>
+      <c r="AI30" s="23" t="n"/>
+      <c r="AJ30" s="23" t="n"/>
       <c r="AK30" s="23" t="n"/>
       <c r="AL30" s="23" t="n"/>
       <c r="AM30" s="23" t="n"/>
@@ -3026,40 +3105,42 @@
       <c r="BB30" s="23" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" s="5" t="n"/>
-      <c r="B31" s="6" t="n"/>
-      <c r="C31" s="6" t="n"/>
-      <c r="D31" s="5" t="n"/>
-      <c r="E31" s="5" t="n"/>
-      <c r="F31" s="5" t="n"/>
-      <c r="G31" s="5" t="n"/>
-      <c r="H31" s="5" t="n"/>
-      <c r="I31" s="5" t="n"/>
-      <c r="J31" s="5" t="n"/>
-      <c r="K31" s="5" t="n"/>
-      <c r="L31" s="5" t="n"/>
-      <c r="M31" s="5" t="n"/>
-      <c r="N31" s="5" t="n"/>
-      <c r="O31" s="5" t="n"/>
-      <c r="P31" s="5" t="n"/>
-      <c r="Q31" s="5" t="n"/>
-      <c r="R31" s="5" t="n"/>
-      <c r="S31" s="5" t="n"/>
-      <c r="T31" s="5" t="n"/>
-      <c r="U31" s="5" t="n"/>
-      <c r="V31" s="5" t="n"/>
-      <c r="W31" s="5" t="n"/>
-      <c r="X31" s="5" t="n"/>
-      <c r="Y31" s="5" t="n"/>
-      <c r="Z31" s="5" t="n"/>
-      <c r="AA31" s="5" t="n"/>
-      <c r="AB31" s="5" t="n"/>
-      <c r="AC31" s="5" t="n"/>
-      <c r="AD31" s="5" t="n"/>
-      <c r="AE31" s="5" t="n"/>
-      <c r="AF31" s="5" t="n"/>
-      <c r="AG31" s="5" t="n"/>
-      <c r="AH31" s="5" t="n"/>
+      <c r="A31" s="52" t="n"/>
+      <c r="B31" s="52" t="n"/>
+      <c r="C31" s="53" t="n"/>
+      <c r="D31" s="52" t="n"/>
+      <c r="E31" s="52" t="n"/>
+      <c r="F31" s="52" t="n"/>
+      <c r="G31" s="52" t="n"/>
+      <c r="H31" s="52" t="n"/>
+      <c r="I31" s="52" t="n"/>
+      <c r="J31" s="52" t="n"/>
+      <c r="K31" s="52" t="n"/>
+      <c r="L31" s="54" t="n"/>
+      <c r="M31" s="54" t="n"/>
+      <c r="N31" s="52" t="n"/>
+      <c r="O31" s="53" t="n"/>
+      <c r="P31" s="23" t="n"/>
+      <c r="Q31" s="23" t="n"/>
+      <c r="R31" s="23" t="n"/>
+      <c r="S31" s="23" t="n"/>
+      <c r="T31" s="23" t="n"/>
+      <c r="U31" s="23" t="n"/>
+      <c r="V31" s="23" t="n"/>
+      <c r="W31" s="23" t="n"/>
+      <c r="X31" s="23" t="n"/>
+      <c r="Y31" s="23" t="n"/>
+      <c r="Z31" s="23" t="n"/>
+      <c r="AA31" s="23" t="n"/>
+      <c r="AB31" s="23" t="n"/>
+      <c r="AC31" s="23" t="n"/>
+      <c r="AD31" s="23" t="n"/>
+      <c r="AE31" s="23" t="n"/>
+      <c r="AF31" s="23" t="n"/>
+      <c r="AG31" s="23" t="n"/>
+      <c r="AH31" s="23" t="n"/>
+      <c r="AI31" s="23" t="n"/>
+      <c r="AJ31" s="23" t="n"/>
       <c r="AK31" s="23" t="n"/>
       <c r="AL31" s="23" t="n"/>
       <c r="AM31" s="23" t="n"/>
@@ -3080,40 +3161,42 @@
       <c r="BB31" s="23" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="5" t="n"/>
-      <c r="B32" s="6" t="n"/>
-      <c r="C32" s="6" t="n"/>
-      <c r="D32" s="5" t="n"/>
-      <c r="E32" s="5" t="n"/>
-      <c r="F32" s="5" t="n"/>
-      <c r="G32" s="5" t="n"/>
-      <c r="H32" s="5" t="n"/>
-      <c r="I32" s="5" t="n"/>
-      <c r="J32" s="5" t="n"/>
-      <c r="K32" s="5" t="n"/>
-      <c r="L32" s="5" t="n"/>
-      <c r="M32" s="5" t="n"/>
-      <c r="N32" s="5" t="n"/>
-      <c r="O32" s="5" t="n"/>
-      <c r="P32" s="5" t="n"/>
-      <c r="Q32" s="5" t="n"/>
-      <c r="R32" s="5" t="n"/>
-      <c r="S32" s="5" t="n"/>
-      <c r="T32" s="5" t="n"/>
-      <c r="U32" s="5" t="n"/>
-      <c r="V32" s="5" t="n"/>
-      <c r="W32" s="5" t="n"/>
-      <c r="X32" s="5" t="n"/>
-      <c r="Y32" s="5" t="n"/>
-      <c r="Z32" s="5" t="n"/>
-      <c r="AA32" s="5" t="n"/>
-      <c r="AB32" s="5" t="n"/>
-      <c r="AC32" s="5" t="n"/>
-      <c r="AD32" s="5" t="n"/>
-      <c r="AE32" s="5" t="n"/>
-      <c r="AF32" s="5" t="n"/>
-      <c r="AG32" s="5" t="n"/>
-      <c r="AH32" s="5" t="n"/>
+      <c r="A32" s="52" t="n"/>
+      <c r="B32" s="52" t="n"/>
+      <c r="C32" s="53" t="n"/>
+      <c r="D32" s="52" t="n"/>
+      <c r="E32" s="52" t="n"/>
+      <c r="F32" s="52" t="n"/>
+      <c r="G32" s="52" t="n"/>
+      <c r="H32" s="52" t="n"/>
+      <c r="I32" s="52" t="n"/>
+      <c r="J32" s="52" t="n"/>
+      <c r="K32" s="52" t="n"/>
+      <c r="L32" s="54" t="n"/>
+      <c r="M32" s="54" t="n"/>
+      <c r="N32" s="52" t="n"/>
+      <c r="O32" s="53" t="n"/>
+      <c r="P32" s="23" t="n"/>
+      <c r="Q32" s="23" t="n"/>
+      <c r="R32" s="23" t="n"/>
+      <c r="S32" s="23" t="n"/>
+      <c r="T32" s="23" t="n"/>
+      <c r="U32" s="23" t="n"/>
+      <c r="V32" s="23" t="n"/>
+      <c r="W32" s="23" t="n"/>
+      <c r="X32" s="23" t="n"/>
+      <c r="Y32" s="23" t="n"/>
+      <c r="Z32" s="23" t="n"/>
+      <c r="AA32" s="23" t="n"/>
+      <c r="AB32" s="23" t="n"/>
+      <c r="AC32" s="23" t="n"/>
+      <c r="AD32" s="23" t="n"/>
+      <c r="AE32" s="23" t="n"/>
+      <c r="AF32" s="23" t="n"/>
+      <c r="AG32" s="23" t="n"/>
+      <c r="AH32" s="23" t="n"/>
+      <c r="AI32" s="23" t="n"/>
+      <c r="AJ32" s="23" t="n"/>
       <c r="AK32" s="23" t="n"/>
       <c r="AL32" s="23" t="n"/>
       <c r="AM32" s="23" t="n"/>
@@ -3134,40 +3217,42 @@
       <c r="BB32" s="23" t="n"/>
     </row>
     <row r="33">
-      <c r="A33" s="5" t="n"/>
-      <c r="B33" s="6" t="n"/>
-      <c r="C33" s="6" t="n"/>
-      <c r="D33" s="5" t="n"/>
-      <c r="E33" s="5" t="n"/>
-      <c r="F33" s="5" t="n"/>
-      <c r="G33" s="5" t="n"/>
-      <c r="H33" s="5" t="n"/>
-      <c r="I33" s="5" t="n"/>
-      <c r="J33" s="5" t="n"/>
-      <c r="K33" s="5" t="n"/>
-      <c r="L33" s="5" t="n"/>
-      <c r="M33" s="5" t="n"/>
-      <c r="N33" s="5" t="n"/>
-      <c r="O33" s="5" t="n"/>
-      <c r="P33" s="5" t="n"/>
-      <c r="Q33" s="5" t="n"/>
-      <c r="R33" s="5" t="n"/>
-      <c r="S33" s="5" t="n"/>
-      <c r="T33" s="5" t="n"/>
-      <c r="U33" s="5" t="n"/>
-      <c r="V33" s="5" t="n"/>
-      <c r="W33" s="5" t="n"/>
-      <c r="X33" s="5" t="n"/>
-      <c r="Y33" s="5" t="n"/>
-      <c r="Z33" s="5" t="n"/>
-      <c r="AA33" s="5" t="n"/>
-      <c r="AB33" s="5" t="n"/>
-      <c r="AC33" s="5" t="n"/>
-      <c r="AD33" s="5" t="n"/>
-      <c r="AE33" s="5" t="n"/>
-      <c r="AF33" s="5" t="n"/>
-      <c r="AG33" s="5" t="n"/>
-      <c r="AH33" s="5" t="n"/>
+      <c r="A33" s="52" t="n"/>
+      <c r="B33" s="52" t="n"/>
+      <c r="C33" s="53" t="n"/>
+      <c r="D33" s="52" t="n"/>
+      <c r="E33" s="52" t="n"/>
+      <c r="F33" s="52" t="n"/>
+      <c r="G33" s="52" t="n"/>
+      <c r="H33" s="52" t="n"/>
+      <c r="I33" s="52" t="n"/>
+      <c r="J33" s="52" t="n"/>
+      <c r="K33" s="52" t="n"/>
+      <c r="L33" s="54" t="n"/>
+      <c r="M33" s="54" t="n"/>
+      <c r="N33" s="52" t="n"/>
+      <c r="O33" s="53" t="n"/>
+      <c r="P33" s="23" t="n"/>
+      <c r="Q33" s="23" t="n"/>
+      <c r="R33" s="23" t="n"/>
+      <c r="S33" s="23" t="n"/>
+      <c r="T33" s="23" t="n"/>
+      <c r="U33" s="23" t="n"/>
+      <c r="V33" s="23" t="n"/>
+      <c r="W33" s="23" t="n"/>
+      <c r="X33" s="23" t="n"/>
+      <c r="Y33" s="23" t="n"/>
+      <c r="Z33" s="23" t="n"/>
+      <c r="AA33" s="23" t="n"/>
+      <c r="AB33" s="23" t="n"/>
+      <c r="AC33" s="23" t="n"/>
+      <c r="AD33" s="23" t="n"/>
+      <c r="AE33" s="23" t="n"/>
+      <c r="AF33" s="23" t="n"/>
+      <c r="AG33" s="23" t="n"/>
+      <c r="AH33" s="23" t="n"/>
+      <c r="AI33" s="23" t="n"/>
+      <c r="AJ33" s="23" t="n"/>
       <c r="AK33" s="23" t="n"/>
       <c r="AL33" s="23" t="n"/>
       <c r="AM33" s="23" t="n"/>
@@ -3188,40 +3273,42 @@
       <c r="BB33" s="23" t="n"/>
     </row>
     <row r="34">
-      <c r="A34" s="5" t="n"/>
-      <c r="B34" s="6" t="n"/>
-      <c r="C34" s="6" t="n"/>
-      <c r="D34" s="5" t="n"/>
-      <c r="E34" s="5" t="n"/>
-      <c r="F34" s="5" t="n"/>
-      <c r="G34" s="5" t="n"/>
-      <c r="H34" s="5" t="n"/>
-      <c r="I34" s="5" t="n"/>
-      <c r="J34" s="5" t="n"/>
-      <c r="K34" s="5" t="n"/>
-      <c r="L34" s="5" t="n"/>
-      <c r="M34" s="5" t="n"/>
-      <c r="N34" s="5" t="n"/>
-      <c r="O34" s="5" t="n"/>
-      <c r="P34" s="5" t="n"/>
-      <c r="Q34" s="5" t="n"/>
-      <c r="R34" s="5" t="n"/>
-      <c r="S34" s="5" t="n"/>
-      <c r="T34" s="5" t="n"/>
-      <c r="U34" s="5" t="n"/>
-      <c r="V34" s="5" t="n"/>
-      <c r="W34" s="5" t="n"/>
-      <c r="X34" s="5" t="n"/>
-      <c r="Y34" s="5" t="n"/>
-      <c r="Z34" s="5" t="n"/>
-      <c r="AA34" s="5" t="n"/>
-      <c r="AB34" s="5" t="n"/>
-      <c r="AC34" s="5" t="n"/>
-      <c r="AD34" s="5" t="n"/>
-      <c r="AE34" s="5" t="n"/>
-      <c r="AF34" s="5" t="n"/>
-      <c r="AG34" s="5" t="n"/>
-      <c r="AH34" s="5" t="n"/>
+      <c r="A34" s="52" t="n"/>
+      <c r="B34" s="52" t="n"/>
+      <c r="C34" s="53" t="n"/>
+      <c r="D34" s="52" t="n"/>
+      <c r="E34" s="52" t="n"/>
+      <c r="F34" s="52" t="n"/>
+      <c r="G34" s="52" t="n"/>
+      <c r="H34" s="52" t="n"/>
+      <c r="I34" s="52" t="n"/>
+      <c r="J34" s="52" t="n"/>
+      <c r="K34" s="52" t="n"/>
+      <c r="L34" s="54" t="n"/>
+      <c r="M34" s="54" t="n"/>
+      <c r="N34" s="52" t="n"/>
+      <c r="O34" s="53" t="n"/>
+      <c r="P34" s="23" t="n"/>
+      <c r="Q34" s="23" t="n"/>
+      <c r="R34" s="23" t="n"/>
+      <c r="S34" s="23" t="n"/>
+      <c r="T34" s="23" t="n"/>
+      <c r="U34" s="23" t="n"/>
+      <c r="V34" s="23" t="n"/>
+      <c r="W34" s="23" t="n"/>
+      <c r="X34" s="23" t="n"/>
+      <c r="Y34" s="23" t="n"/>
+      <c r="Z34" s="23" t="n"/>
+      <c r="AA34" s="23" t="n"/>
+      <c r="AB34" s="23" t="n"/>
+      <c r="AC34" s="23" t="n"/>
+      <c r="AD34" s="23" t="n"/>
+      <c r="AE34" s="23" t="n"/>
+      <c r="AF34" s="23" t="n"/>
+      <c r="AG34" s="23" t="n"/>
+      <c r="AH34" s="23" t="n"/>
+      <c r="AI34" s="23" t="n"/>
+      <c r="AJ34" s="23" t="n"/>
       <c r="AK34" s="23" t="n"/>
       <c r="AL34" s="23" t="n"/>
       <c r="AM34" s="23" t="n"/>
@@ -3242,685 +3329,839 @@
       <c r="BB34" s="23" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="5" t="n"/>
-      <c r="B35" s="6" t="n"/>
-      <c r="C35" s="6" t="n"/>
-      <c r="D35" s="5" t="n"/>
-      <c r="E35" s="5" t="n"/>
-      <c r="F35" s="5" t="n"/>
-      <c r="G35" s="5" t="n"/>
-      <c r="H35" s="5" t="n"/>
-      <c r="I35" s="5" t="n"/>
-      <c r="J35" s="5" t="n"/>
-      <c r="K35" s="5" t="n"/>
-      <c r="L35" s="5" t="n"/>
-      <c r="M35" s="5" t="n"/>
-      <c r="N35" s="5" t="n"/>
-      <c r="O35" s="5" t="n"/>
-      <c r="P35" s="5" t="n"/>
-      <c r="Q35" s="5" t="n"/>
-      <c r="R35" s="5" t="n"/>
-      <c r="S35" s="5" t="n"/>
-      <c r="T35" s="5" t="n"/>
-      <c r="U35" s="5" t="n"/>
-      <c r="V35" s="5" t="n"/>
-      <c r="W35" s="5" t="n"/>
-      <c r="X35" s="5" t="n"/>
-      <c r="Y35" s="5" t="n"/>
-      <c r="Z35" s="5" t="n"/>
-      <c r="AA35" s="5" t="n"/>
-      <c r="AB35" s="5" t="n"/>
-      <c r="AC35" s="5" t="n"/>
-      <c r="AD35" s="5" t="n"/>
-      <c r="AE35" s="5" t="n"/>
-      <c r="AF35" s="5" t="n"/>
-      <c r="AG35" s="5" t="n"/>
-      <c r="AH35" s="5" t="n"/>
+      <c r="A35" s="52" t="n"/>
+      <c r="B35" s="52" t="n"/>
+      <c r="C35" s="53" t="n"/>
+      <c r="D35" s="52" t="n"/>
+      <c r="E35" s="52" t="n"/>
+      <c r="F35" s="52" t="n"/>
+      <c r="G35" s="52" t="n"/>
+      <c r="H35" s="52" t="n"/>
+      <c r="I35" s="52" t="n"/>
+      <c r="J35" s="52" t="n"/>
+      <c r="K35" s="52" t="n"/>
+      <c r="L35" s="54" t="n"/>
+      <c r="M35" s="54" t="n"/>
+      <c r="N35" s="52" t="n"/>
+      <c r="O35" s="53" t="n"/>
+      <c r="P35" s="23" t="n"/>
+      <c r="Q35" s="23" t="n"/>
+      <c r="R35" s="23" t="n"/>
+      <c r="S35" s="23" t="n"/>
+      <c r="T35" s="23" t="n"/>
+      <c r="U35" s="23" t="n"/>
+      <c r="V35" s="23" t="n"/>
+      <c r="W35" s="23" t="n"/>
+      <c r="X35" s="23" t="n"/>
+      <c r="Y35" s="23" t="n"/>
+      <c r="Z35" s="23" t="n"/>
+      <c r="AA35" s="23" t="n"/>
+      <c r="AB35" s="23" t="n"/>
+      <c r="AC35" s="23" t="n"/>
+      <c r="AD35" s="23" t="n"/>
+      <c r="AE35" s="23" t="n"/>
+      <c r="AF35" s="23" t="n"/>
+      <c r="AG35" s="23" t="n"/>
+      <c r="AH35" s="23" t="n"/>
+      <c r="AI35" s="23" t="n"/>
+      <c r="AJ35" s="23" t="n"/>
+      <c r="AK35" s="23" t="n"/>
+      <c r="AL35" s="23" t="n"/>
+      <c r="AM35" s="23" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="5" t="n"/>
-      <c r="B36" s="6" t="n"/>
-      <c r="C36" s="6" t="n"/>
-      <c r="D36" s="5" t="n"/>
-      <c r="E36" s="5" t="n"/>
-      <c r="F36" s="5" t="n"/>
-      <c r="G36" s="5" t="n"/>
-      <c r="H36" s="5" t="n"/>
-      <c r="I36" s="5" t="n"/>
-      <c r="J36" s="5" t="n"/>
-      <c r="K36" s="5" t="n"/>
-      <c r="L36" s="5" t="n"/>
-      <c r="M36" s="5" t="n"/>
-      <c r="N36" s="5" t="n"/>
-      <c r="O36" s="5" t="n"/>
-      <c r="P36" s="5" t="n"/>
-      <c r="Q36" s="5" t="n"/>
-      <c r="R36" s="5" t="n"/>
-      <c r="S36" s="5" t="n"/>
-      <c r="T36" s="5" t="n"/>
-      <c r="U36" s="5" t="n"/>
-      <c r="V36" s="5" t="n"/>
-      <c r="W36" s="5" t="n"/>
-      <c r="X36" s="5" t="n"/>
-      <c r="Y36" s="5" t="n"/>
-      <c r="Z36" s="5" t="n"/>
-      <c r="AA36" s="5" t="n"/>
-      <c r="AB36" s="5" t="n"/>
-      <c r="AC36" s="5" t="n"/>
-      <c r="AD36" s="5" t="n"/>
-      <c r="AE36" s="5" t="n"/>
-      <c r="AF36" s="5" t="n"/>
-      <c r="AG36" s="5" t="n"/>
-      <c r="AH36" s="5" t="n"/>
+      <c r="A36" s="52" t="n"/>
+      <c r="B36" s="52" t="n"/>
+      <c r="C36" s="53" t="n"/>
+      <c r="D36" s="52" t="n"/>
+      <c r="E36" s="52" t="n"/>
+      <c r="F36" s="52" t="n"/>
+      <c r="G36" s="52" t="n"/>
+      <c r="H36" s="52" t="n"/>
+      <c r="I36" s="52" t="n"/>
+      <c r="J36" s="52" t="n"/>
+      <c r="K36" s="52" t="n"/>
+      <c r="L36" s="54" t="n"/>
+      <c r="M36" s="54" t="n"/>
+      <c r="N36" s="52" t="n"/>
+      <c r="O36" s="53" t="n"/>
+      <c r="P36" s="23" t="n"/>
+      <c r="Q36" s="23" t="n"/>
+      <c r="R36" s="23" t="n"/>
+      <c r="S36" s="23" t="n"/>
+      <c r="T36" s="23" t="n"/>
+      <c r="U36" s="23" t="n"/>
+      <c r="V36" s="23" t="n"/>
+      <c r="W36" s="23" t="n"/>
+      <c r="X36" s="23" t="n"/>
+      <c r="Y36" s="23" t="n"/>
+      <c r="Z36" s="23" t="n"/>
+      <c r="AA36" s="23" t="n"/>
+      <c r="AB36" s="23" t="n"/>
+      <c r="AC36" s="23" t="n"/>
+      <c r="AD36" s="23" t="n"/>
+      <c r="AE36" s="23" t="n"/>
+      <c r="AF36" s="23" t="n"/>
+      <c r="AG36" s="23" t="n"/>
+      <c r="AH36" s="23" t="n"/>
+      <c r="AI36" s="23" t="n"/>
+      <c r="AJ36" s="23" t="n"/>
+      <c r="AK36" s="23" t="n"/>
+      <c r="AL36" s="23" t="n"/>
+      <c r="AM36" s="23" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="5" t="n"/>
-      <c r="B37" s="6" t="n"/>
-      <c r="C37" s="6" t="n"/>
-      <c r="D37" s="5" t="n"/>
-      <c r="E37" s="5" t="n"/>
-      <c r="F37" s="5" t="n"/>
-      <c r="G37" s="5" t="n"/>
-      <c r="H37" s="5" t="n"/>
-      <c r="I37" s="5" t="n"/>
-      <c r="J37" s="5" t="n"/>
-      <c r="K37" s="5" t="n"/>
-      <c r="L37" s="5" t="n"/>
-      <c r="M37" s="5" t="n"/>
-      <c r="N37" s="5" t="n"/>
-      <c r="O37" s="5" t="n"/>
-      <c r="P37" s="5" t="n"/>
-      <c r="Q37" s="5" t="n"/>
-      <c r="R37" s="5" t="n"/>
-      <c r="S37" s="5" t="n"/>
-      <c r="T37" s="5" t="n"/>
-      <c r="U37" s="5" t="n"/>
-      <c r="V37" s="5" t="n"/>
-      <c r="W37" s="5" t="n"/>
-      <c r="X37" s="5" t="n"/>
-      <c r="Y37" s="5" t="n"/>
-      <c r="Z37" s="5" t="n"/>
-      <c r="AA37" s="5" t="n"/>
-      <c r="AB37" s="5" t="n"/>
-      <c r="AC37" s="5" t="n"/>
-      <c r="AD37" s="5" t="n"/>
-      <c r="AE37" s="5" t="n"/>
-      <c r="AF37" s="5" t="n"/>
-      <c r="AG37" s="5" t="n"/>
-      <c r="AH37" s="5" t="n"/>
+      <c r="A37" s="52" t="n"/>
+      <c r="B37" s="52" t="n"/>
+      <c r="C37" s="53" t="n"/>
+      <c r="D37" s="52" t="n"/>
+      <c r="E37" s="52" t="n"/>
+      <c r="F37" s="52" t="n"/>
+      <c r="G37" s="52" t="n"/>
+      <c r="H37" s="52" t="n"/>
+      <c r="I37" s="52" t="n"/>
+      <c r="J37" s="52" t="n"/>
+      <c r="K37" s="52" t="n"/>
+      <c r="L37" s="54" t="n"/>
+      <c r="M37" s="54" t="n"/>
+      <c r="N37" s="52" t="n"/>
+      <c r="O37" s="53" t="n"/>
+      <c r="P37" s="23" t="n"/>
+      <c r="Q37" s="23" t="n"/>
+      <c r="R37" s="23" t="n"/>
+      <c r="S37" s="23" t="n"/>
+      <c r="T37" s="23" t="n"/>
+      <c r="U37" s="23" t="n"/>
+      <c r="V37" s="23" t="n"/>
+      <c r="W37" s="23" t="n"/>
+      <c r="X37" s="23" t="n"/>
+      <c r="Y37" s="23" t="n"/>
+      <c r="Z37" s="23" t="n"/>
+      <c r="AA37" s="23" t="n"/>
+      <c r="AB37" s="23" t="n"/>
+      <c r="AC37" s="23" t="n"/>
+      <c r="AD37" s="23" t="n"/>
+      <c r="AE37" s="23" t="n"/>
+      <c r="AF37" s="23" t="n"/>
+      <c r="AG37" s="23" t="n"/>
+      <c r="AH37" s="23" t="n"/>
+      <c r="AI37" s="23" t="n"/>
+      <c r="AJ37" s="23" t="n"/>
+      <c r="AK37" s="23" t="n"/>
+      <c r="AL37" s="23" t="n"/>
+      <c r="AM37" s="23" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="5" t="n"/>
-      <c r="B38" s="6" t="n"/>
-      <c r="C38" s="6" t="n"/>
-      <c r="D38" s="5" t="n"/>
-      <c r="E38" s="5" t="n"/>
-      <c r="F38" s="5" t="n"/>
-      <c r="G38" s="5" t="n"/>
-      <c r="H38" s="5" t="n"/>
-      <c r="I38" s="5" t="n"/>
-      <c r="J38" s="5" t="n"/>
-      <c r="K38" s="5" t="n"/>
-      <c r="L38" s="5" t="n"/>
-      <c r="M38" s="5" t="n"/>
-      <c r="N38" s="5" t="n"/>
-      <c r="O38" s="5" t="n"/>
-      <c r="P38" s="5" t="n"/>
-      <c r="Q38" s="5" t="n"/>
-      <c r="R38" s="5" t="n"/>
-      <c r="S38" s="5" t="n"/>
-      <c r="T38" s="5" t="n"/>
-      <c r="U38" s="5" t="n"/>
-      <c r="V38" s="5" t="n"/>
-      <c r="W38" s="5" t="n"/>
-      <c r="X38" s="5" t="n"/>
-      <c r="Y38" s="5" t="n"/>
-      <c r="Z38" s="5" t="n"/>
-      <c r="AA38" s="5" t="n"/>
-      <c r="AB38" s="5" t="n"/>
-      <c r="AC38" s="5" t="n"/>
-      <c r="AD38" s="5" t="n"/>
-      <c r="AE38" s="5" t="n"/>
-      <c r="AF38" s="5" t="n"/>
-      <c r="AG38" s="5" t="n"/>
-      <c r="AH38" s="5" t="n"/>
+      <c r="A38" s="52" t="n"/>
+      <c r="B38" s="52" t="n"/>
+      <c r="C38" s="53" t="n"/>
+      <c r="D38" s="52" t="n"/>
+      <c r="E38" s="52" t="n"/>
+      <c r="F38" s="52" t="n"/>
+      <c r="G38" s="52" t="n"/>
+      <c r="H38" s="52" t="n"/>
+      <c r="I38" s="52" t="n"/>
+      <c r="J38" s="52" t="n"/>
+      <c r="K38" s="52" t="n"/>
+      <c r="L38" s="54" t="n"/>
+      <c r="M38" s="54" t="n"/>
+      <c r="N38" s="52" t="n"/>
+      <c r="O38" s="53" t="n"/>
+      <c r="P38" s="23" t="n"/>
+      <c r="Q38" s="23" t="n"/>
+      <c r="R38" s="23" t="n"/>
+      <c r="S38" s="23" t="n"/>
+      <c r="T38" s="23" t="n"/>
+      <c r="U38" s="23" t="n"/>
+      <c r="V38" s="23" t="n"/>
+      <c r="W38" s="23" t="n"/>
+      <c r="X38" s="23" t="n"/>
+      <c r="Y38" s="23" t="n"/>
+      <c r="Z38" s="23" t="n"/>
+      <c r="AA38" s="23" t="n"/>
+      <c r="AB38" s="23" t="n"/>
+      <c r="AC38" s="23" t="n"/>
+      <c r="AD38" s="23" t="n"/>
+      <c r="AE38" s="23" t="n"/>
+      <c r="AF38" s="23" t="n"/>
+      <c r="AG38" s="23" t="n"/>
+      <c r="AH38" s="23" t="n"/>
+      <c r="AI38" s="23" t="n"/>
+      <c r="AJ38" s="23" t="n"/>
+      <c r="AK38" s="23" t="n"/>
+      <c r="AL38" s="23" t="n"/>
+      <c r="AM38" s="23" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="5" t="n"/>
-      <c r="B39" s="6" t="n"/>
-      <c r="C39" s="6" t="n"/>
-      <c r="D39" s="5" t="n"/>
-      <c r="E39" s="5" t="n"/>
-      <c r="F39" s="5" t="n"/>
-      <c r="G39" s="5" t="n"/>
-      <c r="H39" s="5" t="n"/>
-      <c r="I39" s="5" t="n"/>
-      <c r="J39" s="5" t="n"/>
-      <c r="K39" s="5" t="n"/>
-      <c r="L39" s="5" t="n"/>
-      <c r="M39" s="5" t="n"/>
-      <c r="N39" s="5" t="n"/>
-      <c r="O39" s="5" t="n"/>
-      <c r="P39" s="5" t="n"/>
-      <c r="Q39" s="5" t="n"/>
-      <c r="R39" s="5" t="n"/>
-      <c r="S39" s="5" t="n"/>
-      <c r="T39" s="5" t="n"/>
-      <c r="U39" s="5" t="n"/>
-      <c r="V39" s="5" t="n"/>
-      <c r="W39" s="5" t="n"/>
-      <c r="X39" s="5" t="n"/>
-      <c r="Y39" s="5" t="n"/>
-      <c r="Z39" s="5" t="n"/>
-      <c r="AA39" s="5" t="n"/>
-      <c r="AB39" s="5" t="n"/>
-      <c r="AC39" s="5" t="n"/>
-      <c r="AD39" s="5" t="n"/>
-      <c r="AE39" s="5" t="n"/>
-      <c r="AF39" s="5" t="n"/>
-      <c r="AG39" s="5" t="n"/>
-      <c r="AH39" s="5" t="n"/>
+      <c r="A39" s="52" t="n"/>
+      <c r="B39" s="52" t="n"/>
+      <c r="C39" s="53" t="n"/>
+      <c r="D39" s="52" t="n"/>
+      <c r="E39" s="52" t="n"/>
+      <c r="F39" s="52" t="n"/>
+      <c r="G39" s="52" t="n"/>
+      <c r="H39" s="52" t="n"/>
+      <c r="I39" s="52" t="n"/>
+      <c r="J39" s="52" t="n"/>
+      <c r="K39" s="52" t="n"/>
+      <c r="L39" s="54" t="n"/>
+      <c r="M39" s="54" t="n"/>
+      <c r="N39" s="52" t="n"/>
+      <c r="O39" s="53" t="n"/>
+      <c r="P39" s="23" t="n"/>
+      <c r="Q39" s="23" t="n"/>
+      <c r="R39" s="23" t="n"/>
+      <c r="S39" s="23" t="n"/>
+      <c r="T39" s="23" t="n"/>
+      <c r="U39" s="23" t="n"/>
+      <c r="V39" s="23" t="n"/>
+      <c r="W39" s="23" t="n"/>
+      <c r="X39" s="23" t="n"/>
+      <c r="Y39" s="23" t="n"/>
+      <c r="Z39" s="23" t="n"/>
+      <c r="AA39" s="23" t="n"/>
+      <c r="AB39" s="23" t="n"/>
+      <c r="AC39" s="23" t="n"/>
+      <c r="AD39" s="23" t="n"/>
+      <c r="AE39" s="23" t="n"/>
+      <c r="AF39" s="23" t="n"/>
+      <c r="AG39" s="23" t="n"/>
+      <c r="AH39" s="23" t="n"/>
+      <c r="AI39" s="23" t="n"/>
+      <c r="AJ39" s="23" t="n"/>
+      <c r="AK39" s="23" t="n"/>
+      <c r="AL39" s="23" t="n"/>
+      <c r="AM39" s="23" t="n"/>
     </row>
     <row r="40">
-      <c r="A40" s="5" t="n"/>
-      <c r="B40" s="6" t="n"/>
-      <c r="C40" s="6" t="n"/>
-      <c r="D40" s="5" t="n"/>
-      <c r="E40" s="5" t="n"/>
-      <c r="F40" s="5" t="n"/>
-      <c r="G40" s="5" t="n"/>
-      <c r="H40" s="5" t="n"/>
-      <c r="I40" s="5" t="n"/>
-      <c r="J40" s="5" t="n"/>
-      <c r="K40" s="5" t="n"/>
-      <c r="L40" s="5" t="n"/>
-      <c r="M40" s="5" t="n"/>
-      <c r="N40" s="5" t="n"/>
-      <c r="O40" s="5" t="n"/>
-      <c r="P40" s="5" t="n"/>
-      <c r="Q40" s="5" t="n"/>
-      <c r="R40" s="5" t="n"/>
-      <c r="S40" s="5" t="n"/>
-      <c r="T40" s="5" t="n"/>
-      <c r="U40" s="5" t="n"/>
-      <c r="V40" s="5" t="n"/>
-      <c r="W40" s="5" t="n"/>
-      <c r="X40" s="5" t="n"/>
-      <c r="Y40" s="5" t="n"/>
-      <c r="Z40" s="5" t="n"/>
-      <c r="AA40" s="5" t="n"/>
-      <c r="AB40" s="5" t="n"/>
-      <c r="AC40" s="5" t="n"/>
-      <c r="AD40" s="5" t="n"/>
-      <c r="AE40" s="5" t="n"/>
-      <c r="AF40" s="5" t="n"/>
-      <c r="AG40" s="5" t="n"/>
-      <c r="AH40" s="5" t="n"/>
+      <c r="A40" s="52" t="n"/>
+      <c r="B40" s="52" t="n"/>
+      <c r="C40" s="53" t="n"/>
+      <c r="D40" s="52" t="n"/>
+      <c r="E40" s="52" t="n"/>
+      <c r="F40" s="52" t="n"/>
+      <c r="G40" s="52" t="n"/>
+      <c r="H40" s="52" t="n"/>
+      <c r="I40" s="52" t="n"/>
+      <c r="J40" s="52" t="n"/>
+      <c r="K40" s="52" t="n"/>
+      <c r="L40" s="54" t="n"/>
+      <c r="M40" s="54" t="n"/>
+      <c r="N40" s="52" t="n"/>
+      <c r="O40" s="53" t="n"/>
+      <c r="P40" s="23" t="n"/>
+      <c r="Q40" s="23" t="n"/>
+      <c r="R40" s="23" t="n"/>
+      <c r="S40" s="23" t="n"/>
+      <c r="T40" s="23" t="n"/>
+      <c r="U40" s="23" t="n"/>
+      <c r="V40" s="23" t="n"/>
+      <c r="W40" s="23" t="n"/>
+      <c r="X40" s="23" t="n"/>
+      <c r="Y40" s="23" t="n"/>
+      <c r="Z40" s="23" t="n"/>
+      <c r="AA40" s="23" t="n"/>
+      <c r="AB40" s="23" t="n"/>
+      <c r="AC40" s="23" t="n"/>
+      <c r="AD40" s="23" t="n"/>
+      <c r="AE40" s="23" t="n"/>
+      <c r="AF40" s="23" t="n"/>
+      <c r="AG40" s="23" t="n"/>
+      <c r="AH40" s="23" t="n"/>
+      <c r="AI40" s="23" t="n"/>
+      <c r="AJ40" s="23" t="n"/>
+      <c r="AK40" s="23" t="n"/>
+      <c r="AL40" s="23" t="n"/>
+      <c r="AM40" s="23" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="5" t="n"/>
-      <c r="B41" s="6" t="n"/>
-      <c r="C41" s="6" t="n"/>
-      <c r="D41" s="5" t="n"/>
-      <c r="E41" s="5" t="n"/>
-      <c r="F41" s="5" t="n"/>
-      <c r="G41" s="5" t="n"/>
-      <c r="H41" s="5" t="n"/>
-      <c r="I41" s="5" t="n"/>
-      <c r="J41" s="5" t="n"/>
-      <c r="K41" s="5" t="n"/>
-      <c r="L41" s="5" t="n"/>
-      <c r="M41" s="5" t="n"/>
-      <c r="N41" s="5" t="n"/>
-      <c r="O41" s="5" t="n"/>
-      <c r="P41" s="5" t="n"/>
-      <c r="Q41" s="5" t="n"/>
-      <c r="R41" s="5" t="n"/>
-      <c r="S41" s="5" t="n"/>
-      <c r="T41" s="5" t="n"/>
-      <c r="U41" s="5" t="n"/>
-      <c r="V41" s="5" t="n"/>
-      <c r="W41" s="5" t="n"/>
-      <c r="X41" s="5" t="n"/>
-      <c r="Y41" s="5" t="n"/>
-      <c r="Z41" s="5" t="n"/>
-      <c r="AA41" s="5" t="n"/>
-      <c r="AB41" s="5" t="n"/>
-      <c r="AC41" s="5" t="n"/>
-      <c r="AD41" s="5" t="n"/>
-      <c r="AE41" s="5" t="n"/>
-      <c r="AF41" s="5" t="n"/>
-      <c r="AG41" s="5" t="n"/>
-      <c r="AH41" s="5" t="n"/>
+      <c r="A41" s="52" t="n"/>
+      <c r="B41" s="52" t="n"/>
+      <c r="C41" s="53" t="n"/>
+      <c r="D41" s="52" t="n"/>
+      <c r="E41" s="52" t="n"/>
+      <c r="F41" s="52" t="n"/>
+      <c r="G41" s="52" t="n"/>
+      <c r="H41" s="52" t="n"/>
+      <c r="I41" s="52" t="n"/>
+      <c r="J41" s="52" t="n"/>
+      <c r="K41" s="52" t="n"/>
+      <c r="L41" s="54" t="n"/>
+      <c r="M41" s="54" t="n"/>
+      <c r="N41" s="52" t="n"/>
+      <c r="O41" s="53" t="n"/>
+      <c r="P41" s="23" t="n"/>
+      <c r="Q41" s="23" t="n"/>
+      <c r="R41" s="23" t="n"/>
+      <c r="S41" s="23" t="n"/>
+      <c r="T41" s="23" t="n"/>
+      <c r="U41" s="23" t="n"/>
+      <c r="V41" s="23" t="n"/>
+      <c r="W41" s="23" t="n"/>
+      <c r="X41" s="23" t="n"/>
+      <c r="Y41" s="23" t="n"/>
+      <c r="Z41" s="23" t="n"/>
+      <c r="AA41" s="23" t="n"/>
+      <c r="AB41" s="23" t="n"/>
+      <c r="AC41" s="23" t="n"/>
+      <c r="AD41" s="23" t="n"/>
+      <c r="AE41" s="23" t="n"/>
+      <c r="AF41" s="23" t="n"/>
+      <c r="AG41" s="23" t="n"/>
+      <c r="AH41" s="23" t="n"/>
+      <c r="AI41" s="23" t="n"/>
+      <c r="AJ41" s="23" t="n"/>
+      <c r="AK41" s="23" t="n"/>
+      <c r="AL41" s="23" t="n"/>
+      <c r="AM41" s="23" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" s="5" t="n"/>
-      <c r="B42" s="6" t="n"/>
-      <c r="C42" s="6" t="n"/>
-      <c r="D42" s="5" t="n"/>
-      <c r="E42" s="5" t="n"/>
-      <c r="F42" s="5" t="n"/>
-      <c r="G42" s="5" t="n"/>
-      <c r="H42" s="5" t="n"/>
-      <c r="I42" s="5" t="n"/>
-      <c r="J42" s="5" t="n"/>
-      <c r="K42" s="5" t="n"/>
-      <c r="L42" s="5" t="n"/>
-      <c r="M42" s="5" t="n"/>
-      <c r="N42" s="5" t="n"/>
-      <c r="O42" s="5" t="n"/>
-      <c r="P42" s="5" t="n"/>
-      <c r="Q42" s="5" t="n"/>
-      <c r="R42" s="5" t="n"/>
-      <c r="S42" s="5" t="n"/>
-      <c r="T42" s="5" t="n"/>
-      <c r="U42" s="5" t="n"/>
-      <c r="V42" s="5" t="n"/>
-      <c r="W42" s="5" t="n"/>
-      <c r="X42" s="5" t="n"/>
-      <c r="Y42" s="5" t="n"/>
-      <c r="Z42" s="5" t="n"/>
-      <c r="AA42" s="5" t="n"/>
-      <c r="AB42" s="5" t="n"/>
-      <c r="AC42" s="5" t="n"/>
-      <c r="AD42" s="5" t="n"/>
-      <c r="AE42" s="5" t="n"/>
-      <c r="AF42" s="5" t="n"/>
-      <c r="AG42" s="5" t="n"/>
-      <c r="AH42" s="5" t="n"/>
+      <c r="A42" s="52" t="n"/>
+      <c r="B42" s="52" t="n"/>
+      <c r="C42" s="53" t="n"/>
+      <c r="D42" s="52" t="n"/>
+      <c r="E42" s="52" t="n"/>
+      <c r="F42" s="52" t="n"/>
+      <c r="G42" s="52" t="n"/>
+      <c r="H42" s="52" t="n"/>
+      <c r="I42" s="52" t="n"/>
+      <c r="J42" s="52" t="n"/>
+      <c r="K42" s="52" t="n"/>
+      <c r="L42" s="54" t="n"/>
+      <c r="M42" s="54" t="n"/>
+      <c r="N42" s="52" t="n"/>
+      <c r="O42" s="53" t="n"/>
+      <c r="P42" s="23" t="n"/>
+      <c r="Q42" s="23" t="n"/>
+      <c r="R42" s="23" t="n"/>
+      <c r="S42" s="23" t="n"/>
+      <c r="T42" s="23" t="n"/>
+      <c r="U42" s="23" t="n"/>
+      <c r="V42" s="23" t="n"/>
+      <c r="W42" s="23" t="n"/>
+      <c r="X42" s="23" t="n"/>
+      <c r="Y42" s="23" t="n"/>
+      <c r="Z42" s="23" t="n"/>
+      <c r="AA42" s="23" t="n"/>
+      <c r="AB42" s="23" t="n"/>
+      <c r="AC42" s="23" t="n"/>
+      <c r="AD42" s="23" t="n"/>
+      <c r="AE42" s="23" t="n"/>
+      <c r="AF42" s="23" t="n"/>
+      <c r="AG42" s="23" t="n"/>
+      <c r="AH42" s="23" t="n"/>
+      <c r="AI42" s="23" t="n"/>
+      <c r="AJ42" s="23" t="n"/>
+      <c r="AK42" s="23" t="n"/>
+      <c r="AL42" s="23" t="n"/>
+      <c r="AM42" s="23" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" s="5" t="n"/>
-      <c r="B43" s="6" t="n"/>
-      <c r="C43" s="6" t="n"/>
-      <c r="D43" s="5" t="n"/>
-      <c r="E43" s="5" t="n"/>
-      <c r="F43" s="5" t="n"/>
-      <c r="G43" s="5" t="n"/>
-      <c r="H43" s="5" t="n"/>
-      <c r="I43" s="5" t="n"/>
-      <c r="J43" s="5" t="n"/>
-      <c r="K43" s="5" t="n"/>
-      <c r="L43" s="5" t="n"/>
-      <c r="M43" s="5" t="n"/>
-      <c r="N43" s="5" t="n"/>
-      <c r="O43" s="5" t="n"/>
-      <c r="P43" s="5" t="n"/>
-      <c r="Q43" s="5" t="n"/>
-      <c r="R43" s="5" t="n"/>
-      <c r="S43" s="5" t="n"/>
-      <c r="T43" s="5" t="n"/>
-      <c r="U43" s="5" t="n"/>
-      <c r="V43" s="5" t="n"/>
-      <c r="W43" s="5" t="n"/>
-      <c r="X43" s="5" t="n"/>
-      <c r="Y43" s="5" t="n"/>
-      <c r="Z43" s="5" t="n"/>
-      <c r="AA43" s="5" t="n"/>
-      <c r="AB43" s="5" t="n"/>
-      <c r="AC43" s="5" t="n"/>
-      <c r="AD43" s="5" t="n"/>
-      <c r="AE43" s="5" t="n"/>
-      <c r="AF43" s="5" t="n"/>
-      <c r="AG43" s="5" t="n"/>
-      <c r="AH43" s="5" t="n"/>
+      <c r="A43" s="52" t="n"/>
+      <c r="B43" s="52" t="n"/>
+      <c r="C43" s="53" t="n"/>
+      <c r="D43" s="52" t="n"/>
+      <c r="E43" s="52" t="n"/>
+      <c r="F43" s="52" t="n"/>
+      <c r="G43" s="52" t="n"/>
+      <c r="H43" s="52" t="n"/>
+      <c r="I43" s="52" t="n"/>
+      <c r="J43" s="52" t="n"/>
+      <c r="K43" s="52" t="n"/>
+      <c r="L43" s="54" t="n"/>
+      <c r="M43" s="54" t="n"/>
+      <c r="N43" s="52" t="n"/>
+      <c r="O43" s="53" t="n"/>
+      <c r="P43" s="23" t="n"/>
+      <c r="Q43" s="23" t="n"/>
+      <c r="R43" s="23" t="n"/>
+      <c r="S43" s="23" t="n"/>
+      <c r="T43" s="23" t="n"/>
+      <c r="U43" s="23" t="n"/>
+      <c r="V43" s="23" t="n"/>
+      <c r="W43" s="23" t="n"/>
+      <c r="X43" s="23" t="n"/>
+      <c r="Y43" s="23" t="n"/>
+      <c r="Z43" s="23" t="n"/>
+      <c r="AA43" s="23" t="n"/>
+      <c r="AB43" s="23" t="n"/>
+      <c r="AC43" s="23" t="n"/>
+      <c r="AD43" s="23" t="n"/>
+      <c r="AE43" s="23" t="n"/>
+      <c r="AF43" s="23" t="n"/>
+      <c r="AG43" s="23" t="n"/>
+      <c r="AH43" s="23" t="n"/>
+      <c r="AI43" s="23" t="n"/>
+      <c r="AJ43" s="23" t="n"/>
+      <c r="AK43" s="23" t="n"/>
+      <c r="AL43" s="23" t="n"/>
+      <c r="AM43" s="23" t="n"/>
     </row>
     <row r="44">
-      <c r="A44" s="5" t="n"/>
-      <c r="B44" s="6" t="n"/>
-      <c r="C44" s="6" t="n"/>
-      <c r="D44" s="5" t="n"/>
-      <c r="E44" s="5" t="n"/>
-      <c r="F44" s="5" t="n"/>
-      <c r="G44" s="5" t="n"/>
-      <c r="H44" s="5" t="n"/>
-      <c r="I44" s="5" t="n"/>
-      <c r="J44" s="5" t="n"/>
-      <c r="K44" s="5" t="n"/>
-      <c r="L44" s="5" t="n"/>
-      <c r="M44" s="5" t="n"/>
-      <c r="N44" s="5" t="n"/>
-      <c r="O44" s="5" t="n"/>
-      <c r="P44" s="5" t="n"/>
-      <c r="Q44" s="5" t="n"/>
-      <c r="R44" s="5" t="n"/>
-      <c r="S44" s="5" t="n"/>
-      <c r="T44" s="5" t="n"/>
-      <c r="U44" s="5" t="n"/>
-      <c r="V44" s="5" t="n"/>
-      <c r="W44" s="5" t="n"/>
-      <c r="X44" s="5" t="n"/>
-      <c r="Y44" s="5" t="n"/>
-      <c r="Z44" s="5" t="n"/>
-      <c r="AA44" s="5" t="n"/>
-      <c r="AB44" s="5" t="n"/>
-      <c r="AC44" s="5" t="n"/>
-      <c r="AD44" s="5" t="n"/>
-      <c r="AE44" s="5" t="n"/>
-      <c r="AF44" s="5" t="n"/>
-      <c r="AG44" s="5" t="n"/>
-      <c r="AH44" s="5" t="n"/>
+      <c r="A44" s="52" t="n"/>
+      <c r="B44" s="52" t="n"/>
+      <c r="C44" s="53" t="n"/>
+      <c r="D44" s="52" t="n"/>
+      <c r="E44" s="52" t="n"/>
+      <c r="F44" s="52" t="n"/>
+      <c r="G44" s="52" t="n"/>
+      <c r="H44" s="52" t="n"/>
+      <c r="I44" s="52" t="n"/>
+      <c r="J44" s="52" t="n"/>
+      <c r="K44" s="52" t="n"/>
+      <c r="L44" s="54" t="n"/>
+      <c r="M44" s="54" t="n"/>
+      <c r="N44" s="52" t="n"/>
+      <c r="O44" s="53" t="n"/>
+      <c r="P44" s="23" t="n"/>
+      <c r="Q44" s="23" t="n"/>
+      <c r="R44" s="23" t="n"/>
+      <c r="S44" s="23" t="n"/>
+      <c r="T44" s="23" t="n"/>
+      <c r="U44" s="23" t="n"/>
+      <c r="V44" s="23" t="n"/>
+      <c r="W44" s="23" t="n"/>
+      <c r="X44" s="23" t="n"/>
+      <c r="Y44" s="23" t="n"/>
+      <c r="Z44" s="23" t="n"/>
+      <c r="AA44" s="23" t="n"/>
+      <c r="AB44" s="23" t="n"/>
+      <c r="AC44" s="23" t="n"/>
+      <c r="AD44" s="23" t="n"/>
+      <c r="AE44" s="23" t="n"/>
+      <c r="AF44" s="23" t="n"/>
+      <c r="AG44" s="23" t="n"/>
+      <c r="AH44" s="23" t="n"/>
+      <c r="AI44" s="23" t="n"/>
+      <c r="AJ44" s="23" t="n"/>
+      <c r="AK44" s="23" t="n"/>
+      <c r="AL44" s="23" t="n"/>
+      <c r="AM44" s="23" t="n"/>
     </row>
     <row r="45">
-      <c r="A45" s="5" t="n"/>
-      <c r="B45" s="6" t="n"/>
-      <c r="C45" s="6" t="n"/>
-      <c r="D45" s="5" t="n"/>
-      <c r="E45" s="5" t="n"/>
-      <c r="F45" s="5" t="n"/>
-      <c r="G45" s="5" t="n"/>
-      <c r="H45" s="5" t="n"/>
-      <c r="I45" s="5" t="n"/>
-      <c r="J45" s="5" t="n"/>
-      <c r="K45" s="5" t="n"/>
-      <c r="L45" s="5" t="n"/>
-      <c r="M45" s="5" t="n"/>
-      <c r="N45" s="5" t="n"/>
-      <c r="O45" s="5" t="n"/>
-      <c r="P45" s="5" t="n"/>
-      <c r="Q45" s="5" t="n"/>
-      <c r="R45" s="5" t="n"/>
-      <c r="S45" s="5" t="n"/>
-      <c r="T45" s="5" t="n"/>
-      <c r="U45" s="5" t="n"/>
-      <c r="V45" s="5" t="n"/>
-      <c r="W45" s="5" t="n"/>
-      <c r="X45" s="5" t="n"/>
-      <c r="Y45" s="5" t="n"/>
-      <c r="Z45" s="5" t="n"/>
-      <c r="AA45" s="5" t="n"/>
-      <c r="AB45" s="5" t="n"/>
-      <c r="AC45" s="5" t="n"/>
-      <c r="AD45" s="5" t="n"/>
-      <c r="AE45" s="5" t="n"/>
-      <c r="AF45" s="5" t="n"/>
-      <c r="AG45" s="5" t="n"/>
-      <c r="AH45" s="5" t="n"/>
+      <c r="A45" s="52" t="n"/>
+      <c r="B45" s="52" t="n"/>
+      <c r="C45" s="53" t="n"/>
+      <c r="D45" s="52" t="n"/>
+      <c r="E45" s="52" t="n"/>
+      <c r="F45" s="52" t="n"/>
+      <c r="G45" s="52" t="n"/>
+      <c r="H45" s="52" t="n"/>
+      <c r="I45" s="52" t="n"/>
+      <c r="J45" s="52" t="n"/>
+      <c r="K45" s="52" t="n"/>
+      <c r="L45" s="54" t="n"/>
+      <c r="M45" s="54" t="n"/>
+      <c r="N45" s="52" t="n"/>
+      <c r="O45" s="53" t="n"/>
+      <c r="P45" s="23" t="n"/>
+      <c r="Q45" s="23" t="n"/>
+      <c r="R45" s="23" t="n"/>
+      <c r="S45" s="23" t="n"/>
+      <c r="T45" s="23" t="n"/>
+      <c r="U45" s="23" t="n"/>
+      <c r="V45" s="23" t="n"/>
+      <c r="W45" s="23" t="n"/>
+      <c r="X45" s="23" t="n"/>
+      <c r="Y45" s="23" t="n"/>
+      <c r="Z45" s="23" t="n"/>
+      <c r="AA45" s="23" t="n"/>
+      <c r="AB45" s="23" t="n"/>
+      <c r="AC45" s="23" t="n"/>
+      <c r="AD45" s="23" t="n"/>
+      <c r="AE45" s="23" t="n"/>
+      <c r="AF45" s="23" t="n"/>
+      <c r="AG45" s="23" t="n"/>
+      <c r="AH45" s="23" t="n"/>
+      <c r="AI45" s="23" t="n"/>
+      <c r="AJ45" s="23" t="n"/>
+      <c r="AK45" s="23" t="n"/>
+      <c r="AL45" s="23" t="n"/>
+      <c r="AM45" s="23" t="n"/>
     </row>
     <row r="46">
-      <c r="A46" s="5" t="n"/>
-      <c r="B46" s="6" t="n"/>
-      <c r="C46" s="6" t="n"/>
-      <c r="D46" s="5" t="n"/>
-      <c r="E46" s="5" t="n"/>
-      <c r="F46" s="5" t="n"/>
-      <c r="G46" s="5" t="n"/>
-      <c r="H46" s="5" t="n"/>
-      <c r="I46" s="5" t="n"/>
-      <c r="J46" s="5" t="n"/>
-      <c r="K46" s="5" t="n"/>
-      <c r="L46" s="5" t="n"/>
-      <c r="M46" s="5" t="n"/>
-      <c r="N46" s="5" t="n"/>
-      <c r="O46" s="5" t="n"/>
-      <c r="P46" s="5" t="n"/>
-      <c r="Q46" s="5" t="n"/>
-      <c r="R46" s="5" t="n"/>
-      <c r="S46" s="5" t="n"/>
-      <c r="T46" s="5" t="n"/>
-      <c r="U46" s="5" t="n"/>
-      <c r="V46" s="5" t="n"/>
-      <c r="W46" s="5" t="n"/>
-      <c r="X46" s="5" t="n"/>
-      <c r="Y46" s="5" t="n"/>
-      <c r="Z46" s="5" t="n"/>
-      <c r="AA46" s="5" t="n"/>
-      <c r="AB46" s="5" t="n"/>
-      <c r="AC46" s="5" t="n"/>
-      <c r="AD46" s="5" t="n"/>
-      <c r="AE46" s="5" t="n"/>
-      <c r="AF46" s="5" t="n"/>
-      <c r="AG46" s="5" t="n"/>
-      <c r="AH46" s="5" t="n"/>
+      <c r="A46" s="52" t="n"/>
+      <c r="B46" s="52" t="n"/>
+      <c r="C46" s="53" t="n"/>
+      <c r="D46" s="52" t="n"/>
+      <c r="E46" s="52" t="n"/>
+      <c r="F46" s="52" t="n"/>
+      <c r="G46" s="52" t="n"/>
+      <c r="H46" s="52" t="n"/>
+      <c r="I46" s="52" t="n"/>
+      <c r="J46" s="52" t="n"/>
+      <c r="K46" s="52" t="n"/>
+      <c r="L46" s="54" t="n"/>
+      <c r="M46" s="54" t="n"/>
+      <c r="N46" s="52" t="n"/>
+      <c r="O46" s="53" t="n"/>
+      <c r="P46" s="23" t="n"/>
+      <c r="Q46" s="23" t="n"/>
+      <c r="R46" s="23" t="n"/>
+      <c r="S46" s="23" t="n"/>
+      <c r="T46" s="23" t="n"/>
+      <c r="U46" s="23" t="n"/>
+      <c r="V46" s="23" t="n"/>
+      <c r="W46" s="23" t="n"/>
+      <c r="X46" s="23" t="n"/>
+      <c r="Y46" s="23" t="n"/>
+      <c r="Z46" s="23" t="n"/>
+      <c r="AA46" s="23" t="n"/>
+      <c r="AB46" s="23" t="n"/>
+      <c r="AC46" s="23" t="n"/>
+      <c r="AD46" s="23" t="n"/>
+      <c r="AE46" s="23" t="n"/>
+      <c r="AF46" s="23" t="n"/>
+      <c r="AG46" s="23" t="n"/>
+      <c r="AH46" s="23" t="n"/>
+      <c r="AI46" s="23" t="n"/>
+      <c r="AJ46" s="23" t="n"/>
+      <c r="AK46" s="23" t="n"/>
+      <c r="AL46" s="23" t="n"/>
+      <c r="AM46" s="23" t="n"/>
     </row>
     <row r="47">
-      <c r="A47" s="5" t="n"/>
-      <c r="B47" s="6" t="n"/>
-      <c r="C47" s="6" t="n"/>
-      <c r="D47" s="5" t="n"/>
-      <c r="E47" s="5" t="n"/>
-      <c r="F47" s="5" t="n"/>
-      <c r="G47" s="5" t="n"/>
-      <c r="H47" s="5" t="n"/>
-      <c r="I47" s="5" t="n"/>
-      <c r="J47" s="5" t="n"/>
-      <c r="K47" s="5" t="n"/>
-      <c r="L47" s="5" t="n"/>
-      <c r="M47" s="5" t="n"/>
-      <c r="N47" s="5" t="n"/>
-      <c r="O47" s="5" t="n"/>
-      <c r="P47" s="5" t="n"/>
-      <c r="Q47" s="5" t="n"/>
-      <c r="R47" s="5" t="n"/>
-      <c r="S47" s="5" t="n"/>
-      <c r="T47" s="5" t="n"/>
-      <c r="U47" s="5" t="n"/>
-      <c r="V47" s="5" t="n"/>
-      <c r="W47" s="5" t="n"/>
-      <c r="X47" s="5" t="n"/>
-      <c r="Y47" s="5" t="n"/>
-      <c r="Z47" s="5" t="n"/>
-      <c r="AA47" s="5" t="n"/>
-      <c r="AB47" s="5" t="n"/>
-      <c r="AC47" s="5" t="n"/>
-      <c r="AD47" s="5" t="n"/>
-      <c r="AE47" s="5" t="n"/>
-      <c r="AF47" s="5" t="n"/>
-      <c r="AG47" s="5" t="n"/>
-      <c r="AH47" s="5" t="n"/>
+      <c r="A47" s="52" t="n"/>
+      <c r="B47" s="52" t="n"/>
+      <c r="C47" s="53" t="n"/>
+      <c r="D47" s="52" t="n"/>
+      <c r="E47" s="52" t="n"/>
+      <c r="F47" s="52" t="n"/>
+      <c r="G47" s="52" t="n"/>
+      <c r="H47" s="52" t="n"/>
+      <c r="I47" s="52" t="n"/>
+      <c r="J47" s="52" t="n"/>
+      <c r="K47" s="52" t="n"/>
+      <c r="L47" s="54" t="n"/>
+      <c r="M47" s="54" t="n"/>
+      <c r="N47" s="52" t="n"/>
+      <c r="O47" s="53" t="n"/>
+      <c r="P47" s="23" t="n"/>
+      <c r="Q47" s="23" t="n"/>
+      <c r="R47" s="23" t="n"/>
+      <c r="S47" s="23" t="n"/>
+      <c r="T47" s="23" t="n"/>
+      <c r="U47" s="23" t="n"/>
+      <c r="V47" s="23" t="n"/>
+      <c r="W47" s="23" t="n"/>
+      <c r="X47" s="23" t="n"/>
+      <c r="Y47" s="23" t="n"/>
+      <c r="Z47" s="23" t="n"/>
+      <c r="AA47" s="23" t="n"/>
+      <c r="AB47" s="23" t="n"/>
+      <c r="AC47" s="23" t="n"/>
+      <c r="AD47" s="23" t="n"/>
+      <c r="AE47" s="23" t="n"/>
+      <c r="AF47" s="23" t="n"/>
+      <c r="AG47" s="23" t="n"/>
+      <c r="AH47" s="23" t="n"/>
+      <c r="AI47" s="23" t="n"/>
+      <c r="AJ47" s="23" t="n"/>
+      <c r="AK47" s="23" t="n"/>
+      <c r="AL47" s="23" t="n"/>
+      <c r="AM47" s="23" t="n"/>
     </row>
     <row r="48">
-      <c r="A48" s="5" t="n"/>
-      <c r="B48" s="6" t="n"/>
-      <c r="C48" s="6" t="n"/>
-      <c r="D48" s="5" t="n"/>
-      <c r="E48" s="5" t="n"/>
-      <c r="F48" s="5" t="n"/>
-      <c r="G48" s="5" t="n"/>
-      <c r="H48" s="5" t="n"/>
-      <c r="I48" s="5" t="n"/>
-      <c r="J48" s="5" t="n"/>
-      <c r="K48" s="5" t="n"/>
-      <c r="L48" s="5" t="n"/>
-      <c r="M48" s="5" t="n"/>
-      <c r="N48" s="5" t="n"/>
-      <c r="O48" s="5" t="n"/>
-      <c r="P48" s="5" t="n"/>
-      <c r="Q48" s="5" t="n"/>
-      <c r="R48" s="5" t="n"/>
-      <c r="S48" s="5" t="n"/>
-      <c r="T48" s="5" t="n"/>
-      <c r="U48" s="5" t="n"/>
-      <c r="V48" s="5" t="n"/>
-      <c r="W48" s="5" t="n"/>
-      <c r="X48" s="5" t="n"/>
-      <c r="Y48" s="5" t="n"/>
-      <c r="Z48" s="5" t="n"/>
-      <c r="AA48" s="5" t="n"/>
-      <c r="AB48" s="5" t="n"/>
-      <c r="AC48" s="5" t="n"/>
-      <c r="AD48" s="5" t="n"/>
-      <c r="AE48" s="5" t="n"/>
-      <c r="AF48" s="5" t="n"/>
-      <c r="AG48" s="5" t="n"/>
-      <c r="AH48" s="5" t="n"/>
+      <c r="A48" s="52" t="n"/>
+      <c r="B48" s="52" t="n"/>
+      <c r="C48" s="53" t="n"/>
+      <c r="D48" s="52" t="n"/>
+      <c r="E48" s="52" t="n"/>
+      <c r="F48" s="52" t="n"/>
+      <c r="G48" s="52" t="n"/>
+      <c r="H48" s="52" t="n"/>
+      <c r="I48" s="52" t="n"/>
+      <c r="J48" s="52" t="n"/>
+      <c r="K48" s="52" t="n"/>
+      <c r="L48" s="54" t="n"/>
+      <c r="M48" s="54" t="n"/>
+      <c r="N48" s="52" t="n"/>
+      <c r="O48" s="53" t="n"/>
+      <c r="P48" s="23" t="n"/>
+      <c r="Q48" s="23" t="n"/>
+      <c r="R48" s="23" t="n"/>
+      <c r="S48" s="23" t="n"/>
+      <c r="T48" s="23" t="n"/>
+      <c r="U48" s="23" t="n"/>
+      <c r="V48" s="23" t="n"/>
+      <c r="W48" s="23" t="n"/>
+      <c r="X48" s="23" t="n"/>
+      <c r="Y48" s="23" t="n"/>
+      <c r="Z48" s="23" t="n"/>
+      <c r="AA48" s="23" t="n"/>
+      <c r="AB48" s="23" t="n"/>
+      <c r="AC48" s="23" t="n"/>
+      <c r="AD48" s="23" t="n"/>
+      <c r="AE48" s="23" t="n"/>
+      <c r="AF48" s="23" t="n"/>
+      <c r="AG48" s="23" t="n"/>
+      <c r="AH48" s="23" t="n"/>
+      <c r="AI48" s="23" t="n"/>
+      <c r="AJ48" s="23" t="n"/>
+      <c r="AK48" s="23" t="n"/>
+      <c r="AL48" s="23" t="n"/>
+      <c r="AM48" s="23" t="n"/>
     </row>
     <row r="49">
-      <c r="A49" s="5" t="n"/>
-      <c r="B49" s="6" t="n"/>
-      <c r="C49" s="6" t="n"/>
-      <c r="D49" s="5" t="n"/>
-      <c r="E49" s="5" t="n"/>
-      <c r="F49" s="5" t="n"/>
-      <c r="G49" s="5" t="n"/>
-      <c r="H49" s="5" t="n"/>
-      <c r="I49" s="5" t="n"/>
-      <c r="J49" s="5" t="n"/>
-      <c r="K49" s="5" t="n"/>
-      <c r="L49" s="5" t="n"/>
-      <c r="M49" s="5" t="n"/>
-      <c r="N49" s="5" t="n"/>
-      <c r="O49" s="5" t="n"/>
-      <c r="P49" s="5" t="n"/>
-      <c r="Q49" s="5" t="n"/>
-      <c r="R49" s="5" t="n"/>
-      <c r="S49" s="5" t="n"/>
-      <c r="T49" s="5" t="n"/>
-      <c r="U49" s="5" t="n"/>
-      <c r="V49" s="5" t="n"/>
-      <c r="W49" s="5" t="n"/>
-      <c r="X49" s="5" t="n"/>
-      <c r="Y49" s="5" t="n"/>
-      <c r="Z49" s="5" t="n"/>
-      <c r="AA49" s="5" t="n"/>
-      <c r="AB49" s="5" t="n"/>
-      <c r="AC49" s="5" t="n"/>
-      <c r="AD49" s="5" t="n"/>
-      <c r="AE49" s="5" t="n"/>
-      <c r="AF49" s="5" t="n"/>
-      <c r="AG49" s="5" t="n"/>
-      <c r="AH49" s="5" t="n"/>
+      <c r="A49" s="52" t="n"/>
+      <c r="B49" s="52" t="n"/>
+      <c r="C49" s="53" t="n"/>
+      <c r="D49" s="52" t="n"/>
+      <c r="E49" s="52" t="n"/>
+      <c r="F49" s="52" t="n"/>
+      <c r="G49" s="52" t="n"/>
+      <c r="H49" s="52" t="n"/>
+      <c r="I49" s="52" t="n"/>
+      <c r="J49" s="52" t="n"/>
+      <c r="K49" s="52" t="n"/>
+      <c r="L49" s="54" t="n"/>
+      <c r="M49" s="54" t="n"/>
+      <c r="N49" s="52" t="n"/>
+      <c r="O49" s="53" t="n"/>
+      <c r="P49" s="23" t="n"/>
+      <c r="Q49" s="23" t="n"/>
+      <c r="R49" s="23" t="n"/>
+      <c r="S49" s="23" t="n"/>
+      <c r="T49" s="23" t="n"/>
+      <c r="U49" s="23" t="n"/>
+      <c r="V49" s="23" t="n"/>
+      <c r="W49" s="23" t="n"/>
+      <c r="X49" s="23" t="n"/>
+      <c r="Y49" s="23" t="n"/>
+      <c r="Z49" s="23" t="n"/>
+      <c r="AA49" s="23" t="n"/>
+      <c r="AB49" s="23" t="n"/>
+      <c r="AC49" s="23" t="n"/>
+      <c r="AD49" s="23" t="n"/>
+      <c r="AE49" s="23" t="n"/>
+      <c r="AF49" s="23" t="n"/>
+      <c r="AG49" s="23" t="n"/>
+      <c r="AH49" s="23" t="n"/>
+      <c r="AI49" s="23" t="n"/>
+      <c r="AJ49" s="23" t="n"/>
+      <c r="AK49" s="23" t="n"/>
+      <c r="AL49" s="23" t="n"/>
+      <c r="AM49" s="23" t="n"/>
     </row>
     <row r="50">
-      <c r="A50" s="5" t="n"/>
-      <c r="B50" s="6" t="n"/>
-      <c r="C50" s="6" t="n"/>
-      <c r="D50" s="5" t="n"/>
-      <c r="E50" s="5" t="n"/>
-      <c r="F50" s="5" t="n"/>
-      <c r="G50" s="5" t="n"/>
-      <c r="H50" s="5" t="n"/>
-      <c r="I50" s="5" t="n"/>
-      <c r="J50" s="5" t="n"/>
-      <c r="K50" s="5" t="n"/>
-      <c r="L50" s="5" t="n"/>
-      <c r="M50" s="5" t="n"/>
-      <c r="N50" s="5" t="n"/>
-      <c r="O50" s="5" t="n"/>
-      <c r="P50" s="5" t="n"/>
-      <c r="Q50" s="5" t="n"/>
-      <c r="R50" s="5" t="n"/>
-      <c r="S50" s="5" t="n"/>
-      <c r="T50" s="5" t="n"/>
-      <c r="U50" s="5" t="n"/>
-      <c r="V50" s="5" t="n"/>
-      <c r="W50" s="5" t="n"/>
-      <c r="X50" s="5" t="n"/>
-      <c r="Y50" s="5" t="n"/>
-      <c r="Z50" s="5" t="n"/>
-      <c r="AA50" s="5" t="n"/>
-      <c r="AB50" s="5" t="n"/>
-      <c r="AC50" s="5" t="n"/>
-      <c r="AD50" s="5" t="n"/>
-      <c r="AE50" s="5" t="n"/>
-      <c r="AF50" s="5" t="n"/>
-      <c r="AG50" s="5" t="n"/>
-      <c r="AH50" s="5" t="n"/>
+      <c r="A50" s="52" t="n"/>
+      <c r="B50" s="52" t="n"/>
+      <c r="C50" s="53" t="n"/>
+      <c r="D50" s="52" t="n"/>
+      <c r="E50" s="52" t="n"/>
+      <c r="F50" s="52" t="n"/>
+      <c r="G50" s="52" t="n"/>
+      <c r="H50" s="52" t="n"/>
+      <c r="I50" s="52" t="n"/>
+      <c r="J50" s="52" t="n"/>
+      <c r="K50" s="52" t="n"/>
+      <c r="L50" s="54" t="n"/>
+      <c r="M50" s="54" t="n"/>
+      <c r="N50" s="52" t="n"/>
+      <c r="O50" s="53" t="n"/>
+      <c r="P50" s="23" t="n"/>
+      <c r="Q50" s="23" t="n"/>
+      <c r="R50" s="23" t="n"/>
+      <c r="S50" s="23" t="n"/>
+      <c r="T50" s="23" t="n"/>
+      <c r="U50" s="23" t="n"/>
+      <c r="V50" s="23" t="n"/>
+      <c r="W50" s="23" t="n"/>
+      <c r="X50" s="23" t="n"/>
+      <c r="Y50" s="23" t="n"/>
+      <c r="Z50" s="23" t="n"/>
+      <c r="AA50" s="23" t="n"/>
+      <c r="AB50" s="23" t="n"/>
+      <c r="AC50" s="23" t="n"/>
+      <c r="AD50" s="23" t="n"/>
+      <c r="AE50" s="23" t="n"/>
+      <c r="AF50" s="23" t="n"/>
+      <c r="AG50" s="23" t="n"/>
+      <c r="AH50" s="23" t="n"/>
+      <c r="AI50" s="23" t="n"/>
+      <c r="AJ50" s="23" t="n"/>
+      <c r="AK50" s="23" t="n"/>
+      <c r="AL50" s="23" t="n"/>
+      <c r="AM50" s="23" t="n"/>
     </row>
     <row r="51">
-      <c r="A51" s="5" t="n"/>
-      <c r="B51" s="6" t="n"/>
-      <c r="C51" s="6" t="n"/>
-      <c r="D51" s="5" t="n"/>
-      <c r="E51" s="5" t="n"/>
-      <c r="F51" s="5" t="n"/>
-      <c r="G51" s="5" t="n"/>
-      <c r="H51" s="5" t="n"/>
-      <c r="I51" s="5" t="n"/>
-      <c r="J51" s="5" t="n"/>
-      <c r="K51" s="5" t="n"/>
-      <c r="L51" s="5" t="n"/>
-      <c r="M51" s="5" t="n"/>
-      <c r="N51" s="5" t="n"/>
-      <c r="O51" s="5" t="n"/>
-      <c r="P51" s="5" t="n"/>
-      <c r="Q51" s="5" t="n"/>
-      <c r="R51" s="5" t="n"/>
-      <c r="S51" s="5" t="n"/>
-      <c r="T51" s="5" t="n"/>
-      <c r="U51" s="5" t="n"/>
-      <c r="V51" s="5" t="n"/>
-      <c r="W51" s="5" t="n"/>
-      <c r="X51" s="5" t="n"/>
-      <c r="Y51" s="5" t="n"/>
-      <c r="Z51" s="5" t="n"/>
-      <c r="AA51" s="5" t="n"/>
-      <c r="AB51" s="5" t="n"/>
-      <c r="AC51" s="5" t="n"/>
-      <c r="AD51" s="5" t="n"/>
-      <c r="AE51" s="5" t="n"/>
-      <c r="AF51" s="5" t="n"/>
-      <c r="AG51" s="5" t="n"/>
-      <c r="AH51" s="5" t="n"/>
+      <c r="A51" s="23" t="n"/>
+      <c r="B51" s="23" t="n"/>
+      <c r="C51" s="23" t="n"/>
+      <c r="D51" s="23" t="n"/>
+      <c r="E51" s="23" t="n"/>
+      <c r="F51" s="23" t="n"/>
+      <c r="G51" s="23" t="n"/>
+      <c r="H51" s="23" t="n"/>
+      <c r="I51" s="23" t="n"/>
+      <c r="J51" s="23" t="n"/>
+      <c r="K51" s="23" t="n"/>
+      <c r="L51" s="23" t="n"/>
+      <c r="M51" s="23" t="n"/>
+      <c r="N51" s="23" t="n"/>
+      <c r="O51" s="23" t="n"/>
+      <c r="P51" s="23" t="n"/>
+      <c r="Q51" s="23" t="n"/>
+      <c r="R51" s="23" t="n"/>
+      <c r="S51" s="23" t="n"/>
+      <c r="T51" s="23" t="n"/>
+      <c r="U51" s="23" t="n"/>
+      <c r="V51" s="23" t="n"/>
+      <c r="W51" s="23" t="n"/>
+      <c r="X51" s="23" t="n"/>
+      <c r="Y51" s="23" t="n"/>
+      <c r="Z51" s="23" t="n"/>
+      <c r="AA51" s="23" t="n"/>
+      <c r="AB51" s="23" t="n"/>
+      <c r="AC51" s="23" t="n"/>
+      <c r="AD51" s="23" t="n"/>
+      <c r="AE51" s="23" t="n"/>
+      <c r="AF51" s="23" t="n"/>
+      <c r="AG51" s="23" t="n"/>
+      <c r="AH51" s="23" t="n"/>
+      <c r="AI51" s="23" t="n"/>
+      <c r="AJ51" s="23" t="n"/>
+      <c r="AK51" s="23" t="n"/>
+      <c r="AL51" s="23" t="n"/>
+      <c r="AM51" s="23" t="n"/>
     </row>
     <row r="52">
-      <c r="A52" s="5" t="n"/>
-      <c r="B52" s="6" t="n"/>
-      <c r="C52" s="6" t="n"/>
-      <c r="D52" s="5" t="n"/>
-      <c r="E52" s="5" t="n"/>
-      <c r="F52" s="5" t="n"/>
-      <c r="G52" s="5" t="n"/>
-      <c r="H52" s="5" t="n"/>
-      <c r="I52" s="5" t="n"/>
-      <c r="J52" s="5" t="n"/>
-      <c r="K52" s="5" t="n"/>
-      <c r="L52" s="5" t="n"/>
-      <c r="M52" s="5" t="n"/>
-      <c r="N52" s="5" t="n"/>
-      <c r="O52" s="5" t="n"/>
-      <c r="P52" s="5" t="n"/>
-      <c r="Q52" s="5" t="n"/>
-      <c r="R52" s="5" t="n"/>
-      <c r="S52" s="5" t="n"/>
-      <c r="T52" s="5" t="n"/>
-      <c r="U52" s="5" t="n"/>
-      <c r="V52" s="5" t="n"/>
-      <c r="W52" s="5" t="n"/>
-      <c r="X52" s="5" t="n"/>
-      <c r="Y52" s="5" t="n"/>
-      <c r="Z52" s="5" t="n"/>
-      <c r="AA52" s="5" t="n"/>
-      <c r="AB52" s="5" t="n"/>
-      <c r="AC52" s="5" t="n"/>
-      <c r="AD52" s="5" t="n"/>
-      <c r="AE52" s="5" t="n"/>
-      <c r="AF52" s="5" t="n"/>
-      <c r="AG52" s="5" t="n"/>
-      <c r="AH52" s="5" t="n"/>
+      <c r="A52" s="23" t="n"/>
+      <c r="B52" s="23" t="n"/>
+      <c r="C52" s="23" t="n"/>
+      <c r="D52" s="23" t="n"/>
+      <c r="E52" s="23" t="n"/>
+      <c r="F52" s="23" t="n"/>
+      <c r="G52" s="23" t="n"/>
+      <c r="H52" s="23" t="n"/>
+      <c r="I52" s="23" t="n"/>
+      <c r="J52" s="23" t="n"/>
+      <c r="K52" s="23" t="n"/>
+      <c r="L52" s="23" t="n"/>
+      <c r="M52" s="23" t="n"/>
+      <c r="N52" s="23" t="n"/>
+      <c r="O52" s="23" t="n"/>
+      <c r="P52" s="23" t="n"/>
+      <c r="Q52" s="23" t="n"/>
+      <c r="R52" s="23" t="n"/>
+      <c r="S52" s="23" t="n"/>
+      <c r="T52" s="23" t="n"/>
+      <c r="U52" s="23" t="n"/>
+      <c r="V52" s="23" t="n"/>
+      <c r="W52" s="23" t="n"/>
+      <c r="X52" s="23" t="n"/>
+      <c r="Y52" s="23" t="n"/>
+      <c r="Z52" s="23" t="n"/>
+      <c r="AA52" s="23" t="n"/>
+      <c r="AB52" s="23" t="n"/>
+      <c r="AC52" s="23" t="n"/>
+      <c r="AD52" s="23" t="n"/>
+      <c r="AE52" s="23" t="n"/>
+      <c r="AF52" s="23" t="n"/>
+      <c r="AG52" s="23" t="n"/>
+      <c r="AH52" s="23" t="n"/>
+      <c r="AI52" s="23" t="n"/>
+      <c r="AJ52" s="23" t="n"/>
+      <c r="AK52" s="23" t="n"/>
+      <c r="AL52" s="23" t="n"/>
+      <c r="AM52" s="23" t="n"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="23" t="n"/>
+      <c r="B53" s="23" t="n"/>
+      <c r="C53" s="23" t="n"/>
+      <c r="D53" s="23" t="n"/>
+      <c r="E53" s="23" t="n"/>
+      <c r="F53" s="23" t="n"/>
+      <c r="G53" s="23" t="n"/>
+      <c r="H53" s="23" t="n"/>
+      <c r="I53" s="23" t="n"/>
+      <c r="J53" s="23" t="n"/>
+      <c r="K53" s="23" t="n"/>
+      <c r="L53" s="23" t="n"/>
+      <c r="M53" s="23" t="n"/>
+      <c r="N53" s="23" t="n"/>
+      <c r="O53" s="23" t="n"/>
+      <c r="P53" s="23" t="n"/>
+      <c r="Q53" s="23" t="n"/>
+      <c r="R53" s="23" t="n"/>
+      <c r="S53" s="23" t="n"/>
+      <c r="T53" s="23" t="n"/>
+      <c r="U53" s="23" t="n"/>
+      <c r="V53" s="23" t="n"/>
+      <c r="W53" s="23" t="n"/>
+      <c r="X53" s="23" t="n"/>
+      <c r="Y53" s="23" t="n"/>
+      <c r="Z53" s="23" t="n"/>
+      <c r="AA53" s="23" t="n"/>
+      <c r="AB53" s="23" t="n"/>
+      <c r="AC53" s="23" t="n"/>
+      <c r="AD53" s="23" t="n"/>
+      <c r="AE53" s="23" t="n"/>
+      <c r="AF53" s="23" t="n"/>
+      <c r="AG53" s="23" t="n"/>
+      <c r="AH53" s="23" t="n"/>
+      <c r="AI53" s="23" t="n"/>
+      <c r="AJ53" s="23" t="n"/>
+      <c r="AK53" s="23" t="n"/>
+      <c r="AL53" s="23" t="n"/>
+      <c r="AM53" s="23" t="n"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="23" t="n"/>
+      <c r="B54" s="23" t="n"/>
+      <c r="C54" s="23" t="n"/>
+      <c r="D54" s="23" t="n"/>
+      <c r="E54" s="23" t="n"/>
+      <c r="F54" s="23" t="n"/>
+      <c r="G54" s="23" t="n"/>
+      <c r="H54" s="23" t="n"/>
+      <c r="I54" s="23" t="n"/>
+      <c r="J54" s="23" t="n"/>
+      <c r="K54" s="23" t="n"/>
+      <c r="L54" s="23" t="n"/>
+      <c r="M54" s="23" t="n"/>
+      <c r="N54" s="23" t="n"/>
+      <c r="O54" s="23" t="n"/>
+      <c r="P54" s="23" t="n"/>
+      <c r="Q54" s="23" t="n"/>
+      <c r="R54" s="23" t="n"/>
+      <c r="S54" s="23" t="n"/>
+      <c r="T54" s="23" t="n"/>
+      <c r="U54" s="23" t="n"/>
+      <c r="V54" s="23" t="n"/>
+      <c r="W54" s="23" t="n"/>
+      <c r="X54" s="23" t="n"/>
+      <c r="Y54" s="23" t="n"/>
+      <c r="Z54" s="23" t="n"/>
+      <c r="AA54" s="23" t="n"/>
+      <c r="AB54" s="23" t="n"/>
+      <c r="AC54" s="23" t="n"/>
+      <c r="AD54" s="23" t="n"/>
+      <c r="AE54" s="23" t="n"/>
+      <c r="AF54" s="23" t="n"/>
+      <c r="AG54" s="23" t="n"/>
+      <c r="AH54" s="23" t="n"/>
+      <c r="AI54" s="23" t="n"/>
+      <c r="AJ54" s="23" t="n"/>
+      <c r="AK54" s="23" t="n"/>
+      <c r="AL54" s="23" t="n"/>
+      <c r="AM54" s="23" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="AD1:AD2"/>
+  <autoFilter ref="A2:O50"/>
+  <mergeCells count="9">
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="K1:K2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="O1:O2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="W1:W2"/>
-    <mergeCell ref="AH1:AH2"/>
-    <mergeCell ref="Y1:Y2"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="D1:J1"/>
-    <mergeCell ref="AC1:AC2"/>
+    <mergeCell ref="N1:N2"/>
     <mergeCell ref="L1:L2"/>
-    <mergeCell ref="AG1:AG2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="AE1:AE2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="AF1:AF2"/>
-    <mergeCell ref="X1:X2"/>
-    <mergeCell ref="Z1:Z2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="E1:K1"/>
+    <mergeCell ref="D1:D2"/>
     <mergeCell ref="A1:A2"/>
   </mergeCells>
-  <conditionalFormatting sqref="D3:J52">
+  <conditionalFormatting sqref="E3:K50">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="2">
       <formula>"R"</formula>
     </cfRule>
@@ -3937,7 +4178,7 @@
       <formula>"I"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:AH52">
+  <conditionalFormatting sqref="N3:N50">
     <cfRule type="cellIs" priority="6" operator="equal" dxfId="8">
       <formula>"Plan"</formula>
     </cfRule>
@@ -3952,11 +4193,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation sqref="D3:J52" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="E3:K50" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>RASI_List</formula1>
     </dataValidation>
-    <dataValidation sqref="K3:AH52" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"Plan,Active,Done,Delay"</formula1>
+    <dataValidation sqref="N3:N50" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>Status_List</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>